<commit_message>
Remplissage du excell + ajout imgs
</commit_message>
<xml_diff>
--- a/Referentiel_DFS.xlsx
+++ b/Referentiel_DFS.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="274" uniqueCount="157">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="330" uniqueCount="188">
   <si>
     <t>Tableau 1</t>
   </si>
@@ -105,8 +105,19 @@
       <t/>
     </r>
     <r>
-      <t>style="font-family: Avenir Next Demi Bold;font-size: 15px;color: #00bfff;"&gt;Achievement</t>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF00bfff"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Achievement</t>
     </r>
+  </si>
+  <si>
+    <t>Commentaires</t>
   </si>
   <si>
     <r>
@@ -134,6 +145,9 @@
     <t>Fait</t>
   </si>
   <si>
+    <t>Purpaws, Comprendre les besoins de l'ecole et mettre en place notre projet commun</t>
+  </si>
+  <si>
     <t xml:space="preserve">Description :
 Le/la développeur.euse Full Stack participe aux réunions de projets en lien avec les clients et participe à l’élaboration d’une réponse adaptée aux besoins  exprimés. Il/elle conseille le maître d’ouvrage en s’appuyant sur ses compétences techniques pour la réalisation de cahiers des charges. Il/elle participe à la planification des projets et met en œuvre aussi bien les méthodes de gestion de projet que les outils collaboratifs de l’environnement technique de développement au sein de son équipe. Il/elle veille enfin à permettre un suivi et une traçabilité des projets en rédigeant régulièrement des compte-rendu d’activité à destination des équipes projet.
 </t>
@@ -145,7 +159,13 @@
     <t>aucun</t>
   </si>
   <si>
+    <t>Cahier des charges fonctionnel dans canva</t>
+  </si>
+  <si>
     <t>C3 - Participer à l’élaboration d’une planification réaliste en tenant compte de ses propres contraintes et compétences afin de garantir l’atteinte des objectifs fixés pour la réussite du projet</t>
+  </si>
+  <si>
+    <t>Avec purpaws, on a fait un etat des lieux pour savoir qui fera quoi, et comment le faire pour szavoir si c'est réalisable, ryan/yannis back, mel/moi front</t>
   </si>
   <si>
     <t>C4 - Concevoir une ou plusieurs maquettes « wireframe » en utilisant un outil spécialiser afin de fournir une ébauche au demandeur</t>
@@ -153,6 +173,9 @@
   <si>
     <t>débutant.
 cadre personnel : utilisation de photoshop et/ou illustrator pour concevoir une maquette de site.</t>
+  </si>
+  <si>
+    <t>Wireframes dans canva</t>
   </si>
   <si>
     <t xml:space="preserve">C5 - Mettre en œuvre un environnement de développement collaboratif adapté au projet d’application afin d’optimiser le temps de développement, le transfert de compétences auprès de ses pairs et la qualité logicielle
@@ -167,22 +190,43 @@
 C5.4 : aucun</t>
   </si>
   <si>
+    <t>A été imposé React, PHP pour le front/back</t>
+  </si>
+  <si>
     <t>C5.1 - Mettre en oeuvre et maîtriser l’utilisation d’un système de gestion de code source distribué (SCM) permettant de conserver l’historique des développements, d’organiser la collaboration des développeurs et d’appliquer un workflow standard pour la revue de code et le suivi des bugs.</t>
   </si>
   <si>
+    <t>Utilisation de Notion et github</t>
+  </si>
+  <si>
     <t>C5.2 - Mettre en oeuvre un environnement de développement local ou distribué reproductible reposant sur l’utilisation de la virtualisation système ou de la virtualisation applicative</t>
   </si>
   <si>
+    <t>Push/pull github sur notre IDE</t>
+  </si>
+  <si>
     <t>C5.3 Utiliser un environnement de développement intégré (IDE) adapté aux technologies sur lesquelles repose l’application et tirer partie de ses fonctionnalités</t>
   </si>
   <si>
+    <t>vscode</t>
+  </si>
+  <si>
     <t>C5.4 - Sélectionner et mettre en oeuvre les outils et méthodes Agile de développement afin de collaborer efficacement avec les acteurs du projet d’application</t>
   </si>
   <si>
+    <t>Réunion tout les soirs a 16h45 pour un compte rendu de la journée et de l'objectif pour le lendemain</t>
+  </si>
+  <si>
     <t xml:space="preserve">C6 - Comprendre le cycle de développement et mettre en oeuvre les principales méthodes de gestion de projet de développement afin de les appliquer au sein d’une équipe (XP, SCRUM, DSDM, ASD). </t>
   </si>
   <si>
+    <t>Scrum master Yannis, et répartition des taches entre nous</t>
+  </si>
+  <si>
     <t>C7 - Rédiger des compte-rendu d’activité destinés aux membres d’une équipe de projet afin de permettre le suivi de l’avancement du projet et la traçabilité des réalisations techniques</t>
+  </si>
+  <si>
+    <t>Ryan a fait les compte rendu sur notion</t>
   </si>
   <si>
     <r>
@@ -202,6 +246,9 @@
     <t>C8 - Rédiger les spécifications techniques de besoin (STB) d’un projet d’application ou de site web à partir d’un cahier des charges afin de décrire de manière exhaustif les exigences à satisfaire en termes d’utilisation</t>
   </si>
   <si>
+    <t>Vu avec julio</t>
+  </si>
+  <si>
     <t xml:space="preserve">Le/la développeur.euse Full Stack constitue les dossiers de conception en traduisant les besoins client exprimés dans un cahier des charges sous forme de spécifications techniques de besoin (STB). Il/elle modélise les cas d’utilisation, les classes d’analyse et de conception, les schémas entité-association et les schémas de données selon des normes standards. Il/elle est enfin amené.e à décrire les architectures logicielles choisies en vue du développement d’ applications ou de sites web.
 </t>
   </si>
@@ -213,13 +260,22 @@
 vu dans le cadre de scolaire</t>
   </si>
   <si>
+    <t>maquettes? canva</t>
+  </si>
+  <si>
     <t>C9.1 - Utiliser le formalisme du langage de modélisation unifié UML et de UP afin de traduire les besoins de l’application</t>
   </si>
   <si>
+    <t>canva, diagrammes</t>
+  </si>
+  <si>
     <t>C9.2 - Constituer le dossier de modélisation comprenant les diagrammes, les cas d’utilisation, les classes d’analyse et décrivant l’architecture logicielle n-tiers de l’application</t>
   </si>
   <si>
     <t>C9.3 - Utiliser des patrons de conceptions afin d’appliquer des solutions logicielles standards</t>
+  </si>
+  <si>
+    <t>julio , chercher ou on l'a fait</t>
   </si>
   <si>
     <t>C10 - Concevoir l’architecture des bases de données à l’aide d’un outil de modélisation afin de représenter la structure de la couche de persistance nécessaire au fonctionnement de l’application ou du site web</t>
@@ -229,24 +285,45 @@
 vu dans le cadre scolaire</t>
   </si>
   <si>
+    <t>En cours,  pas de plan purpaws, a faire ? fait ?</t>
+  </si>
+  <si>
     <t>C10.1 - Recenser les informations / données du domaine</t>
   </si>
   <si>
+    <t>vague ...pas sur de comprendre le contexte</t>
+  </si>
+  <si>
     <t>C10.2 - Établir le schéma entité-association des données et définir le schéma de la base de données afin de permettre l’élaboration d’une base de données normalisée</t>
+  </si>
+  <si>
+    <t>Purpaws Ryan?</t>
   </si>
   <si>
     <t xml:space="preserve">C10.3 - Dans le cas d’une base de données existante, déduire le schéma entité-association des données de la base à faire évoluer
 </t>
   </si>
   <si>
+    <t>En cours, purpaws, notion ?</t>
+  </si>
+  <si>
     <t>C11 - À partir du dossier de spécifications fonctionnelles et techniques, déterminer l’architecture logicielle de l’application ou du site web</t>
+  </si>
+  <si>
+    <t>Yannis, MVC</t>
   </si>
   <si>
     <r>
       <t/>
     </r>
     <r>
-      <t>style="font-family: Avenir Next Demi Bold;font-size: 15px;color: #00bfff;"&gt;A3 - Développer la partie front-end d’une application ou d’un site web en appliquant les bonnes pratiques d’UX, de sécurité informatique et d’éco-conception</t>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF00bfff"/>
+        <rFont val="Avenir Next Demi Bold"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">A3 - Développer la partie front-end d’une application ou d’un site web en appliquant les bonnes pratiques d’UX, de sécurité informatique et d’éco-conception </t>
     </r>
   </si>
   <si>
@@ -260,6 +337,9 @@
 </t>
   </si>
   <si>
+    <t>En cours, Purpaws, voir img</t>
+  </si>
+  <si>
     <t xml:space="preserve">Le/la développeur.euse Full Stack conçoit, généralement en équipe, la partie front-end d’une application web, hybride, mobile ou desktop en utilisant plusieurs langages de programmation et en appliquant les bonnes pratiques d’UX, de sécurité informatique et d’écoconception. Il/elle valide ses réalisations front-end en utilisant des méthodes de test standards permettant de garantir leur conformité vis-à-vis des spécifications et assurer la non-régression des composants développés. Il/elle participe enfin à l’industrialisation des développements front-end en automatisant les processus d’assurance qualité logicielle.
 </t>
   </si>
@@ -267,15 +347,24 @@
     <t>C12.1 - À partir d’une maquette et/ou d’une charte graphique, structurer et intégrer une interface utilisateur</t>
   </si>
   <si>
+    <t>Purpaws</t>
+  </si>
+  <si>
     <t xml:space="preserve">C12.2 - À partir d’une maquette, structurer et intégrer une interface utilisateur  en utilisant une technologie hybride </t>
   </si>
   <si>
     <t>C12.4 - Sélectionner et mettre en oeuvre un ou plusieurs langages de programmation front-end adaptés aux exigences et contraintes de l’application ou du site web</t>
   </si>
   <si>
+    <t>git, React ectect</t>
+  </si>
+  <si>
     <t>C12.5 - Sélectionner et mettre en oeuvre un framework de développement front-end adapté aux exigences et contraintes de l’application ou du site web</t>
   </si>
   <si>
+    <t>React, jquery</t>
+  </si>
+  <si>
     <t>C12.6 - Développer des composants front-end graphiques et / ou fonctionnels en choisissant des structures de données adaptées et des algorithmes pertinents afin d’assurer la qualité logicielle</t>
   </si>
   <si>
@@ -283,6 +372,9 @@
   </si>
   <si>
     <t>C12.8 - Appliquer les recommandations de sécurité pour le développement front-end afin de s’inscrire dans une démarche de « sécurité en profondeur »</t>
+  </si>
+  <si>
+    <t>Pas sur de ou on l'a fait ca ...</t>
   </si>
   <si>
     <t>C12.9 - Appliquer les bonnes pratiques d’éco-conception afin de minimiser l’impact écologique de la partie front-end de l’application</t>
@@ -295,54 +387,73 @@
 Vu dans le cadre d'une formation mais pas assez pratiqué pour être considéré comme débutant.</t>
   </si>
   <si>
+    <t xml:space="preserve">Arc europe France, confection de boutons </t>
+  </si>
+  <si>
     <t xml:space="preserve">C13.1 - Élaborer un plan de test logiciel exhaustif </t>
+  </si>
+  <si>
+    <t>A voir</t>
+  </si>
+  <si>
+    <t>C13.2 - Réaliser des tests de conformité du langage de balisage structurant le contenu des interfaces web, mobile hybride et desktop</t>
+  </si>
+  <si>
+    <t>C13.3 - Réaliser des tests unitaires pour les composants fonctionnels</t>
+  </si>
+  <si>
+    <t>Arc europe img</t>
+  </si>
+  <si>
+    <t>C13.4 - Réaliser des tests fonctionnels, utilisateurs et de compatibilité avec les différentes plateformes</t>
+  </si>
+  <si>
+    <t>???</t>
+  </si>
+  <si>
+    <t>C14 - Industrialiser le développement de la partie front-end de l’application et automatiser les processus d’assurance qualité</t>
+  </si>
+  <si>
+    <t>débutant.
+Cadre personnel : Utilisation de node.js pour automatiser la gestion des dépendances et webpack
+comme groupeur de module dans le cadre de tutoriel.</t>
+  </si>
+  <si>
+    <t>C14.1 - Automatiser l’exécution d’un vérificateur / correcteur de syntaxe pour chaque langage de programmation constituant le code source de la partie front-end, si nécessaire.</t>
+  </si>
+  <si>
+    <t>IDE VScode</t>
+  </si>
+  <si>
+    <t>C14.2 - Utiliser un gestionnaire de paquets pour automatiser la gestion des dépendances (composants tiers)</t>
+  </si>
+  <si>
+    <t>Homebrew, yarn</t>
+  </si>
+  <si>
+    <t>En cours</t>
+  </si>
+  <si>
+    <t>C14.3 - Utiliser un groupeur de modules afin de configurer et d’exécuter la chaine de build et ainsi optimiser les performances de l’interface</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Webpack   </t>
+  </si>
+  <si>
+    <t>????</t>
   </si>
   <si>
     <r>
       <t/>
     </r>
     <r>
-      <t>style="font-family: Avenir Next Regular;font-size: 15px;color: #FF0000;"&gt;A voir</t>
-    </r>
-  </si>
-  <si>
-    <t>C13.2 - Réaliser des tests de conformité du langage de balisage structurant le contenu des interfaces web, mobile hybride et desktop</t>
-  </si>
-  <si>
-    <t>C13.3 - Réaliser des tests unitaires pour les composants fonctionnels</t>
-  </si>
-  <si>
-    <t>C13.4 - Réaliser des tests fonctionnels, utilisateurs et de compatibilité avec les différentes plateformes</t>
-  </si>
-  <si>
-    <t>C14 - Industrialiser le développement de la partie front-end de l’application et automatiser les processus d’assurance qualité</t>
-  </si>
-  <si>
-    <t>débutant.
-Cadre personnel : Utilisation de node.js pour automatiser la gestion des dépendances et webpack
-comme groupeur de module dans le cadre de tutoriel.</t>
-  </si>
-  <si>
-    <t>C14.1 - Automatiser l’exécution d’un vérificateur / correcteur de syntaxe pour chaque langage de programmation constituant le code source de la partie front-end, si nécessaire.</t>
-  </si>
-  <si>
-    <t>C14.2 - Utiliser un gestionnaire de paquets pour automatiser la gestion des dépendances (composants tiers)</t>
-  </si>
-  <si>
-    <t>Homebrew, yarn</t>
-  </si>
-  <si>
-    <t>C14.3 - Utiliser un groupeur de modules afin de configurer et d’exécuter la chaine de build et ainsi optimiser les performances de l’interface</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Webpack   </t>
-  </si>
-  <si>
-    <r>
-      <t/>
-    </r>
-    <r>
-      <t>style="font-family: Avenir Next Demi Bold;font-size: 15px;color: #00bfff;"&gt;A4 - Développer la partie back-end d’une application ou d’un site web en appliquant les bonnes pratiques de sécurité informatique, d’éco-conception et DevOps</t>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF00bfff"/>
+        <rFont val="Avenir Next Demi Bold"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">A4 - Développer la partie back-end d’une application ou d’un site web en appliquant les bonnes pratiques de sécurité informatique, d’éco-conception et DevOps </t>
     </r>
   </si>
   <si>
@@ -354,7 +465,10 @@
 débutant</t>
   </si>
   <si>
-    <t>Fait front BDD API</t>
+    <t xml:space="preserve">Fait </t>
+  </si>
+  <si>
+    <t>front BDD API</t>
   </si>
   <si>
     <t xml:space="preserve">Le/la développeur.euse Full Stack conçoit ou fait évoluer, généralement en équipe, la couche de persistance des données d’une application web, hybride, mobile ou desktoppuis développe la partie back-end, y compris des API, en utilisant plusieurs langages de programmation et en appliquant les bonnes pratiques de sécurité informatique et d’écoconception. Il/elle est également amené.e à intégrer des services tiers en consommant des API. Il/elle valide ses réalisations back-end en utilisant des méthodes de test standards permettant de garantir leur conformité vis-à-vis des spécifications et assurer la non-régression des composants développés. Il/elle participe enfin à l’industrialisation des développements back-end en automatisant les processus d’assurance qualité logicielle.
@@ -385,7 +499,7 @@
     <t>C16.2 - Sélectionner et mettre en oeuvre un framework de développement back-end adaptés aux exigences et contraintes de l’application ou du site web</t>
   </si>
   <si>
-    <t>Fait Node/express ASP.NET</t>
+    <t>Node/express ASP.NET</t>
   </si>
   <si>
     <t>C16.3 - À partir du référentiel de modélisation, développer des composants back-end fonctionnels en choisissant des structures de données adaptées et des algorithmes pertinents afin d’assurer la qualité logicielle</t>
@@ -424,12 +538,7 @@
     <t>C19.1 - Élaborer un plan de tests logiciels exhaustif  pour le back-end</t>
   </si>
   <si>
-    <r>
-      <t/>
-    </r>
-    <r>
-      <t>style="font-family: Avenir Next Demi Bold;font-size: 15px;color: #FF0000;"&gt;Document a voir (décrit comment approcher, concevoir et exécuter les tests)</t>
-    </r>
+    <t>Document a voir (décrit comment approcher, concevoir et exécuter les tests)</t>
   </si>
   <si>
     <t>C19.2 - Réaliser des tests unitaires sur les composants du back-end</t>
@@ -439,14 +548,6 @@
   </si>
   <si>
     <t>C19.3 - Réaliser des tests fonctionnels sur les composants du back-end</t>
-  </si>
-  <si>
-    <r>
-      <t/>
-    </r>
-    <r>
-      <t>style="font-family: Avenir Next Demi Bold;font-size: 15px;color: #FF0000;"&gt;A voir</t>
-    </r>
   </si>
   <si>
     <t>C20 - Industrialiser le développement de la partie back-end de l’application ou du site web et automatiser les processus d’assurance qualité</t>
@@ -605,12 +706,7 @@
     <t>C24.4 - Rédiger la documentation d’une API afin de faciliter sa consommation par des tiers</t>
   </si>
   <si>
-    <r>
-      <t/>
-    </r>
-    <r>
-      <t>style="font-family: Avenir Next Demi Bold;font-size: 15px;color: #00bfff;"&gt;A6 - Mettre en oeuvre des solutions techniques répondant aux besoins contextuels d’une application ou d’un site web (lois, normes et règlements, accessibilité, outils marketing et e-commerce) et piloter les performances.</t>
-    </r>
+    <t>style="font-family: Avenir Next Demi Bold;font-size: 15px;color: #00bfff;"&gt;A6 - Mettre en oeuvre des solutions techniques répondant aux besoins contextuels d’une application ou d’un site web (lois, normes et règlements, accessibilité, outils marketing et e-commerce) et piloter les performances.</t>
   </si>
   <si>
     <t>C25 - Mettre en oeuvre les outils et techniques permettant de respecter les aspects réglementaires au regard des données informatiques traitées et stockées</t>
@@ -831,9 +927,6 @@
       </rPr>
       <t xml:space="preserve"> et marketing d’affiliation) adaptée au contexte et à l’environnement d’une application</t>
     </r>
-  </si>
-  <si>
-    <t>style="font-family: Avenir Next Demi Bold;font-size: 15px;color: #FF0000;"&gt;A voir</t>
   </si>
 </sst>
 </file>
@@ -1596,7 +1689,9 @@
       <c r="D2" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="E2" s="4"/>
+      <c r="E2" s="4" t="s">
+        <v>5</v>
+      </c>
       <c r="F2" s="4"/>
       <c r="G2" s="4"/>
       <c r="H2" s="4"/>
@@ -1621,18 +1716,20 @@
     </row>
     <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="85.5" customFormat="1" s="1">
       <c r="A3" s="7" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B3" s="8" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C3" s="8" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="E3" s="4"/>
+        <v>9</v>
+      </c>
+      <c r="E3" s="4" t="s">
+        <v>10</v>
+      </c>
       <c r="F3" s="4"/>
       <c r="G3" s="4"/>
       <c r="H3" s="4"/>
@@ -1657,18 +1754,20 @@
     </row>
     <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="47.4375" customFormat="1" s="1">
       <c r="A4" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="B4" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="C4" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="D4" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="B4" s="8" t="s">
-        <v>10</v>
-      </c>
-      <c r="C4" s="8" t="s">
-        <v>11</v>
-      </c>
-      <c r="D4" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="E4" s="4"/>
+      <c r="E4" s="4" t="s">
+        <v>14</v>
+      </c>
       <c r="F4" s="4"/>
       <c r="G4" s="4"/>
       <c r="H4" s="4"/>
@@ -1694,15 +1793,17 @@
     <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="40.5" customFormat="1" s="1">
       <c r="A5" s="10"/>
       <c r="B5" s="8" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="C5" s="8" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="E5" s="4"/>
+        <v>9</v>
+      </c>
+      <c r="E5" s="4" t="s">
+        <v>16</v>
+      </c>
       <c r="F5" s="4"/>
       <c r="G5" s="4"/>
       <c r="H5" s="4"/>
@@ -1728,15 +1829,17 @@
     <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="63" customFormat="1" s="1">
       <c r="A6" s="10"/>
       <c r="B6" s="8" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="C6" s="8" t="s">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="E6" s="4"/>
+        <v>9</v>
+      </c>
+      <c r="E6" s="4" t="s">
+        <v>19</v>
+      </c>
       <c r="F6" s="4"/>
       <c r="G6" s="4"/>
       <c r="H6" s="4"/>
@@ -1762,15 +1865,17 @@
     <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="39.75" customFormat="1" s="1">
       <c r="A7" s="11"/>
       <c r="B7" s="7" t="s">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="C7" s="12" t="s">
-        <v>16</v>
+        <v>21</v>
       </c>
       <c r="D7" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="E7" s="4"/>
+        <v>9</v>
+      </c>
+      <c r="E7" s="4" t="s">
+        <v>22</v>
+      </c>
       <c r="F7" s="4"/>
       <c r="G7" s="4"/>
       <c r="H7" s="4"/>
@@ -1796,13 +1901,15 @@
     <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="54" customFormat="1" s="1">
       <c r="A8" s="13"/>
       <c r="B8" s="14" t="s">
-        <v>17</v>
+        <v>23</v>
       </c>
       <c r="C8" s="10"/>
       <c r="D8" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="E8" s="4"/>
+        <v>9</v>
+      </c>
+      <c r="E8" s="4" t="s">
+        <v>24</v>
+      </c>
       <c r="F8" s="4"/>
       <c r="G8" s="4"/>
       <c r="H8" s="4"/>
@@ -1828,13 +1935,15 @@
     <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="44.25" customFormat="1" s="1">
       <c r="A9" s="13"/>
       <c r="B9" s="14" t="s">
-        <v>18</v>
+        <v>25</v>
       </c>
       <c r="C9" s="10"/>
       <c r="D9" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="E9" s="4"/>
+        <v>9</v>
+      </c>
+      <c r="E9" s="4" t="s">
+        <v>26</v>
+      </c>
       <c r="F9" s="4"/>
       <c r="G9" s="4"/>
       <c r="H9" s="4"/>
@@ -1860,13 +1969,15 @@
     <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="36" customFormat="1" s="1">
       <c r="A10" s="13"/>
       <c r="B10" s="15" t="s">
-        <v>19</v>
+        <v>27</v>
       </c>
       <c r="C10" s="10"/>
       <c r="D10" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="E10" s="4"/>
+        <v>9</v>
+      </c>
+      <c r="E10" s="4" t="s">
+        <v>28</v>
+      </c>
       <c r="F10" s="4"/>
       <c r="G10" s="4"/>
       <c r="H10" s="4"/>
@@ -1892,13 +2003,15 @@
     <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="31.5" customFormat="1" s="1">
       <c r="A11" s="16"/>
       <c r="B11" s="17" t="s">
-        <v>20</v>
+        <v>29</v>
       </c>
       <c r="C11" s="18"/>
       <c r="D11" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="E11" s="4"/>
+        <v>9</v>
+      </c>
+      <c r="E11" s="4" t="s">
+        <v>30</v>
+      </c>
       <c r="F11" s="4"/>
       <c r="G11" s="4"/>
       <c r="H11" s="4"/>
@@ -1924,15 +2037,17 @@
     <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="42" customFormat="1" s="1">
       <c r="A12" s="19"/>
       <c r="B12" s="8" t="s">
-        <v>21</v>
+        <v>31</v>
       </c>
       <c r="C12" s="8" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="D12" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="E12" s="4"/>
+        <v>9</v>
+      </c>
+      <c r="E12" s="4" t="s">
+        <v>32</v>
+      </c>
       <c r="F12" s="4"/>
       <c r="G12" s="4"/>
       <c r="H12" s="4"/>
@@ -1958,15 +2073,17 @@
     <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="33.75" customFormat="1" s="1">
       <c r="A13" s="17"/>
       <c r="B13" s="8" t="s">
-        <v>22</v>
+        <v>33</v>
       </c>
       <c r="C13" s="8" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="D13" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="E13" s="4"/>
+        <v>9</v>
+      </c>
+      <c r="E13" s="4" t="s">
+        <v>34</v>
+      </c>
       <c r="F13" s="4"/>
       <c r="G13" s="4"/>
       <c r="H13" s="4"/>
@@ -1991,18 +2108,20 @@
     </row>
     <row x14ac:dyDescent="0.25" r="14" customHeight="1" ht="45" customFormat="1" s="1">
       <c r="A14" s="7" t="s">
-        <v>23</v>
+        <v>35</v>
       </c>
       <c r="B14" s="8" t="s">
-        <v>24</v>
+        <v>36</v>
       </c>
       <c r="C14" s="8" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="D14" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="E14" s="4"/>
+        <v>9</v>
+      </c>
+      <c r="E14" s="4" t="s">
+        <v>37</v>
+      </c>
       <c r="F14" s="4"/>
       <c r="G14" s="4"/>
       <c r="H14" s="4"/>
@@ -2027,18 +2146,20 @@
     </row>
     <row x14ac:dyDescent="0.25" r="15" customHeight="1" ht="36.75" customFormat="1" s="1">
       <c r="A15" s="20" t="s">
-        <v>25</v>
+        <v>38</v>
       </c>
       <c r="B15" s="7" t="s">
-        <v>26</v>
+        <v>39</v>
       </c>
       <c r="C15" s="12" t="s">
-        <v>27</v>
+        <v>40</v>
       </c>
       <c r="D15" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="E15" s="4"/>
+        <v>9</v>
+      </c>
+      <c r="E15" s="4" t="s">
+        <v>41</v>
+      </c>
       <c r="F15" s="4"/>
       <c r="G15" s="4"/>
       <c r="H15" s="4"/>
@@ -2064,13 +2185,15 @@
     <row x14ac:dyDescent="0.25" r="16" customHeight="1" ht="36" customFormat="1" s="1">
       <c r="A16" s="10"/>
       <c r="B16" s="14" t="s">
-        <v>28</v>
+        <v>42</v>
       </c>
       <c r="C16" s="10"/>
       <c r="D16" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="E16" s="4"/>
+        <v>9</v>
+      </c>
+      <c r="E16" s="4" t="s">
+        <v>43</v>
+      </c>
       <c r="F16" s="4"/>
       <c r="G16" s="4"/>
       <c r="H16" s="4"/>
@@ -2096,13 +2219,15 @@
     <row x14ac:dyDescent="0.25" r="17" customHeight="1" ht="42.75" customFormat="1" s="1">
       <c r="A17" s="11"/>
       <c r="B17" s="14" t="s">
-        <v>29</v>
+        <v>44</v>
       </c>
       <c r="C17" s="10"/>
       <c r="D17" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="E17" s="4"/>
+        <v>9</v>
+      </c>
+      <c r="E17" s="4" t="s">
+        <v>43</v>
+      </c>
       <c r="F17" s="4"/>
       <c r="G17" s="4"/>
       <c r="H17" s="4"/>
@@ -2128,13 +2253,15 @@
     <row x14ac:dyDescent="0.25" r="18" customHeight="1" ht="36.75" customFormat="1" s="1">
       <c r="A18" s="13"/>
       <c r="B18" s="21" t="s">
-        <v>30</v>
+        <v>45</v>
       </c>
       <c r="C18" s="18"/>
       <c r="D18" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="E18" s="4"/>
+        <v>9</v>
+      </c>
+      <c r="E18" s="4" t="s">
+        <v>46</v>
+      </c>
       <c r="F18" s="4"/>
       <c r="G18" s="4"/>
       <c r="H18" s="4"/>
@@ -2160,15 +2287,17 @@
     <row x14ac:dyDescent="0.25" r="19" customHeight="1" ht="51" customFormat="1" s="1">
       <c r="A19" s="13"/>
       <c r="B19" s="22" t="s">
-        <v>31</v>
+        <v>47</v>
       </c>
       <c r="C19" s="12" t="s">
-        <v>32</v>
+        <v>48</v>
       </c>
       <c r="D19" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="E19" s="4"/>
+        <v>9</v>
+      </c>
+      <c r="E19" s="4" t="s">
+        <v>49</v>
+      </c>
       <c r="F19" s="4"/>
       <c r="G19" s="4"/>
       <c r="H19" s="4"/>
@@ -2194,13 +2323,15 @@
     <row x14ac:dyDescent="0.25" r="20" customHeight="1" ht="36" customFormat="1" s="1">
       <c r="A20" s="13"/>
       <c r="B20" s="23" t="s">
-        <v>33</v>
+        <v>50</v>
       </c>
       <c r="C20" s="10"/>
       <c r="D20" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="E20" s="4"/>
+        <v>9</v>
+      </c>
+      <c r="E20" s="4" t="s">
+        <v>51</v>
+      </c>
       <c r="F20" s="4"/>
       <c r="G20" s="4"/>
       <c r="H20" s="4"/>
@@ -2226,13 +2357,15 @@
     <row x14ac:dyDescent="0.25" r="21" customHeight="1" ht="50.25" customFormat="1" s="1">
       <c r="A21" s="13"/>
       <c r="B21" s="23" t="s">
-        <v>34</v>
+        <v>52</v>
       </c>
       <c r="C21" s="10"/>
       <c r="D21" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="E21" s="4"/>
+        <v>9</v>
+      </c>
+      <c r="E21" s="4" t="s">
+        <v>53</v>
+      </c>
       <c r="F21" s="4"/>
       <c r="G21" s="4"/>
       <c r="H21" s="4"/>
@@ -2258,13 +2391,15 @@
     <row x14ac:dyDescent="0.25" r="22" customHeight="1" ht="51" customFormat="1" s="1">
       <c r="A22" s="13"/>
       <c r="B22" s="24" t="s">
-        <v>35</v>
+        <v>54</v>
       </c>
       <c r="C22" s="18"/>
       <c r="D22" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="E22" s="4"/>
+        <v>9</v>
+      </c>
+      <c r="E22" s="4" t="s">
+        <v>55</v>
+      </c>
       <c r="F22" s="4"/>
       <c r="G22" s="4"/>
       <c r="H22" s="4"/>
@@ -2290,15 +2425,17 @@
     <row x14ac:dyDescent="0.25" r="23" customHeight="1" ht="37.5" customFormat="1" s="1">
       <c r="A23" s="25"/>
       <c r="B23" s="8" t="s">
-        <v>36</v>
+        <v>56</v>
       </c>
       <c r="C23" s="8" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="D23" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="E23" s="4"/>
+        <v>9</v>
+      </c>
+      <c r="E23" s="4" t="s">
+        <v>57</v>
+      </c>
       <c r="F23" s="4"/>
       <c r="G23" s="4"/>
       <c r="H23" s="4"/>
@@ -2323,18 +2460,20 @@
     </row>
     <row x14ac:dyDescent="0.25" r="24" customHeight="1" ht="57" customFormat="1" s="1">
       <c r="A24" s="7" t="s">
-        <v>37</v>
+        <v>58</v>
       </c>
       <c r="B24" s="7" t="s">
-        <v>38</v>
+        <v>59</v>
       </c>
       <c r="C24" s="12" t="s">
-        <v>39</v>
+        <v>60</v>
       </c>
       <c r="D24" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="E24" s="4"/>
+        <v>9</v>
+      </c>
+      <c r="E24" s="4" t="s">
+        <v>61</v>
+      </c>
       <c r="F24" s="4"/>
       <c r="G24" s="4"/>
       <c r="H24" s="4"/>
@@ -2359,16 +2498,18 @@
     </row>
     <row x14ac:dyDescent="0.25" r="25" customHeight="1" ht="36" customFormat="1" s="1">
       <c r="A25" s="20" t="s">
-        <v>40</v>
+        <v>62</v>
       </c>
       <c r="B25" s="14" t="s">
-        <v>41</v>
+        <v>63</v>
       </c>
       <c r="C25" s="10"/>
       <c r="D25" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="E25" s="4"/>
+        <v>9</v>
+      </c>
+      <c r="E25" s="4" t="s">
+        <v>64</v>
+      </c>
       <c r="F25" s="4"/>
       <c r="G25" s="4"/>
       <c r="H25" s="4"/>
@@ -2394,13 +2535,15 @@
     <row x14ac:dyDescent="0.25" r="26" customHeight="1" ht="50.25" customFormat="1" s="1">
       <c r="A26" s="10"/>
       <c r="B26" s="14" t="s">
-        <v>42</v>
+        <v>65</v>
       </c>
       <c r="C26" s="10"/>
       <c r="D26" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="E26" s="4"/>
+        <v>9</v>
+      </c>
+      <c r="E26" s="4" t="s">
+        <v>64</v>
+      </c>
       <c r="F26" s="4"/>
       <c r="G26" s="4"/>
       <c r="H26" s="4"/>
@@ -2423,16 +2566,18 @@
       <c r="Y26" s="4"/>
       <c r="Z26" s="4"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="27" customHeight="1" ht="38.25" customFormat="1" s="1">
+    <row x14ac:dyDescent="0.25" r="27" customHeight="1" ht="35.75" customFormat="1" s="1">
       <c r="A27" s="11"/>
       <c r="B27" s="14" t="s">
-        <v>43</v>
+        <v>66</v>
       </c>
       <c r="C27" s="10"/>
       <c r="D27" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="E27" s="4"/>
+        <v>9</v>
+      </c>
+      <c r="E27" s="4" t="s">
+        <v>67</v>
+      </c>
       <c r="F27" s="4"/>
       <c r="G27" s="4"/>
       <c r="H27" s="4"/>
@@ -2455,16 +2600,18 @@
       <c r="Y27" s="4"/>
       <c r="Z27" s="4"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="28" customHeight="1" ht="36" customFormat="1" s="1">
+    <row x14ac:dyDescent="0.25" r="28" customHeight="1" ht="28.5" customFormat="1" s="1">
       <c r="A28" s="13"/>
       <c r="B28" s="14" t="s">
-        <v>44</v>
+        <v>68</v>
       </c>
       <c r="C28" s="10"/>
       <c r="D28" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="E28" s="4"/>
+        <v>9</v>
+      </c>
+      <c r="E28" s="4" t="s">
+        <v>69</v>
+      </c>
       <c r="F28" s="4"/>
       <c r="G28" s="4"/>
       <c r="H28" s="4"/>
@@ -2487,16 +2634,18 @@
       <c r="Y28" s="4"/>
       <c r="Z28" s="4"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="29" customHeight="1" ht="50.25" customFormat="1" s="1">
+    <row x14ac:dyDescent="0.25" r="29" customHeight="1" ht="39.75" customFormat="1" s="1">
       <c r="A29" s="13"/>
       <c r="B29" s="14" t="s">
-        <v>45</v>
+        <v>70</v>
       </c>
       <c r="C29" s="10"/>
       <c r="D29" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="E29" s="4"/>
+        <v>9</v>
+      </c>
+      <c r="E29" s="4" t="s">
+        <v>64</v>
+      </c>
       <c r="F29" s="4"/>
       <c r="G29" s="4"/>
       <c r="H29" s="4"/>
@@ -2519,16 +2668,18 @@
       <c r="Y29" s="4"/>
       <c r="Z29" s="4"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="30" customHeight="1" ht="21.75" customFormat="1" s="1">
+    <row x14ac:dyDescent="0.25" r="30" customHeight="1" ht="18.75" customFormat="1" s="1">
       <c r="A30" s="13"/>
       <c r="B30" s="14" t="s">
-        <v>46</v>
+        <v>71</v>
       </c>
       <c r="C30" s="10"/>
       <c r="D30" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="E30" s="4"/>
+        <v>9</v>
+      </c>
+      <c r="E30" s="4" t="s">
+        <v>64</v>
+      </c>
       <c r="F30" s="4"/>
       <c r="G30" s="4"/>
       <c r="H30" s="4"/>
@@ -2551,16 +2702,18 @@
       <c r="Y30" s="4"/>
       <c r="Z30" s="4"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="31" customHeight="1" ht="36" customFormat="1" s="1">
+    <row x14ac:dyDescent="0.25" r="31" customHeight="1" ht="28.5" customFormat="1" s="1">
       <c r="A31" s="13"/>
       <c r="B31" s="14" t="s">
-        <v>47</v>
+        <v>72</v>
       </c>
       <c r="C31" s="10"/>
       <c r="D31" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="E31" s="4"/>
+        <v>9</v>
+      </c>
+      <c r="E31" s="4" t="s">
+        <v>73</v>
+      </c>
       <c r="F31" s="4"/>
       <c r="G31" s="4"/>
       <c r="H31" s="4"/>
@@ -2583,16 +2736,18 @@
       <c r="Y31" s="4"/>
       <c r="Z31" s="4"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="32" customHeight="1" ht="36.75" customFormat="1" s="1">
+    <row x14ac:dyDescent="0.25" r="32" customHeight="1" ht="29.25" customFormat="1" s="1">
       <c r="A32" s="13"/>
       <c r="B32" s="21" t="s">
-        <v>48</v>
+        <v>74</v>
       </c>
       <c r="C32" s="18"/>
       <c r="D32" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="E32" s="4"/>
+        <v>9</v>
+      </c>
+      <c r="E32" s="4" t="s">
+        <v>64</v>
+      </c>
       <c r="F32" s="4"/>
       <c r="G32" s="4"/>
       <c r="H32" s="4"/>
@@ -2615,18 +2770,20 @@
       <c r="Y32" s="4"/>
       <c r="Z32" s="4"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="33" customHeight="1" ht="51" customFormat="1" s="1">
+    <row x14ac:dyDescent="0.25" r="33" customHeight="1" ht="39.75" customFormat="1" s="1">
       <c r="A33" s="13"/>
       <c r="B33" s="7" t="s">
-        <v>49</v>
+        <v>75</v>
       </c>
       <c r="C33" s="12" t="s">
-        <v>50</v>
+        <v>76</v>
       </c>
       <c r="D33" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="E33" s="4"/>
+        <v>9</v>
+      </c>
+      <c r="E33" s="4" t="s">
+        <v>77</v>
+      </c>
       <c r="F33" s="4"/>
       <c r="G33" s="4"/>
       <c r="H33" s="4"/>
@@ -2649,14 +2806,14 @@
       <c r="Y33" s="4"/>
       <c r="Z33" s="4"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="34" customHeight="1" ht="21.75" customFormat="1" s="1">
+    <row x14ac:dyDescent="0.25" r="34" customHeight="1" ht="51" customFormat="1" s="1">
       <c r="A34" s="13"/>
       <c r="B34" s="14" t="s">
-        <v>51</v>
+        <v>78</v>
       </c>
       <c r="C34" s="10"/>
       <c r="D34" s="4" t="s">
-        <v>52</v>
+        <v>79</v>
       </c>
       <c r="E34" s="4"/>
       <c r="F34" s="4"/>
@@ -2681,14 +2838,14 @@
       <c r="Y34" s="4"/>
       <c r="Z34" s="4"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="35" customHeight="1" ht="36" customFormat="1" s="1">
+    <row x14ac:dyDescent="0.25" r="35" customHeight="1" ht="51" customFormat="1" s="1">
       <c r="A35" s="13"/>
       <c r="B35" s="14" t="s">
-        <v>53</v>
+        <v>80</v>
       </c>
       <c r="C35" s="10"/>
       <c r="D35" s="4" t="s">
-        <v>52</v>
+        <v>79</v>
       </c>
       <c r="E35" s="4"/>
       <c r="F35" s="4"/>
@@ -2713,16 +2870,18 @@
       <c r="Y35" s="4"/>
       <c r="Z35" s="4"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="36" customHeight="1" ht="21.75" customFormat="1" s="1">
+    <row x14ac:dyDescent="0.25" r="36" customHeight="1" ht="18.75" customFormat="1" s="1">
       <c r="A36" s="13"/>
       <c r="B36" s="14" t="s">
-        <v>54</v>
+        <v>81</v>
       </c>
       <c r="C36" s="10"/>
       <c r="D36" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="E36" s="4"/>
+        <v>9</v>
+      </c>
+      <c r="E36" s="4" t="s">
+        <v>82</v>
+      </c>
       <c r="F36" s="4"/>
       <c r="G36" s="4"/>
       <c r="H36" s="4"/>
@@ -2745,16 +2904,18 @@
       <c r="Y36" s="4"/>
       <c r="Z36" s="4"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="37" customHeight="1" ht="36.75" customFormat="1" s="1">
+    <row x14ac:dyDescent="0.25" r="37" customHeight="1" ht="29.25" customFormat="1" s="1">
       <c r="A37" s="13"/>
       <c r="B37" s="21" t="s">
-        <v>55</v>
+        <v>83</v>
       </c>
       <c r="C37" s="18"/>
       <c r="D37" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="E37" s="4"/>
+        <v>9</v>
+      </c>
+      <c r="E37" s="4" t="s">
+        <v>84</v>
+      </c>
       <c r="F37" s="4"/>
       <c r="G37" s="4"/>
       <c r="H37" s="4"/>
@@ -2777,18 +2938,20 @@
       <c r="Y37" s="4"/>
       <c r="Z37" s="4"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="38" customHeight="1" ht="36.75" customFormat="1" s="1">
+    <row x14ac:dyDescent="0.25" r="38" customHeight="1" ht="28.5" customFormat="1" s="1">
       <c r="A38" s="13"/>
       <c r="B38" s="7" t="s">
-        <v>56</v>
+        <v>85</v>
       </c>
       <c r="C38" s="12" t="s">
-        <v>57</v>
+        <v>86</v>
       </c>
       <c r="D38" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="E38" s="4"/>
+        <v>9</v>
+      </c>
+      <c r="E38" s="4" t="s">
+        <v>84</v>
+      </c>
       <c r="F38" s="4"/>
       <c r="G38" s="4"/>
       <c r="H38" s="4"/>
@@ -2811,16 +2974,18 @@
       <c r="Y38" s="4"/>
       <c r="Z38" s="4"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="39" customHeight="1" ht="50.25" customFormat="1" s="1">
+    <row x14ac:dyDescent="0.25" r="39" customHeight="1" ht="28.5" customFormat="1" s="1">
       <c r="A39" s="13"/>
       <c r="B39" s="14" t="s">
-        <v>58</v>
+        <v>87</v>
       </c>
       <c r="C39" s="10"/>
       <c r="D39" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="E39" s="4"/>
+        <v>9</v>
+      </c>
+      <c r="E39" s="4" t="s">
+        <v>88</v>
+      </c>
       <c r="F39" s="4"/>
       <c r="G39" s="4"/>
       <c r="H39" s="4"/>
@@ -2843,16 +3008,18 @@
       <c r="Y39" s="4"/>
       <c r="Z39" s="4"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="40" customHeight="1" ht="38.25" customFormat="1" s="1">
+    <row x14ac:dyDescent="0.25" r="40" customHeight="1" ht="28.5" customFormat="1" s="1">
       <c r="A40" s="13"/>
       <c r="B40" s="14" t="s">
-        <v>59</v>
+        <v>89</v>
       </c>
       <c r="C40" s="10"/>
       <c r="D40" s="4" t="s">
-        <v>60</v>
-      </c>
-      <c r="E40" s="4"/>
+        <v>90</v>
+      </c>
+      <c r="E40" s="4" t="s">
+        <v>91</v>
+      </c>
       <c r="F40" s="4"/>
       <c r="G40" s="4"/>
       <c r="H40" s="4"/>
@@ -2875,16 +3042,18 @@
       <c r="Y40" s="4"/>
       <c r="Z40" s="4"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="41" customHeight="1" ht="62.25" customFormat="1" s="1">
+    <row x14ac:dyDescent="0.25" r="41" customHeight="1" ht="40.5" customFormat="1" s="1">
       <c r="A41" s="25"/>
       <c r="B41" s="21" t="s">
-        <v>61</v>
+        <v>92</v>
       </c>
       <c r="C41" s="18"/>
       <c r="D41" s="4" t="s">
-        <v>62</v>
-      </c>
-      <c r="E41" s="4"/>
+        <v>93</v>
+      </c>
+      <c r="E41" s="4" t="s">
+        <v>94</v>
+      </c>
       <c r="F41" s="4"/>
       <c r="G41" s="4"/>
       <c r="H41" s="4"/>
@@ -2909,18 +3078,20 @@
     </row>
     <row x14ac:dyDescent="0.25" r="42" customHeight="1" ht="51" customFormat="1" s="1">
       <c r="A42" s="7" t="s">
-        <v>63</v>
+        <v>95</v>
       </c>
       <c r="B42" s="7" t="s">
-        <v>64</v>
+        <v>96</v>
       </c>
       <c r="C42" s="12" t="s">
-        <v>65</v>
+        <v>97</v>
       </c>
       <c r="D42" s="4" t="s">
-        <v>66</v>
-      </c>
-      <c r="E42" s="4"/>
+        <v>98</v>
+      </c>
+      <c r="E42" s="4" t="s">
+        <v>99</v>
+      </c>
       <c r="F42" s="4"/>
       <c r="G42" s="4"/>
       <c r="H42" s="4"/>
@@ -2945,16 +3116,18 @@
     </row>
     <row x14ac:dyDescent="0.25" r="43" customHeight="1" ht="27.75" customFormat="1" s="1">
       <c r="A43" s="20" t="s">
-        <v>67</v>
+        <v>100</v>
       </c>
       <c r="B43" s="14" t="s">
-        <v>68</v>
+        <v>101</v>
       </c>
       <c r="C43" s="10"/>
       <c r="D43" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="E43" s="4"/>
+        <v>9</v>
+      </c>
+      <c r="E43" s="4" t="s">
+        <v>91</v>
+      </c>
       <c r="F43" s="4"/>
       <c r="G43" s="4"/>
       <c r="H43" s="4"/>
@@ -2980,13 +3153,15 @@
     <row x14ac:dyDescent="0.25" r="44" customHeight="1" ht="27.75" customFormat="1" s="1">
       <c r="A44" s="10"/>
       <c r="B44" s="14" t="s">
-        <v>69</v>
+        <v>102</v>
       </c>
       <c r="C44" s="10"/>
       <c r="D44" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="E44" s="4"/>
+        <v>9</v>
+      </c>
+      <c r="E44" s="4" t="s">
+        <v>91</v>
+      </c>
       <c r="F44" s="4"/>
       <c r="G44" s="4"/>
       <c r="H44" s="4"/>
@@ -3012,13 +3187,15 @@
     <row x14ac:dyDescent="0.25" r="45" customHeight="1" ht="27.75" customFormat="1" s="1">
       <c r="A45" s="10"/>
       <c r="B45" s="14" t="s">
-        <v>70</v>
+        <v>103</v>
       </c>
       <c r="C45" s="10"/>
       <c r="D45" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="E45" s="4"/>
+        <v>9</v>
+      </c>
+      <c r="E45" s="4" t="s">
+        <v>91</v>
+      </c>
       <c r="F45" s="4"/>
       <c r="G45" s="4"/>
       <c r="H45" s="4"/>
@@ -3044,13 +3221,15 @@
     <row x14ac:dyDescent="0.25" r="46" customHeight="1" ht="66" customFormat="1" s="1">
       <c r="A46" s="11"/>
       <c r="B46" s="14" t="s">
-        <v>71</v>
+        <v>104</v>
       </c>
       <c r="C46" s="10"/>
       <c r="D46" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="E46" s="4"/>
+        <v>9</v>
+      </c>
+      <c r="E46" s="4" t="s">
+        <v>91</v>
+      </c>
       <c r="F46" s="4"/>
       <c r="G46" s="4"/>
       <c r="H46" s="4"/>
@@ -3076,13 +3255,15 @@
     <row x14ac:dyDescent="0.25" r="47" customHeight="1" ht="30.75" customFormat="1" s="1">
       <c r="A47" s="13"/>
       <c r="B47" s="21" t="s">
-        <v>72</v>
+        <v>105</v>
       </c>
       <c r="C47" s="18"/>
       <c r="D47" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="E47" s="4"/>
+        <v>9</v>
+      </c>
+      <c r="E47" s="4" t="s">
+        <v>91</v>
+      </c>
       <c r="F47" s="4"/>
       <c r="G47" s="4"/>
       <c r="H47" s="4"/>
@@ -3108,15 +3289,17 @@
     <row x14ac:dyDescent="0.25" r="48" customHeight="1" ht="42.75" customFormat="1" s="1">
       <c r="A48" s="13"/>
       <c r="B48" s="7" t="s">
-        <v>73</v>
+        <v>106</v>
       </c>
       <c r="C48" s="12" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="D48" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="E48" s="4"/>
+        <v>9</v>
+      </c>
+      <c r="E48" s="4" t="s">
+        <v>91</v>
+      </c>
       <c r="F48" s="4"/>
       <c r="G48" s="4"/>
       <c r="H48" s="4"/>
@@ -3142,13 +3325,15 @@
     <row x14ac:dyDescent="0.25" r="49" customHeight="1" ht="35.25" customFormat="1" s="1">
       <c r="A49" s="13"/>
       <c r="B49" s="14" t="s">
-        <v>74</v>
+        <v>107</v>
       </c>
       <c r="C49" s="10"/>
       <c r="D49" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="E49" s="4"/>
+        <v>9</v>
+      </c>
+      <c r="E49" s="4" t="s">
+        <v>91</v>
+      </c>
       <c r="F49" s="4"/>
       <c r="G49" s="4"/>
       <c r="H49" s="4"/>
@@ -3174,13 +3359,15 @@
     <row x14ac:dyDescent="0.25" r="50" customHeight="1" ht="36" customFormat="1" s="1">
       <c r="A50" s="13"/>
       <c r="B50" s="14" t="s">
-        <v>75</v>
+        <v>108</v>
       </c>
       <c r="C50" s="10"/>
       <c r="D50" s="4" t="s">
-        <v>76</v>
-      </c>
-      <c r="E50" s="4"/>
+        <v>98</v>
+      </c>
+      <c r="E50" s="4" t="s">
+        <v>109</v>
+      </c>
       <c r="F50" s="4"/>
       <c r="G50" s="4"/>
       <c r="H50" s="4"/>
@@ -3206,13 +3393,15 @@
     <row x14ac:dyDescent="0.25" r="51" customHeight="1" ht="50.25" customFormat="1" s="1">
       <c r="A51" s="13"/>
       <c r="B51" s="14" t="s">
-        <v>77</v>
+        <v>110</v>
       </c>
       <c r="C51" s="10"/>
       <c r="D51" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="E51" s="4"/>
+        <v>9</v>
+      </c>
+      <c r="E51" s="4" t="s">
+        <v>91</v>
+      </c>
       <c r="F51" s="4"/>
       <c r="G51" s="4"/>
       <c r="H51" s="4"/>
@@ -3238,13 +3427,15 @@
     <row x14ac:dyDescent="0.25" r="52" customHeight="1" ht="36" customFormat="1" s="1">
       <c r="A52" s="13"/>
       <c r="B52" s="14" t="s">
-        <v>78</v>
+        <v>111</v>
       </c>
       <c r="C52" s="10"/>
       <c r="D52" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="E52" s="4"/>
+        <v>9</v>
+      </c>
+      <c r="E52" s="4" t="s">
+        <v>91</v>
+      </c>
       <c r="F52" s="4"/>
       <c r="G52" s="4"/>
       <c r="H52" s="4"/>
@@ -3270,13 +3461,15 @@
     <row x14ac:dyDescent="0.25" r="53" customHeight="1" ht="36.75" customFormat="1" s="1">
       <c r="A53" s="13"/>
       <c r="B53" s="21" t="s">
-        <v>79</v>
+        <v>112</v>
       </c>
       <c r="C53" s="18"/>
       <c r="D53" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="E53" s="4"/>
+        <v>9</v>
+      </c>
+      <c r="E53" s="4" t="s">
+        <v>91</v>
+      </c>
       <c r="F53" s="4"/>
       <c r="G53" s="4"/>
       <c r="H53" s="4"/>
@@ -3302,15 +3495,17 @@
     <row x14ac:dyDescent="0.25" r="54" customHeight="1" ht="44.25" customFormat="1" s="1">
       <c r="A54" s="13"/>
       <c r="B54" s="8" t="s">
-        <v>80</v>
+        <v>113</v>
       </c>
       <c r="C54" s="8" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="D54" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="E54" s="4"/>
+        <v>9</v>
+      </c>
+      <c r="E54" s="4" t="s">
+        <v>91</v>
+      </c>
       <c r="F54" s="4"/>
       <c r="G54" s="4"/>
       <c r="H54" s="4"/>
@@ -3336,15 +3531,17 @@
     <row x14ac:dyDescent="0.25" r="55" customHeight="1" ht="30" customFormat="1" s="1">
       <c r="A55" s="13"/>
       <c r="B55" s="7" t="s">
-        <v>81</v>
+        <v>114</v>
       </c>
       <c r="C55" s="12" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="D55" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="E55" s="4"/>
+        <v>9</v>
+      </c>
+      <c r="E55" s="4" t="s">
+        <v>91</v>
+      </c>
       <c r="F55" s="4"/>
       <c r="G55" s="4"/>
       <c r="H55" s="4"/>
@@ -3370,13 +3567,15 @@
     <row x14ac:dyDescent="0.25" r="56" customHeight="1" ht="30" customFormat="1" s="1">
       <c r="A56" s="13"/>
       <c r="B56" s="14" t="s">
-        <v>82</v>
+        <v>115</v>
       </c>
       <c r="C56" s="10"/>
       <c r="D56" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="E56" s="4"/>
+        <v>9</v>
+      </c>
+      <c r="E56" s="4" t="s">
+        <v>64</v>
+      </c>
       <c r="F56" s="4"/>
       <c r="G56" s="4"/>
       <c r="H56" s="4"/>
@@ -3402,13 +3601,15 @@
     <row x14ac:dyDescent="0.25" r="57" customHeight="1" ht="30" customFormat="1" s="1">
       <c r="A57" s="13"/>
       <c r="B57" s="14" t="s">
-        <v>83</v>
+        <v>116</v>
       </c>
       <c r="C57" s="10"/>
       <c r="D57" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="E57" s="4"/>
+        <v>9</v>
+      </c>
+      <c r="E57" s="4" t="s">
+        <v>64</v>
+      </c>
       <c r="F57" s="4"/>
       <c r="G57" s="4"/>
       <c r="H57" s="4"/>
@@ -3434,13 +3635,15 @@
     <row x14ac:dyDescent="0.25" r="58" customHeight="1" ht="32.25" customFormat="1" s="1">
       <c r="A58" s="13"/>
       <c r="B58" s="14" t="s">
-        <v>84</v>
+        <v>117</v>
       </c>
       <c r="C58" s="10"/>
       <c r="D58" s="4" t="s">
-        <v>85</v>
-      </c>
-      <c r="E58" s="4"/>
+        <v>118</v>
+      </c>
+      <c r="E58" s="4" t="s">
+        <v>91</v>
+      </c>
       <c r="F58" s="4"/>
       <c r="G58" s="4"/>
       <c r="H58" s="4"/>
@@ -3463,14 +3666,14 @@
       <c r="Y58" s="4"/>
       <c r="Z58" s="4"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="59" customHeight="1" ht="18.75" customFormat="1" s="1">
+    <row x14ac:dyDescent="0.25" r="59" customHeight="1" ht="26.25" customFormat="1" s="1">
       <c r="A59" s="13"/>
       <c r="B59" s="21" t="s">
-        <v>86</v>
+        <v>119</v>
       </c>
       <c r="C59" s="18"/>
       <c r="D59" s="4" t="s">
-        <v>52</v>
+        <v>79</v>
       </c>
       <c r="E59" s="4"/>
       <c r="F59" s="4"/>
@@ -3495,18 +3698,20 @@
       <c r="Y59" s="4"/>
       <c r="Z59" s="4"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="60" customHeight="1" ht="30" customFormat="1" s="1">
+    <row x14ac:dyDescent="0.25" r="60" customHeight="1" ht="40.5" customFormat="1" s="1">
       <c r="A60" s="13"/>
       <c r="B60" s="22" t="s">
-        <v>87</v>
+        <v>120</v>
       </c>
       <c r="C60" s="12" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="D60" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="E60" s="4"/>
+        <v>9</v>
+      </c>
+      <c r="E60" s="4" t="s">
+        <v>91</v>
+      </c>
       <c r="F60" s="4"/>
       <c r="G60" s="4"/>
       <c r="H60" s="4"/>
@@ -3529,14 +3734,14 @@
       <c r="Y60" s="4"/>
       <c r="Z60" s="4"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="61" customHeight="1" ht="75.75" customFormat="1" s="1">
+    <row x14ac:dyDescent="0.25" r="61" customHeight="1" ht="49.5" customFormat="1" s="1">
       <c r="A61" s="13"/>
       <c r="B61" s="26" t="s">
-        <v>88</v>
+        <v>121</v>
       </c>
       <c r="C61" s="10"/>
       <c r="D61" s="4" t="s">
-        <v>89</v>
+        <v>122</v>
       </c>
       <c r="E61" s="4"/>
       <c r="F61" s="4"/>
@@ -3564,11 +3769,11 @@
     <row x14ac:dyDescent="0.25" r="62" customHeight="1" ht="18.75" customFormat="1" s="1">
       <c r="A62" s="13"/>
       <c r="B62" s="14" t="s">
-        <v>90</v>
+        <v>123</v>
       </c>
       <c r="C62" s="10"/>
       <c r="D62" s="4" t="s">
-        <v>91</v>
+        <v>124</v>
       </c>
       <c r="E62" s="4"/>
       <c r="F62" s="4"/>
@@ -3596,11 +3801,11 @@
     <row x14ac:dyDescent="0.25" r="63" customHeight="1" ht="18.75" customFormat="1" s="1">
       <c r="A63" s="13"/>
       <c r="B63" s="21" t="s">
-        <v>92</v>
+        <v>125</v>
       </c>
       <c r="C63" s="18"/>
       <c r="D63" s="4" t="s">
-        <v>93</v>
+        <v>79</v>
       </c>
       <c r="E63" s="4"/>
       <c r="F63" s="4"/>
@@ -3628,13 +3833,13 @@
     <row x14ac:dyDescent="0.25" r="64" customHeight="1" ht="33.75" customFormat="1" s="1">
       <c r="A64" s="13"/>
       <c r="B64" s="7" t="s">
-        <v>94</v>
+        <v>126</v>
       </c>
       <c r="C64" s="12" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="D64" s="4" t="s">
-        <v>93</v>
+        <v>79</v>
       </c>
       <c r="E64" s="4"/>
       <c r="F64" s="4"/>
@@ -3662,11 +3867,11 @@
     <row x14ac:dyDescent="0.25" r="65" customHeight="1" ht="30" customFormat="1" s="1">
       <c r="A65" s="13"/>
       <c r="B65" s="14" t="s">
-        <v>95</v>
+        <v>127</v>
       </c>
       <c r="C65" s="10"/>
       <c r="D65" s="4" t="s">
-        <v>96</v>
+        <v>128</v>
       </c>
       <c r="E65" s="4"/>
       <c r="F65" s="4"/>
@@ -3694,11 +3899,11 @@
     <row x14ac:dyDescent="0.25" r="66" customHeight="1" ht="36.75" customFormat="1" s="1">
       <c r="A66" s="13"/>
       <c r="B66" s="14" t="s">
-        <v>97</v>
+        <v>129</v>
       </c>
       <c r="C66" s="10"/>
       <c r="D66" s="4" t="s">
-        <v>93</v>
+        <v>79</v>
       </c>
       <c r="E66" s="4"/>
       <c r="F66" s="4"/>
@@ -3726,11 +3931,11 @@
     <row x14ac:dyDescent="0.25" r="67" customHeight="1" ht="36.75" customFormat="1" s="1">
       <c r="A67" s="13"/>
       <c r="B67" s="21" t="s">
-        <v>98</v>
+        <v>130</v>
       </c>
       <c r="C67" s="18"/>
       <c r="D67" s="4" t="s">
-        <v>93</v>
+        <v>79</v>
       </c>
       <c r="E67" s="4"/>
       <c r="F67" s="4"/>
@@ -3758,13 +3963,13 @@
     <row x14ac:dyDescent="0.25" r="68" customHeight="1" ht="18.75" customFormat="1" s="1">
       <c r="A68" s="13"/>
       <c r="B68" s="7" t="s">
-        <v>99</v>
+        <v>131</v>
       </c>
       <c r="C68" s="12" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="D68" s="4" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E68" s="4"/>
       <c r="F68" s="4"/>
@@ -3792,11 +3997,11 @@
     <row x14ac:dyDescent="0.25" r="69" customHeight="1" ht="18.75" customFormat="1" s="1">
       <c r="A69" s="13"/>
       <c r="B69" s="14" t="s">
-        <v>100</v>
+        <v>132</v>
       </c>
       <c r="C69" s="10"/>
       <c r="D69" s="4" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E69" s="4"/>
       <c r="F69" s="4"/>
@@ -3824,11 +4029,11 @@
     <row x14ac:dyDescent="0.25" r="70" customHeight="1" ht="27" customFormat="1" s="1">
       <c r="A70" s="25"/>
       <c r="B70" s="21" t="s">
-        <v>101</v>
+        <v>133</v>
       </c>
       <c r="C70" s="18"/>
       <c r="D70" s="4" t="s">
-        <v>102</v>
+        <v>134</v>
       </c>
       <c r="E70" s="4"/>
       <c r="F70" s="4"/>
@@ -3855,16 +4060,16 @@
     </row>
     <row x14ac:dyDescent="0.25" r="71" customHeight="1" ht="43.5" customFormat="1" s="1">
       <c r="A71" s="7" t="s">
-        <v>103</v>
+        <v>135</v>
       </c>
       <c r="B71" s="7" t="s">
-        <v>104</v>
+        <v>136</v>
       </c>
       <c r="C71" s="12" t="s">
-        <v>105</v>
+        <v>137</v>
       </c>
       <c r="D71" s="4" t="s">
-        <v>93</v>
+        <v>79</v>
       </c>
       <c r="E71" s="4"/>
       <c r="F71" s="4"/>
@@ -3891,14 +4096,14 @@
     </row>
     <row x14ac:dyDescent="0.25" r="72" customHeight="1" ht="45.75" customFormat="1" s="1">
       <c r="A72" s="20" t="s">
-        <v>106</v>
+        <v>138</v>
       </c>
       <c r="B72" s="14" t="s">
-        <v>107</v>
+        <v>139</v>
       </c>
       <c r="C72" s="10"/>
       <c r="D72" s="4" t="s">
-        <v>108</v>
+        <v>140</v>
       </c>
       <c r="E72" s="4"/>
       <c r="F72" s="4"/>
@@ -3926,11 +4131,11 @@
     <row x14ac:dyDescent="0.25" r="73" customHeight="1" ht="45.75" customFormat="1" s="1">
       <c r="A73" s="10"/>
       <c r="B73" s="14" t="s">
-        <v>109</v>
+        <v>141</v>
       </c>
       <c r="C73" s="10"/>
       <c r="D73" s="4" t="s">
-        <v>93</v>
+        <v>79</v>
       </c>
       <c r="E73" s="4"/>
       <c r="F73" s="4"/>
@@ -3958,11 +4163,11 @@
     <row x14ac:dyDescent="0.25" r="74" customHeight="1" ht="39" customFormat="1" s="1">
       <c r="A74" s="11"/>
       <c r="B74" s="14" t="s">
-        <v>110</v>
+        <v>142</v>
       </c>
       <c r="C74" s="10"/>
       <c r="D74" s="4" t="s">
-        <v>93</v>
+        <v>79</v>
       </c>
       <c r="E74" s="4"/>
       <c r="F74" s="4"/>
@@ -3990,11 +4195,11 @@
     <row x14ac:dyDescent="0.25" r="75" customHeight="1" ht="26.25" customFormat="1" s="1">
       <c r="A75" s="13"/>
       <c r="B75" s="27" t="s">
-        <v>111</v>
+        <v>143</v>
       </c>
       <c r="C75" s="10"/>
       <c r="D75" s="4" t="s">
-        <v>93</v>
+        <v>79</v>
       </c>
       <c r="E75" s="4"/>
       <c r="F75" s="4"/>
@@ -4022,11 +4227,11 @@
     <row x14ac:dyDescent="0.25" r="76" customHeight="1" ht="62.25" customFormat="1" s="1">
       <c r="A76" s="13"/>
       <c r="B76" s="14" t="s">
-        <v>112</v>
+        <v>144</v>
       </c>
       <c r="C76" s="10"/>
       <c r="D76" s="4" t="s">
-        <v>93</v>
+        <v>79</v>
       </c>
       <c r="E76" s="4"/>
       <c r="F76" s="4"/>
@@ -4054,11 +4259,11 @@
     <row x14ac:dyDescent="0.25" r="77" customHeight="1" ht="43.5" customFormat="1" s="1">
       <c r="A77" s="13"/>
       <c r="B77" s="14" t="s">
-        <v>113</v>
+        <v>145</v>
       </c>
       <c r="C77" s="10"/>
       <c r="D77" s="4" t="s">
-        <v>93</v>
+        <v>79</v>
       </c>
       <c r="E77" s="4"/>
       <c r="F77" s="4"/>
@@ -4086,11 +4291,11 @@
     <row x14ac:dyDescent="0.25" r="78" customHeight="1" ht="42" customFormat="1" s="1">
       <c r="A78" s="13"/>
       <c r="B78" s="21" t="s">
-        <v>114</v>
+        <v>146</v>
       </c>
       <c r="C78" s="18"/>
       <c r="D78" s="4" t="s">
-        <v>93</v>
+        <v>79</v>
       </c>
       <c r="E78" s="4"/>
       <c r="F78" s="4"/>
@@ -4118,13 +4323,13 @@
     <row x14ac:dyDescent="0.25" r="79" customHeight="1" ht="36.75" customFormat="1" s="1">
       <c r="A79" s="13"/>
       <c r="B79" s="7" t="s">
-        <v>115</v>
+        <v>147</v>
       </c>
       <c r="C79" s="12" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="D79" s="4" t="s">
-        <v>93</v>
+        <v>79</v>
       </c>
       <c r="E79" s="4"/>
       <c r="F79" s="4"/>
@@ -4152,11 +4357,11 @@
     <row x14ac:dyDescent="0.25" r="80" customHeight="1" ht="62.25" customFormat="1" s="1">
       <c r="A80" s="13"/>
       <c r="B80" s="14" t="s">
-        <v>116</v>
+        <v>148</v>
       </c>
       <c r="C80" s="10"/>
       <c r="D80" s="4" t="s">
-        <v>93</v>
+        <v>79</v>
       </c>
       <c r="E80" s="4"/>
       <c r="F80" s="4"/>
@@ -4184,11 +4389,11 @@
     <row x14ac:dyDescent="0.25" r="81" customHeight="1" ht="62.25" customFormat="1" s="1">
       <c r="A81" s="13"/>
       <c r="B81" s="14" t="s">
-        <v>117</v>
+        <v>149</v>
       </c>
       <c r="C81" s="10"/>
       <c r="D81" s="4" t="s">
-        <v>93</v>
+        <v>79</v>
       </c>
       <c r="E81" s="4"/>
       <c r="F81" s="4"/>
@@ -4216,11 +4421,11 @@
     <row x14ac:dyDescent="0.25" r="82" customHeight="1" ht="62.25" customFormat="1" s="1">
       <c r="A82" s="13"/>
       <c r="B82" s="14" t="s">
-        <v>118</v>
+        <v>150</v>
       </c>
       <c r="C82" s="10"/>
       <c r="D82" s="4" t="s">
-        <v>93</v>
+        <v>79</v>
       </c>
       <c r="E82" s="4"/>
       <c r="F82" s="4"/>
@@ -4248,11 +4453,11 @@
     <row x14ac:dyDescent="0.25" r="83" customHeight="1" ht="62.25" customFormat="1" s="1">
       <c r="A83" s="13"/>
       <c r="B83" s="14" t="s">
-        <v>119</v>
+        <v>151</v>
       </c>
       <c r="C83" s="10"/>
       <c r="D83" s="4" t="s">
-        <v>93</v>
+        <v>79</v>
       </c>
       <c r="E83" s="4"/>
       <c r="F83" s="4"/>
@@ -4280,11 +4485,11 @@
     <row x14ac:dyDescent="0.25" r="84" customHeight="1" ht="62.25" customFormat="1" s="1">
       <c r="A84" s="13"/>
       <c r="B84" s="14" t="s">
-        <v>120</v>
+        <v>152</v>
       </c>
       <c r="C84" s="10"/>
       <c r="D84" s="4" t="s">
-        <v>93</v>
+        <v>79</v>
       </c>
       <c r="E84" s="4"/>
       <c r="F84" s="4"/>
@@ -4312,11 +4517,11 @@
     <row x14ac:dyDescent="0.25" r="85" customHeight="1" ht="36" customFormat="1" s="1">
       <c r="A85" s="13"/>
       <c r="B85" s="14" t="s">
-        <v>121</v>
+        <v>153</v>
       </c>
       <c r="C85" s="10"/>
       <c r="D85" s="4" t="s">
-        <v>93</v>
+        <v>79</v>
       </c>
       <c r="E85" s="4"/>
       <c r="F85" s="4"/>
@@ -4344,11 +4549,11 @@
     <row x14ac:dyDescent="0.25" r="86" customHeight="1" ht="36" customFormat="1" s="1">
       <c r="A86" s="13"/>
       <c r="B86" s="14" t="s">
-        <v>122</v>
+        <v>154</v>
       </c>
       <c r="C86" s="10"/>
       <c r="D86" s="4" t="s">
-        <v>93</v>
+        <v>79</v>
       </c>
       <c r="E86" s="4"/>
       <c r="F86" s="4"/>
@@ -4376,11 +4581,11 @@
     <row x14ac:dyDescent="0.25" r="87" customHeight="1" ht="36" customFormat="1" s="1">
       <c r="A87" s="13"/>
       <c r="B87" s="14" t="s">
-        <v>123</v>
+        <v>155</v>
       </c>
       <c r="C87" s="10"/>
       <c r="D87" s="4" t="s">
-        <v>93</v>
+        <v>79</v>
       </c>
       <c r="E87" s="4"/>
       <c r="F87" s="4"/>
@@ -4408,11 +4613,11 @@
     <row x14ac:dyDescent="0.25" r="88" customHeight="1" ht="50.25" customFormat="1" s="1">
       <c r="A88" s="13"/>
       <c r="B88" s="14" t="s">
-        <v>124</v>
+        <v>156</v>
       </c>
       <c r="C88" s="10"/>
       <c r="D88" s="4" t="s">
-        <v>93</v>
+        <v>79</v>
       </c>
       <c r="E88" s="4"/>
       <c r="F88" s="4"/>
@@ -4440,11 +4645,11 @@
     <row x14ac:dyDescent="0.25" r="89" customHeight="1" ht="36" customFormat="1" s="1">
       <c r="A89" s="13"/>
       <c r="B89" s="14" t="s">
-        <v>125</v>
+        <v>157</v>
       </c>
       <c r="C89" s="10"/>
       <c r="D89" s="4" t="s">
-        <v>93</v>
+        <v>79</v>
       </c>
       <c r="E89" s="4"/>
       <c r="F89" s="4"/>
@@ -4472,11 +4677,11 @@
     <row x14ac:dyDescent="0.25" r="90" customHeight="1" ht="36.75" customFormat="1" s="1">
       <c r="A90" s="13"/>
       <c r="B90" s="21" t="s">
-        <v>126</v>
+        <v>158</v>
       </c>
       <c r="C90" s="18"/>
       <c r="D90" s="4" t="s">
-        <v>93</v>
+        <v>79</v>
       </c>
       <c r="E90" s="4"/>
       <c r="F90" s="4"/>
@@ -4504,13 +4709,13 @@
     <row x14ac:dyDescent="0.25" r="91" customHeight="1" ht="51" customFormat="1" s="1">
       <c r="A91" s="13"/>
       <c r="B91" s="22" t="s">
-        <v>127</v>
+        <v>159</v>
       </c>
       <c r="C91" s="12" t="s">
-        <v>128</v>
+        <v>160</v>
       </c>
       <c r="D91" s="4" t="s">
-        <v>93</v>
+        <v>79</v>
       </c>
       <c r="E91" s="4"/>
       <c r="F91" s="4"/>
@@ -4538,11 +4743,11 @@
     <row x14ac:dyDescent="0.25" r="92" customHeight="1" ht="50.25" customFormat="1" s="1">
       <c r="A92" s="13"/>
       <c r="B92" s="23" t="s">
-        <v>129</v>
+        <v>161</v>
       </c>
       <c r="C92" s="10"/>
       <c r="D92" s="4" t="s">
-        <v>93</v>
+        <v>79</v>
       </c>
       <c r="E92" s="4"/>
       <c r="F92" s="4"/>
@@ -4570,11 +4775,11 @@
     <row x14ac:dyDescent="0.25" r="93" customHeight="1" ht="36" customFormat="1" s="1">
       <c r="A93" s="13"/>
       <c r="B93" s="23" t="s">
-        <v>130</v>
+        <v>162</v>
       </c>
       <c r="C93" s="10"/>
       <c r="D93" s="4" t="s">
-        <v>93</v>
+        <v>79</v>
       </c>
       <c r="E93" s="4"/>
       <c r="F93" s="4"/>
@@ -4602,11 +4807,11 @@
     <row x14ac:dyDescent="0.25" r="94" customHeight="1" ht="36" customFormat="1" s="1">
       <c r="A94" s="13"/>
       <c r="B94" s="23" t="s">
-        <v>131</v>
+        <v>163</v>
       </c>
       <c r="C94" s="10"/>
       <c r="D94" s="4" t="s">
-        <v>93</v>
+        <v>79</v>
       </c>
       <c r="E94" s="4"/>
       <c r="F94" s="4"/>
@@ -4634,11 +4839,11 @@
     <row x14ac:dyDescent="0.25" r="95" customHeight="1" ht="36.75" customFormat="1" s="1">
       <c r="A95" s="25"/>
       <c r="B95" s="17" t="s">
-        <v>132</v>
+        <v>164</v>
       </c>
       <c r="C95" s="18"/>
       <c r="D95" s="4" t="s">
-        <v>93</v>
+        <v>79</v>
       </c>
       <c r="E95" s="4"/>
       <c r="F95" s="4"/>
@@ -4665,16 +4870,16 @@
     </row>
     <row x14ac:dyDescent="0.25" r="96" customHeight="1" ht="64.5" customFormat="1" s="1">
       <c r="A96" s="7" t="s">
-        <v>133</v>
+        <v>165</v>
       </c>
       <c r="B96" s="7" t="s">
-        <v>134</v>
+        <v>166</v>
       </c>
       <c r="C96" s="12" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="D96" s="4" t="s">
-        <v>93</v>
+        <v>79</v>
       </c>
       <c r="E96" s="4"/>
       <c r="F96" s="4"/>
@@ -4701,14 +4906,14 @@
     </row>
     <row x14ac:dyDescent="0.25" r="97" customHeight="1" ht="36" customFormat="1" s="1">
       <c r="A97" s="20" t="s">
-        <v>135</v>
+        <v>167</v>
       </c>
       <c r="B97" s="14" t="s">
-        <v>136</v>
+        <v>168</v>
       </c>
       <c r="C97" s="10"/>
       <c r="D97" s="4" t="s">
-        <v>93</v>
+        <v>79</v>
       </c>
       <c r="E97" s="4"/>
       <c r="F97" s="4"/>
@@ -4736,11 +4941,11 @@
     <row x14ac:dyDescent="0.25" r="98" customHeight="1" ht="50.25" customFormat="1" s="1">
       <c r="A98" s="10"/>
       <c r="B98" s="14" t="s">
-        <v>137</v>
+        <v>169</v>
       </c>
       <c r="C98" s="10"/>
       <c r="D98" s="4" t="s">
-        <v>93</v>
+        <v>79</v>
       </c>
       <c r="E98" s="4"/>
       <c r="F98" s="4"/>
@@ -4768,11 +4973,11 @@
     <row x14ac:dyDescent="0.25" r="99" customHeight="1" ht="72.75" customFormat="1" s="1">
       <c r="A99" s="11"/>
       <c r="B99" s="21" t="s">
-        <v>138</v>
+        <v>170</v>
       </c>
       <c r="C99" s="18"/>
       <c r="D99" s="4" t="s">
-        <v>93</v>
+        <v>79</v>
       </c>
       <c r="E99" s="4"/>
       <c r="F99" s="4"/>
@@ -4800,13 +5005,13 @@
     <row x14ac:dyDescent="0.25" r="100" customHeight="1" ht="36" customFormat="1" s="1">
       <c r="A100" s="13"/>
       <c r="B100" s="7" t="s">
-        <v>139</v>
+        <v>171</v>
       </c>
       <c r="C100" s="12" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="D100" s="4" t="s">
-        <v>93</v>
+        <v>79</v>
       </c>
       <c r="E100" s="4"/>
       <c r="F100" s="4"/>
@@ -4834,11 +5039,11 @@
     <row x14ac:dyDescent="0.25" r="101" customHeight="1" ht="50.25" customFormat="1" s="1">
       <c r="A101" s="13"/>
       <c r="B101" s="14" t="s">
-        <v>140</v>
+        <v>172</v>
       </c>
       <c r="C101" s="10"/>
       <c r="D101" s="4" t="s">
-        <v>93</v>
+        <v>79</v>
       </c>
       <c r="E101" s="4"/>
       <c r="F101" s="4"/>
@@ -4866,11 +5071,11 @@
     <row x14ac:dyDescent="0.25" r="102" customHeight="1" ht="63" customFormat="1" s="1">
       <c r="A102" s="13"/>
       <c r="B102" s="21" t="s">
-        <v>141</v>
+        <v>173</v>
       </c>
       <c r="C102" s="18"/>
       <c r="D102" s="4" t="s">
-        <v>93</v>
+        <v>79</v>
       </c>
       <c r="E102" s="4"/>
       <c r="F102" s="4"/>
@@ -4898,13 +5103,13 @@
     <row x14ac:dyDescent="0.25" r="103" customHeight="1" ht="36.75" customFormat="1" s="1">
       <c r="A103" s="13"/>
       <c r="B103" s="7" t="s">
-        <v>142</v>
+        <v>174</v>
       </c>
       <c r="C103" s="12" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="D103" s="4" t="s">
-        <v>93</v>
+        <v>79</v>
       </c>
       <c r="E103" s="4"/>
       <c r="F103" s="4"/>
@@ -4932,11 +5137,11 @@
     <row x14ac:dyDescent="0.25" r="104" customHeight="1" ht="50.25" customFormat="1" s="1">
       <c r="A104" s="13"/>
       <c r="B104" s="14" t="s">
-        <v>143</v>
+        <v>175</v>
       </c>
       <c r="C104" s="10"/>
       <c r="D104" s="4" t="s">
-        <v>93</v>
+        <v>79</v>
       </c>
       <c r="E104" s="4"/>
       <c r="F104" s="4"/>
@@ -4964,11 +5169,11 @@
     <row x14ac:dyDescent="0.25" r="105" customHeight="1" ht="36.75" customFormat="1" s="1">
       <c r="A105" s="13"/>
       <c r="B105" s="21" t="s">
-        <v>144</v>
+        <v>176</v>
       </c>
       <c r="C105" s="18"/>
       <c r="D105" s="4" t="s">
-        <v>93</v>
+        <v>79</v>
       </c>
       <c r="E105" s="4"/>
       <c r="F105" s="4"/>
@@ -4996,13 +5201,13 @@
     <row x14ac:dyDescent="0.25" r="106" customHeight="1" ht="51" customFormat="1" s="1">
       <c r="A106" s="13"/>
       <c r="B106" s="7" t="s">
-        <v>145</v>
+        <v>177</v>
       </c>
       <c r="C106" s="12" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="D106" s="4" t="s">
-        <v>93</v>
+        <v>79</v>
       </c>
       <c r="E106" s="4"/>
       <c r="F106" s="4"/>
@@ -5030,11 +5235,11 @@
     <row x14ac:dyDescent="0.25" r="107" customHeight="1" ht="36" customFormat="1" s="1">
       <c r="A107" s="13"/>
       <c r="B107" s="14" t="s">
-        <v>146</v>
+        <v>178</v>
       </c>
       <c r="C107" s="10"/>
       <c r="D107" s="4" t="s">
-        <v>93</v>
+        <v>79</v>
       </c>
       <c r="E107" s="4"/>
       <c r="F107" s="4"/>
@@ -5062,11 +5267,11 @@
     <row x14ac:dyDescent="0.25" r="108" customHeight="1" ht="36" customFormat="1" s="1">
       <c r="A108" s="13"/>
       <c r="B108" s="14" t="s">
-        <v>147</v>
+        <v>179</v>
       </c>
       <c r="C108" s="10"/>
       <c r="D108" s="4" t="s">
-        <v>93</v>
+        <v>79</v>
       </c>
       <c r="E108" s="4"/>
       <c r="F108" s="4"/>
@@ -5094,11 +5299,11 @@
     <row x14ac:dyDescent="0.25" r="109" customHeight="1" ht="21.75" customFormat="1" s="1">
       <c r="A109" s="13"/>
       <c r="B109" s="14" t="s">
-        <v>148</v>
+        <v>180</v>
       </c>
       <c r="C109" s="10"/>
       <c r="D109" s="4" t="s">
-        <v>93</v>
+        <v>79</v>
       </c>
       <c r="E109" s="4"/>
       <c r="F109" s="4"/>
@@ -5126,11 +5331,11 @@
     <row x14ac:dyDescent="0.25" r="110" customHeight="1" ht="36" customFormat="1" s="1">
       <c r="A110" s="13"/>
       <c r="B110" s="14" t="s">
-        <v>149</v>
+        <v>181</v>
       </c>
       <c r="C110" s="10"/>
       <c r="D110" s="4" t="s">
-        <v>93</v>
+        <v>79</v>
       </c>
       <c r="E110" s="4"/>
       <c r="F110" s="4"/>
@@ -5158,11 +5363,11 @@
     <row x14ac:dyDescent="0.25" r="111" customHeight="1" ht="36.75" customFormat="1" s="1">
       <c r="A111" s="13"/>
       <c r="B111" s="21" t="s">
-        <v>150</v>
+        <v>182</v>
       </c>
       <c r="C111" s="18"/>
       <c r="D111" s="4" t="s">
-        <v>93</v>
+        <v>79</v>
       </c>
       <c r="E111" s="4"/>
       <c r="F111" s="4"/>
@@ -5190,13 +5395,13 @@
     <row x14ac:dyDescent="0.25" r="112" customHeight="1" ht="36.75" customFormat="1" s="1">
       <c r="A112" s="13"/>
       <c r="B112" s="7" t="s">
-        <v>151</v>
+        <v>183</v>
       </c>
       <c r="C112" s="12" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="D112" s="4" t="s">
-        <v>93</v>
+        <v>79</v>
       </c>
       <c r="E112" s="4"/>
       <c r="F112" s="4"/>
@@ -5224,11 +5429,11 @@
     <row x14ac:dyDescent="0.25" r="113" customHeight="1" ht="36" customFormat="1" s="1">
       <c r="A113" s="13"/>
       <c r="B113" s="14" t="s">
-        <v>152</v>
+        <v>184</v>
       </c>
       <c r="C113" s="10"/>
       <c r="D113" s="4" t="s">
-        <v>93</v>
+        <v>79</v>
       </c>
       <c r="E113" s="4"/>
       <c r="F113" s="4"/>
@@ -5256,11 +5461,11 @@
     <row x14ac:dyDescent="0.25" r="114" customHeight="1" ht="50.25" customFormat="1" s="1">
       <c r="A114" s="13"/>
       <c r="B114" s="14" t="s">
-        <v>153</v>
+        <v>185</v>
       </c>
       <c r="C114" s="10"/>
       <c r="D114" s="4" t="s">
-        <v>93</v>
+        <v>79</v>
       </c>
       <c r="E114" s="4"/>
       <c r="F114" s="4"/>
@@ -5288,11 +5493,11 @@
     <row x14ac:dyDescent="0.25" r="115" customHeight="1" ht="36" customFormat="1" s="1">
       <c r="A115" s="13"/>
       <c r="B115" s="14" t="s">
-        <v>154</v>
+        <v>186</v>
       </c>
       <c r="C115" s="10"/>
       <c r="D115" s="4" t="s">
-        <v>93</v>
+        <v>79</v>
       </c>
       <c r="E115" s="4"/>
       <c r="F115" s="4"/>
@@ -5320,11 +5525,11 @@
     <row x14ac:dyDescent="0.25" r="116" customHeight="1" ht="30.75" customFormat="1" s="1">
       <c r="A116" s="25"/>
       <c r="B116" s="21" t="s">
-        <v>155</v>
+        <v>187</v>
       </c>
       <c r="C116" s="18"/>
       <c r="D116" s="4" t="s">
-        <v>156</v>
+        <v>79</v>
       </c>
       <c r="E116" s="4"/>
       <c r="F116" s="4"/>

</xml_diff>

<commit_message>
Ajout Notion dans referenciel
</commit_message>
<xml_diff>
--- a/Referentiel_DFS.xlsx
+++ b/Referentiel_DFS.xlsx
@@ -14,9 +14,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="330" uniqueCount="188">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="332" uniqueCount="190">
   <si>
     <t>Tableau 1</t>
+  </si>
+  <si>
+    <t>Adresse Notion Purpaws</t>
   </si>
   <si>
     <r>
@@ -117,7 +120,23 @@
     </r>
   </si>
   <si>
-    <t>Commentaires</t>
+    <r>
+      <t/>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF00bfff"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Commentaires</t>
+    </r>
+  </si>
+  <si>
+    <t>https://www.notion.so/2bc88f7eba4b44e4966981b8d4813649?v=cc756b50ed1d45a59888e91eab66719d</t>
   </si>
   <si>
     <r>
@@ -1623,7 +1642,7 @@
     <col min="3" max="3" style="28" width="29.576428571428572" customWidth="1" bestFit="1"/>
     <col min="4" max="4" style="28" width="22.14785714285714" customWidth="1" bestFit="1"/>
     <col min="5" max="5" style="28" width="16.290714285714284" customWidth="1" bestFit="1"/>
-    <col min="6" max="6" style="28" width="16.290714285714284" customWidth="1" bestFit="1"/>
+    <col min="6" max="6" style="28" width="51.86214285714286" customWidth="1" bestFit="1"/>
     <col min="7" max="7" style="28" width="16.290714285714284" customWidth="1" bestFit="1"/>
     <col min="8" max="8" style="28" width="16.290714285714284" customWidth="1" bestFit="1"/>
     <col min="9" max="9" style="28" width="16.290714285714284" customWidth="1" bestFit="1"/>
@@ -1654,7 +1673,9 @@
       <c r="C1" s="3"/>
       <c r="D1" s="4"/>
       <c r="E1" s="4"/>
-      <c r="F1" s="4"/>
+      <c r="F1" s="4" t="s">
+        <v>1</v>
+      </c>
       <c r="G1" s="4"/>
       <c r="H1" s="4"/>
       <c r="I1" s="4"/>
@@ -1678,21 +1699,23 @@
     </row>
     <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="139.5" customFormat="1" s="1">
       <c r="A2" s="5" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C2" s="6" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="F2" s="4"/>
+        <v>6</v>
+      </c>
+      <c r="F2" s="4" t="s">
+        <v>7</v>
+      </c>
       <c r="G2" s="4"/>
       <c r="H2" s="4"/>
       <c r="I2" s="4"/>
@@ -1716,19 +1739,19 @@
     </row>
     <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="85.5" customFormat="1" s="1">
       <c r="A3" s="7" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="B3" s="8" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="C3" s="8" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="E3" s="4" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="F3" s="4"/>
       <c r="G3" s="4"/>
@@ -1754,19 +1777,19 @@
     </row>
     <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="47.4375" customFormat="1" s="1">
       <c r="A4" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="B4" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="C4" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="D4" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="B4" s="8" t="s">
-        <v>12</v>
-      </c>
-      <c r="C4" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="D4" s="4" t="s">
-        <v>9</v>
-      </c>
       <c r="E4" s="4" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="F4" s="4"/>
       <c r="G4" s="4"/>
@@ -1790,19 +1813,19 @@
       <c r="Y4" s="4"/>
       <c r="Z4" s="4"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="40.5" customFormat="1" s="1">
+    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="96" customFormat="1" s="1">
       <c r="A5" s="10"/>
       <c r="B5" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="C5" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="C5" s="8" t="s">
-        <v>13</v>
-      </c>
       <c r="D5" s="4" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="E5" s="4" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="F5" s="4"/>
       <c r="G5" s="4"/>
@@ -1829,16 +1852,16 @@
     <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="63" customFormat="1" s="1">
       <c r="A6" s="10"/>
       <c r="B6" s="8" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="C6" s="8" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="E6" s="4" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="F6" s="4"/>
       <c r="G6" s="4"/>
@@ -1865,16 +1888,16 @@
     <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="39.75" customFormat="1" s="1">
       <c r="A7" s="11"/>
       <c r="B7" s="7" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="C7" s="12" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="D7" s="4" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="E7" s="4" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="F7" s="4"/>
       <c r="G7" s="4"/>
@@ -1898,17 +1921,17 @@
       <c r="Y7" s="4"/>
       <c r="Z7" s="4"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="54" customFormat="1" s="1">
+    <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="51" customFormat="1" s="1">
       <c r="A8" s="13"/>
       <c r="B8" s="14" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="C8" s="10"/>
       <c r="D8" s="4" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="E8" s="4" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="F8" s="4"/>
       <c r="G8" s="4"/>
@@ -1935,14 +1958,14 @@
     <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="44.25" customFormat="1" s="1">
       <c r="A9" s="13"/>
       <c r="B9" s="14" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="C9" s="10"/>
       <c r="D9" s="4" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="E9" s="4" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="F9" s="4"/>
       <c r="G9" s="4"/>
@@ -1969,14 +1992,14 @@
     <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="36" customFormat="1" s="1">
       <c r="A10" s="13"/>
       <c r="B10" s="15" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="C10" s="10"/>
       <c r="D10" s="4" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="E10" s="4" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="F10" s="4"/>
       <c r="G10" s="4"/>
@@ -2003,14 +2026,14 @@
     <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="31.5" customFormat="1" s="1">
       <c r="A11" s="16"/>
       <c r="B11" s="17" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="C11" s="18"/>
       <c r="D11" s="4" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="E11" s="4" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="F11" s="4"/>
       <c r="G11" s="4"/>
@@ -2037,16 +2060,16 @@
     <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="42" customFormat="1" s="1">
       <c r="A12" s="19"/>
       <c r="B12" s="8" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="C12" s="8" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="D12" s="4" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="E12" s="4" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="F12" s="4"/>
       <c r="G12" s="4"/>
@@ -2073,16 +2096,16 @@
     <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="33.75" customFormat="1" s="1">
       <c r="A13" s="17"/>
       <c r="B13" s="8" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="C13" s="8" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="D13" s="4" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="E13" s="4" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="F13" s="4"/>
       <c r="G13" s="4"/>
@@ -2108,19 +2131,19 @@
     </row>
     <row x14ac:dyDescent="0.25" r="14" customHeight="1" ht="45" customFormat="1" s="1">
       <c r="A14" s="7" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="B14" s="8" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="C14" s="8" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="D14" s="4" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="E14" s="4" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="F14" s="4"/>
       <c r="G14" s="4"/>
@@ -2146,19 +2169,19 @@
     </row>
     <row x14ac:dyDescent="0.25" r="15" customHeight="1" ht="36.75" customFormat="1" s="1">
       <c r="A15" s="20" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="B15" s="7" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="C15" s="12" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="D15" s="4" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="E15" s="4" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="F15" s="4"/>
       <c r="G15" s="4"/>
@@ -2185,14 +2208,14 @@
     <row x14ac:dyDescent="0.25" r="16" customHeight="1" ht="36" customFormat="1" s="1">
       <c r="A16" s="10"/>
       <c r="B16" s="14" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="C16" s="10"/>
       <c r="D16" s="4" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="E16" s="4" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="F16" s="4"/>
       <c r="G16" s="4"/>
@@ -2219,14 +2242,14 @@
     <row x14ac:dyDescent="0.25" r="17" customHeight="1" ht="42.75" customFormat="1" s="1">
       <c r="A17" s="11"/>
       <c r="B17" s="14" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="C17" s="10"/>
       <c r="D17" s="4" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="E17" s="4" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="F17" s="4"/>
       <c r="G17" s="4"/>
@@ -2253,14 +2276,14 @@
     <row x14ac:dyDescent="0.25" r="18" customHeight="1" ht="36.75" customFormat="1" s="1">
       <c r="A18" s="13"/>
       <c r="B18" s="21" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="C18" s="18"/>
       <c r="D18" s="4" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="E18" s="4" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="F18" s="4"/>
       <c r="G18" s="4"/>
@@ -2287,16 +2310,16 @@
     <row x14ac:dyDescent="0.25" r="19" customHeight="1" ht="51" customFormat="1" s="1">
       <c r="A19" s="13"/>
       <c r="B19" s="22" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="C19" s="12" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="D19" s="4" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="E19" s="4" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="F19" s="4"/>
       <c r="G19" s="4"/>
@@ -2323,14 +2346,14 @@
     <row x14ac:dyDescent="0.25" r="20" customHeight="1" ht="36" customFormat="1" s="1">
       <c r="A20" s="13"/>
       <c r="B20" s="23" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="C20" s="10"/>
       <c r="D20" s="4" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="E20" s="4" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="F20" s="4"/>
       <c r="G20" s="4"/>
@@ -2357,14 +2380,14 @@
     <row x14ac:dyDescent="0.25" r="21" customHeight="1" ht="50.25" customFormat="1" s="1">
       <c r="A21" s="13"/>
       <c r="B21" s="23" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="C21" s="10"/>
       <c r="D21" s="4" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="E21" s="4" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="F21" s="4"/>
       <c r="G21" s="4"/>
@@ -2391,14 +2414,14 @@
     <row x14ac:dyDescent="0.25" r="22" customHeight="1" ht="51" customFormat="1" s="1">
       <c r="A22" s="13"/>
       <c r="B22" s="24" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="C22" s="18"/>
       <c r="D22" s="4" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="E22" s="4" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="F22" s="4"/>
       <c r="G22" s="4"/>
@@ -2425,16 +2448,16 @@
     <row x14ac:dyDescent="0.25" r="23" customHeight="1" ht="37.5" customFormat="1" s="1">
       <c r="A23" s="25"/>
       <c r="B23" s="8" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="C23" s="8" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="D23" s="4" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="E23" s="4" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="F23" s="4"/>
       <c r="G23" s="4"/>
@@ -2460,19 +2483,19 @@
     </row>
     <row x14ac:dyDescent="0.25" r="24" customHeight="1" ht="57" customFormat="1" s="1">
       <c r="A24" s="7" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="B24" s="7" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="C24" s="12" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="D24" s="4" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="E24" s="4" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="F24" s="4"/>
       <c r="G24" s="4"/>
@@ -2498,17 +2521,17 @@
     </row>
     <row x14ac:dyDescent="0.25" r="25" customHeight="1" ht="36" customFormat="1" s="1">
       <c r="A25" s="20" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="B25" s="14" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="C25" s="10"/>
       <c r="D25" s="4" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="E25" s="4" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="F25" s="4"/>
       <c r="G25" s="4"/>
@@ -2535,14 +2558,14 @@
     <row x14ac:dyDescent="0.25" r="26" customHeight="1" ht="50.25" customFormat="1" s="1">
       <c r="A26" s="10"/>
       <c r="B26" s="14" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="C26" s="10"/>
       <c r="D26" s="4" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="E26" s="4" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="F26" s="4"/>
       <c r="G26" s="4"/>
@@ -2569,14 +2592,14 @@
     <row x14ac:dyDescent="0.25" r="27" customHeight="1" ht="35.75" customFormat="1" s="1">
       <c r="A27" s="11"/>
       <c r="B27" s="14" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="C27" s="10"/>
       <c r="D27" s="4" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="E27" s="4" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="F27" s="4"/>
       <c r="G27" s="4"/>
@@ -2603,14 +2626,14 @@
     <row x14ac:dyDescent="0.25" r="28" customHeight="1" ht="28.5" customFormat="1" s="1">
       <c r="A28" s="13"/>
       <c r="B28" s="14" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="C28" s="10"/>
       <c r="D28" s="4" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="E28" s="4" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="F28" s="4"/>
       <c r="G28" s="4"/>
@@ -2637,14 +2660,14 @@
     <row x14ac:dyDescent="0.25" r="29" customHeight="1" ht="39.75" customFormat="1" s="1">
       <c r="A29" s="13"/>
       <c r="B29" s="14" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="C29" s="10"/>
       <c r="D29" s="4" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="E29" s="4" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="F29" s="4"/>
       <c r="G29" s="4"/>
@@ -2671,14 +2694,14 @@
     <row x14ac:dyDescent="0.25" r="30" customHeight="1" ht="18.75" customFormat="1" s="1">
       <c r="A30" s="13"/>
       <c r="B30" s="14" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="C30" s="10"/>
       <c r="D30" s="4" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="E30" s="4" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="F30" s="4"/>
       <c r="G30" s="4"/>
@@ -2705,14 +2728,14 @@
     <row x14ac:dyDescent="0.25" r="31" customHeight="1" ht="28.5" customFormat="1" s="1">
       <c r="A31" s="13"/>
       <c r="B31" s="14" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="C31" s="10"/>
       <c r="D31" s="4" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="E31" s="4" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="F31" s="4"/>
       <c r="G31" s="4"/>
@@ -2739,14 +2762,14 @@
     <row x14ac:dyDescent="0.25" r="32" customHeight="1" ht="29.25" customFormat="1" s="1">
       <c r="A32" s="13"/>
       <c r="B32" s="21" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="C32" s="18"/>
       <c r="D32" s="4" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="E32" s="4" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="F32" s="4"/>
       <c r="G32" s="4"/>
@@ -2773,16 +2796,16 @@
     <row x14ac:dyDescent="0.25" r="33" customHeight="1" ht="39.75" customFormat="1" s="1">
       <c r="A33" s="13"/>
       <c r="B33" s="7" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="C33" s="12" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="D33" s="4" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="E33" s="4" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="F33" s="4"/>
       <c r="G33" s="4"/>
@@ -2809,11 +2832,11 @@
     <row x14ac:dyDescent="0.25" r="34" customHeight="1" ht="51" customFormat="1" s="1">
       <c r="A34" s="13"/>
       <c r="B34" s="14" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="C34" s="10"/>
       <c r="D34" s="4" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="E34" s="4"/>
       <c r="F34" s="4"/>
@@ -2841,11 +2864,11 @@
     <row x14ac:dyDescent="0.25" r="35" customHeight="1" ht="51" customFormat="1" s="1">
       <c r="A35" s="13"/>
       <c r="B35" s="14" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="C35" s="10"/>
       <c r="D35" s="4" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="E35" s="4"/>
       <c r="F35" s="4"/>
@@ -2873,14 +2896,14 @@
     <row x14ac:dyDescent="0.25" r="36" customHeight="1" ht="18.75" customFormat="1" s="1">
       <c r="A36" s="13"/>
       <c r="B36" s="14" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="C36" s="10"/>
       <c r="D36" s="4" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="E36" s="4" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="F36" s="4"/>
       <c r="G36" s="4"/>
@@ -2907,14 +2930,14 @@
     <row x14ac:dyDescent="0.25" r="37" customHeight="1" ht="29.25" customFormat="1" s="1">
       <c r="A37" s="13"/>
       <c r="B37" s="21" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="C37" s="18"/>
       <c r="D37" s="4" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="E37" s="4" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="F37" s="4"/>
       <c r="G37" s="4"/>
@@ -2941,16 +2964,16 @@
     <row x14ac:dyDescent="0.25" r="38" customHeight="1" ht="28.5" customFormat="1" s="1">
       <c r="A38" s="13"/>
       <c r="B38" s="7" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="C38" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="D38" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="E38" s="4" t="s">
         <v>86</v>
-      </c>
-      <c r="D38" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="E38" s="4" t="s">
-        <v>84</v>
       </c>
       <c r="F38" s="4"/>
       <c r="G38" s="4"/>
@@ -2977,14 +3000,14 @@
     <row x14ac:dyDescent="0.25" r="39" customHeight="1" ht="28.5" customFormat="1" s="1">
       <c r="A39" s="13"/>
       <c r="B39" s="14" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="C39" s="10"/>
       <c r="D39" s="4" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="E39" s="4" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="F39" s="4"/>
       <c r="G39" s="4"/>
@@ -3011,14 +3034,14 @@
     <row x14ac:dyDescent="0.25" r="40" customHeight="1" ht="28.5" customFormat="1" s="1">
       <c r="A40" s="13"/>
       <c r="B40" s="14" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="C40" s="10"/>
       <c r="D40" s="4" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="E40" s="4" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="F40" s="4"/>
       <c r="G40" s="4"/>
@@ -3045,14 +3068,14 @@
     <row x14ac:dyDescent="0.25" r="41" customHeight="1" ht="40.5" customFormat="1" s="1">
       <c r="A41" s="25"/>
       <c r="B41" s="21" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="C41" s="18"/>
       <c r="D41" s="4" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="E41" s="4" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="F41" s="4"/>
       <c r="G41" s="4"/>
@@ -3078,19 +3101,19 @@
     </row>
     <row x14ac:dyDescent="0.25" r="42" customHeight="1" ht="51" customFormat="1" s="1">
       <c r="A42" s="7" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="B42" s="7" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
       <c r="C42" s="12" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="D42" s="4" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="E42" s="4" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="F42" s="4"/>
       <c r="G42" s="4"/>
@@ -3116,17 +3139,17 @@
     </row>
     <row x14ac:dyDescent="0.25" r="43" customHeight="1" ht="27.75" customFormat="1" s="1">
       <c r="A43" s="20" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="B43" s="14" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="C43" s="10"/>
       <c r="D43" s="4" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="E43" s="4" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="F43" s="4"/>
       <c r="G43" s="4"/>
@@ -3153,14 +3176,14 @@
     <row x14ac:dyDescent="0.25" r="44" customHeight="1" ht="27.75" customFormat="1" s="1">
       <c r="A44" s="10"/>
       <c r="B44" s="14" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="C44" s="10"/>
       <c r="D44" s="4" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="E44" s="4" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="F44" s="4"/>
       <c r="G44" s="4"/>
@@ -3187,14 +3210,14 @@
     <row x14ac:dyDescent="0.25" r="45" customHeight="1" ht="27.75" customFormat="1" s="1">
       <c r="A45" s="10"/>
       <c r="B45" s="14" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="C45" s="10"/>
       <c r="D45" s="4" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="E45" s="4" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="F45" s="4"/>
       <c r="G45" s="4"/>
@@ -3221,14 +3244,14 @@
     <row x14ac:dyDescent="0.25" r="46" customHeight="1" ht="66" customFormat="1" s="1">
       <c r="A46" s="11"/>
       <c r="B46" s="14" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="C46" s="10"/>
       <c r="D46" s="4" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="E46" s="4" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="F46" s="4"/>
       <c r="G46" s="4"/>
@@ -3255,14 +3278,14 @@
     <row x14ac:dyDescent="0.25" r="47" customHeight="1" ht="30.75" customFormat="1" s="1">
       <c r="A47" s="13"/>
       <c r="B47" s="21" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="C47" s="18"/>
       <c r="D47" s="4" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="E47" s="4" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="F47" s="4"/>
       <c r="G47" s="4"/>
@@ -3289,16 +3312,16 @@
     <row x14ac:dyDescent="0.25" r="48" customHeight="1" ht="42.75" customFormat="1" s="1">
       <c r="A48" s="13"/>
       <c r="B48" s="7" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="C48" s="12" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="D48" s="4" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="E48" s="4" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="F48" s="4"/>
       <c r="G48" s="4"/>
@@ -3325,14 +3348,14 @@
     <row x14ac:dyDescent="0.25" r="49" customHeight="1" ht="35.25" customFormat="1" s="1">
       <c r="A49" s="13"/>
       <c r="B49" s="14" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="C49" s="10"/>
       <c r="D49" s="4" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="E49" s="4" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="F49" s="4"/>
       <c r="G49" s="4"/>
@@ -3359,14 +3382,14 @@
     <row x14ac:dyDescent="0.25" r="50" customHeight="1" ht="36" customFormat="1" s="1">
       <c r="A50" s="13"/>
       <c r="B50" s="14" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
       <c r="C50" s="10"/>
       <c r="D50" s="4" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="E50" s="4" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
       <c r="F50" s="4"/>
       <c r="G50" s="4"/>
@@ -3393,14 +3416,14 @@
     <row x14ac:dyDescent="0.25" r="51" customHeight="1" ht="50.25" customFormat="1" s="1">
       <c r="A51" s="13"/>
       <c r="B51" s="14" t="s">
-        <v>110</v>
+        <v>112</v>
       </c>
       <c r="C51" s="10"/>
       <c r="D51" s="4" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="E51" s="4" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="F51" s="4"/>
       <c r="G51" s="4"/>
@@ -3427,14 +3450,14 @@
     <row x14ac:dyDescent="0.25" r="52" customHeight="1" ht="36" customFormat="1" s="1">
       <c r="A52" s="13"/>
       <c r="B52" s="14" t="s">
-        <v>111</v>
+        <v>113</v>
       </c>
       <c r="C52" s="10"/>
       <c r="D52" s="4" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="E52" s="4" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="F52" s="4"/>
       <c r="G52" s="4"/>
@@ -3461,14 +3484,14 @@
     <row x14ac:dyDescent="0.25" r="53" customHeight="1" ht="36.75" customFormat="1" s="1">
       <c r="A53" s="13"/>
       <c r="B53" s="21" t="s">
-        <v>112</v>
+        <v>114</v>
       </c>
       <c r="C53" s="18"/>
       <c r="D53" s="4" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="E53" s="4" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="F53" s="4"/>
       <c r="G53" s="4"/>
@@ -3495,16 +3518,16 @@
     <row x14ac:dyDescent="0.25" r="54" customHeight="1" ht="44.25" customFormat="1" s="1">
       <c r="A54" s="13"/>
       <c r="B54" s="8" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="C54" s="8" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="D54" s="4" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="E54" s="4" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="F54" s="4"/>
       <c r="G54" s="4"/>
@@ -3531,16 +3554,16 @@
     <row x14ac:dyDescent="0.25" r="55" customHeight="1" ht="30" customFormat="1" s="1">
       <c r="A55" s="13"/>
       <c r="B55" s="7" t="s">
-        <v>114</v>
+        <v>116</v>
       </c>
       <c r="C55" s="12" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="D55" s="4" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="E55" s="4" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="F55" s="4"/>
       <c r="G55" s="4"/>
@@ -3567,14 +3590,14 @@
     <row x14ac:dyDescent="0.25" r="56" customHeight="1" ht="30" customFormat="1" s="1">
       <c r="A56" s="13"/>
       <c r="B56" s="14" t="s">
-        <v>115</v>
+        <v>117</v>
       </c>
       <c r="C56" s="10"/>
       <c r="D56" s="4" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="E56" s="4" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="F56" s="4"/>
       <c r="G56" s="4"/>
@@ -3601,14 +3624,14 @@
     <row x14ac:dyDescent="0.25" r="57" customHeight="1" ht="30" customFormat="1" s="1">
       <c r="A57" s="13"/>
       <c r="B57" s="14" t="s">
-        <v>116</v>
+        <v>118</v>
       </c>
       <c r="C57" s="10"/>
       <c r="D57" s="4" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="E57" s="4" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="F57" s="4"/>
       <c r="G57" s="4"/>
@@ -3635,14 +3658,14 @@
     <row x14ac:dyDescent="0.25" r="58" customHeight="1" ht="32.25" customFormat="1" s="1">
       <c r="A58" s="13"/>
       <c r="B58" s="14" t="s">
-        <v>117</v>
+        <v>119</v>
       </c>
       <c r="C58" s="10"/>
       <c r="D58" s="4" t="s">
-        <v>118</v>
+        <v>120</v>
       </c>
       <c r="E58" s="4" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="F58" s="4"/>
       <c r="G58" s="4"/>
@@ -3669,11 +3692,11 @@
     <row x14ac:dyDescent="0.25" r="59" customHeight="1" ht="26.25" customFormat="1" s="1">
       <c r="A59" s="13"/>
       <c r="B59" s="21" t="s">
-        <v>119</v>
+        <v>121</v>
       </c>
       <c r="C59" s="18"/>
       <c r="D59" s="4" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="E59" s="4"/>
       <c r="F59" s="4"/>
@@ -3701,16 +3724,16 @@
     <row x14ac:dyDescent="0.25" r="60" customHeight="1" ht="40.5" customFormat="1" s="1">
       <c r="A60" s="13"/>
       <c r="B60" s="22" t="s">
-        <v>120</v>
+        <v>122</v>
       </c>
       <c r="C60" s="12" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="D60" s="4" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="E60" s="4" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="F60" s="4"/>
       <c r="G60" s="4"/>
@@ -3737,11 +3760,11 @@
     <row x14ac:dyDescent="0.25" r="61" customHeight="1" ht="49.5" customFormat="1" s="1">
       <c r="A61" s="13"/>
       <c r="B61" s="26" t="s">
-        <v>121</v>
+        <v>123</v>
       </c>
       <c r="C61" s="10"/>
       <c r="D61" s="4" t="s">
-        <v>122</v>
+        <v>124</v>
       </c>
       <c r="E61" s="4"/>
       <c r="F61" s="4"/>
@@ -3769,11 +3792,11 @@
     <row x14ac:dyDescent="0.25" r="62" customHeight="1" ht="18.75" customFormat="1" s="1">
       <c r="A62" s="13"/>
       <c r="B62" s="14" t="s">
-        <v>123</v>
+        <v>125</v>
       </c>
       <c r="C62" s="10"/>
       <c r="D62" s="4" t="s">
-        <v>124</v>
+        <v>126</v>
       </c>
       <c r="E62" s="4"/>
       <c r="F62" s="4"/>
@@ -3801,11 +3824,11 @@
     <row x14ac:dyDescent="0.25" r="63" customHeight="1" ht="18.75" customFormat="1" s="1">
       <c r="A63" s="13"/>
       <c r="B63" s="21" t="s">
-        <v>125</v>
+        <v>127</v>
       </c>
       <c r="C63" s="18"/>
       <c r="D63" s="4" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="E63" s="4"/>
       <c r="F63" s="4"/>
@@ -3833,13 +3856,13 @@
     <row x14ac:dyDescent="0.25" r="64" customHeight="1" ht="33.75" customFormat="1" s="1">
       <c r="A64" s="13"/>
       <c r="B64" s="7" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
       <c r="C64" s="12" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="D64" s="4" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="E64" s="4"/>
       <c r="F64" s="4"/>
@@ -3867,11 +3890,11 @@
     <row x14ac:dyDescent="0.25" r="65" customHeight="1" ht="30" customFormat="1" s="1">
       <c r="A65" s="13"/>
       <c r="B65" s="14" t="s">
-        <v>127</v>
+        <v>129</v>
       </c>
       <c r="C65" s="10"/>
       <c r="D65" s="4" t="s">
-        <v>128</v>
+        <v>130</v>
       </c>
       <c r="E65" s="4"/>
       <c r="F65" s="4"/>
@@ -3899,11 +3922,11 @@
     <row x14ac:dyDescent="0.25" r="66" customHeight="1" ht="36.75" customFormat="1" s="1">
       <c r="A66" s="13"/>
       <c r="B66" s="14" t="s">
-        <v>129</v>
+        <v>131</v>
       </c>
       <c r="C66" s="10"/>
       <c r="D66" s="4" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="E66" s="4"/>
       <c r="F66" s="4"/>
@@ -3931,11 +3954,11 @@
     <row x14ac:dyDescent="0.25" r="67" customHeight="1" ht="36.75" customFormat="1" s="1">
       <c r="A67" s="13"/>
       <c r="B67" s="21" t="s">
-        <v>130</v>
+        <v>132</v>
       </c>
       <c r="C67" s="18"/>
       <c r="D67" s="4" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="E67" s="4"/>
       <c r="F67" s="4"/>
@@ -3963,13 +3986,13 @@
     <row x14ac:dyDescent="0.25" r="68" customHeight="1" ht="18.75" customFormat="1" s="1">
       <c r="A68" s="13"/>
       <c r="B68" s="7" t="s">
-        <v>131</v>
+        <v>133</v>
       </c>
       <c r="C68" s="12" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="D68" s="4" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="E68" s="4"/>
       <c r="F68" s="4"/>
@@ -3997,11 +4020,11 @@
     <row x14ac:dyDescent="0.25" r="69" customHeight="1" ht="18.75" customFormat="1" s="1">
       <c r="A69" s="13"/>
       <c r="B69" s="14" t="s">
-        <v>132</v>
+        <v>134</v>
       </c>
       <c r="C69" s="10"/>
       <c r="D69" s="4" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="E69" s="4"/>
       <c r="F69" s="4"/>
@@ -4029,11 +4052,11 @@
     <row x14ac:dyDescent="0.25" r="70" customHeight="1" ht="27" customFormat="1" s="1">
       <c r="A70" s="25"/>
       <c r="B70" s="21" t="s">
-        <v>133</v>
+        <v>135</v>
       </c>
       <c r="C70" s="18"/>
       <c r="D70" s="4" t="s">
-        <v>134</v>
+        <v>136</v>
       </c>
       <c r="E70" s="4"/>
       <c r="F70" s="4"/>
@@ -4060,16 +4083,16 @@
     </row>
     <row x14ac:dyDescent="0.25" r="71" customHeight="1" ht="43.5" customFormat="1" s="1">
       <c r="A71" s="7" t="s">
-        <v>135</v>
+        <v>137</v>
       </c>
       <c r="B71" s="7" t="s">
-        <v>136</v>
+        <v>138</v>
       </c>
       <c r="C71" s="12" t="s">
-        <v>137</v>
+        <v>139</v>
       </c>
       <c r="D71" s="4" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="E71" s="4"/>
       <c r="F71" s="4"/>
@@ -4096,14 +4119,14 @@
     </row>
     <row x14ac:dyDescent="0.25" r="72" customHeight="1" ht="45.75" customFormat="1" s="1">
       <c r="A72" s="20" t="s">
-        <v>138</v>
+        <v>140</v>
       </c>
       <c r="B72" s="14" t="s">
-        <v>139</v>
+        <v>141</v>
       </c>
       <c r="C72" s="10"/>
       <c r="D72" s="4" t="s">
-        <v>140</v>
+        <v>142</v>
       </c>
       <c r="E72" s="4"/>
       <c r="F72" s="4"/>
@@ -4131,11 +4154,11 @@
     <row x14ac:dyDescent="0.25" r="73" customHeight="1" ht="45.75" customFormat="1" s="1">
       <c r="A73" s="10"/>
       <c r="B73" s="14" t="s">
-        <v>141</v>
+        <v>143</v>
       </c>
       <c r="C73" s="10"/>
       <c r="D73" s="4" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="E73" s="4"/>
       <c r="F73" s="4"/>
@@ -4163,11 +4186,11 @@
     <row x14ac:dyDescent="0.25" r="74" customHeight="1" ht="39" customFormat="1" s="1">
       <c r="A74" s="11"/>
       <c r="B74" s="14" t="s">
-        <v>142</v>
+        <v>144</v>
       </c>
       <c r="C74" s="10"/>
       <c r="D74" s="4" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="E74" s="4"/>
       <c r="F74" s="4"/>
@@ -4195,11 +4218,11 @@
     <row x14ac:dyDescent="0.25" r="75" customHeight="1" ht="26.25" customFormat="1" s="1">
       <c r="A75" s="13"/>
       <c r="B75" s="27" t="s">
-        <v>143</v>
+        <v>145</v>
       </c>
       <c r="C75" s="10"/>
       <c r="D75" s="4" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="E75" s="4"/>
       <c r="F75" s="4"/>
@@ -4227,11 +4250,11 @@
     <row x14ac:dyDescent="0.25" r="76" customHeight="1" ht="62.25" customFormat="1" s="1">
       <c r="A76" s="13"/>
       <c r="B76" s="14" t="s">
-        <v>144</v>
+        <v>146</v>
       </c>
       <c r="C76" s="10"/>
       <c r="D76" s="4" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="E76" s="4"/>
       <c r="F76" s="4"/>
@@ -4259,11 +4282,11 @@
     <row x14ac:dyDescent="0.25" r="77" customHeight="1" ht="43.5" customFormat="1" s="1">
       <c r="A77" s="13"/>
       <c r="B77" s="14" t="s">
-        <v>145</v>
+        <v>147</v>
       </c>
       <c r="C77" s="10"/>
       <c r="D77" s="4" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="E77" s="4"/>
       <c r="F77" s="4"/>
@@ -4291,11 +4314,11 @@
     <row x14ac:dyDescent="0.25" r="78" customHeight="1" ht="42" customFormat="1" s="1">
       <c r="A78" s="13"/>
       <c r="B78" s="21" t="s">
-        <v>146</v>
+        <v>148</v>
       </c>
       <c r="C78" s="18"/>
       <c r="D78" s="4" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="E78" s="4"/>
       <c r="F78" s="4"/>
@@ -4323,13 +4346,13 @@
     <row x14ac:dyDescent="0.25" r="79" customHeight="1" ht="36.75" customFormat="1" s="1">
       <c r="A79" s="13"/>
       <c r="B79" s="7" t="s">
-        <v>147</v>
+        <v>149</v>
       </c>
       <c r="C79" s="12" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="D79" s="4" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="E79" s="4"/>
       <c r="F79" s="4"/>
@@ -4357,11 +4380,11 @@
     <row x14ac:dyDescent="0.25" r="80" customHeight="1" ht="62.25" customFormat="1" s="1">
       <c r="A80" s="13"/>
       <c r="B80" s="14" t="s">
-        <v>148</v>
+        <v>150</v>
       </c>
       <c r="C80" s="10"/>
       <c r="D80" s="4" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="E80" s="4"/>
       <c r="F80" s="4"/>
@@ -4389,11 +4412,11 @@
     <row x14ac:dyDescent="0.25" r="81" customHeight="1" ht="62.25" customFormat="1" s="1">
       <c r="A81" s="13"/>
       <c r="B81" s="14" t="s">
-        <v>149</v>
+        <v>151</v>
       </c>
       <c r="C81" s="10"/>
       <c r="D81" s="4" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="E81" s="4"/>
       <c r="F81" s="4"/>
@@ -4421,11 +4444,11 @@
     <row x14ac:dyDescent="0.25" r="82" customHeight="1" ht="62.25" customFormat="1" s="1">
       <c r="A82" s="13"/>
       <c r="B82" s="14" t="s">
-        <v>150</v>
+        <v>152</v>
       </c>
       <c r="C82" s="10"/>
       <c r="D82" s="4" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="E82" s="4"/>
       <c r="F82" s="4"/>
@@ -4453,11 +4476,11 @@
     <row x14ac:dyDescent="0.25" r="83" customHeight="1" ht="62.25" customFormat="1" s="1">
       <c r="A83" s="13"/>
       <c r="B83" s="14" t="s">
-        <v>151</v>
+        <v>153</v>
       </c>
       <c r="C83" s="10"/>
       <c r="D83" s="4" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="E83" s="4"/>
       <c r="F83" s="4"/>
@@ -4485,11 +4508,11 @@
     <row x14ac:dyDescent="0.25" r="84" customHeight="1" ht="62.25" customFormat="1" s="1">
       <c r="A84" s="13"/>
       <c r="B84" s="14" t="s">
-        <v>152</v>
+        <v>154</v>
       </c>
       <c r="C84" s="10"/>
       <c r="D84" s="4" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="E84" s="4"/>
       <c r="F84" s="4"/>
@@ -4517,11 +4540,11 @@
     <row x14ac:dyDescent="0.25" r="85" customHeight="1" ht="36" customFormat="1" s="1">
       <c r="A85" s="13"/>
       <c r="B85" s="14" t="s">
-        <v>153</v>
+        <v>155</v>
       </c>
       <c r="C85" s="10"/>
       <c r="D85" s="4" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="E85" s="4"/>
       <c r="F85" s="4"/>
@@ -4549,11 +4572,11 @@
     <row x14ac:dyDescent="0.25" r="86" customHeight="1" ht="36" customFormat="1" s="1">
       <c r="A86" s="13"/>
       <c r="B86" s="14" t="s">
-        <v>154</v>
+        <v>156</v>
       </c>
       <c r="C86" s="10"/>
       <c r="D86" s="4" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="E86" s="4"/>
       <c r="F86" s="4"/>
@@ -4581,11 +4604,11 @@
     <row x14ac:dyDescent="0.25" r="87" customHeight="1" ht="36" customFormat="1" s="1">
       <c r="A87" s="13"/>
       <c r="B87" s="14" t="s">
-        <v>155</v>
+        <v>157</v>
       </c>
       <c r="C87" s="10"/>
       <c r="D87" s="4" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="E87" s="4"/>
       <c r="F87" s="4"/>
@@ -4613,11 +4636,11 @@
     <row x14ac:dyDescent="0.25" r="88" customHeight="1" ht="50.25" customFormat="1" s="1">
       <c r="A88" s="13"/>
       <c r="B88" s="14" t="s">
-        <v>156</v>
+        <v>158</v>
       </c>
       <c r="C88" s="10"/>
       <c r="D88" s="4" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="E88" s="4"/>
       <c r="F88" s="4"/>
@@ -4645,11 +4668,11 @@
     <row x14ac:dyDescent="0.25" r="89" customHeight="1" ht="36" customFormat="1" s="1">
       <c r="A89" s="13"/>
       <c r="B89" s="14" t="s">
-        <v>157</v>
+        <v>159</v>
       </c>
       <c r="C89" s="10"/>
       <c r="D89" s="4" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="E89" s="4"/>
       <c r="F89" s="4"/>
@@ -4677,11 +4700,11 @@
     <row x14ac:dyDescent="0.25" r="90" customHeight="1" ht="36.75" customFormat="1" s="1">
       <c r="A90" s="13"/>
       <c r="B90" s="21" t="s">
-        <v>158</v>
+        <v>160</v>
       </c>
       <c r="C90" s="18"/>
       <c r="D90" s="4" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="E90" s="4"/>
       <c r="F90" s="4"/>
@@ -4709,13 +4732,13 @@
     <row x14ac:dyDescent="0.25" r="91" customHeight="1" ht="51" customFormat="1" s="1">
       <c r="A91" s="13"/>
       <c r="B91" s="22" t="s">
-        <v>159</v>
+        <v>161</v>
       </c>
       <c r="C91" s="12" t="s">
-        <v>160</v>
+        <v>162</v>
       </c>
       <c r="D91" s="4" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="E91" s="4"/>
       <c r="F91" s="4"/>
@@ -4743,11 +4766,11 @@
     <row x14ac:dyDescent="0.25" r="92" customHeight="1" ht="50.25" customFormat="1" s="1">
       <c r="A92" s="13"/>
       <c r="B92" s="23" t="s">
-        <v>161</v>
+        <v>163</v>
       </c>
       <c r="C92" s="10"/>
       <c r="D92" s="4" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="E92" s="4"/>
       <c r="F92" s="4"/>
@@ -4775,11 +4798,11 @@
     <row x14ac:dyDescent="0.25" r="93" customHeight="1" ht="36" customFormat="1" s="1">
       <c r="A93" s="13"/>
       <c r="B93" s="23" t="s">
-        <v>162</v>
+        <v>164</v>
       </c>
       <c r="C93" s="10"/>
       <c r="D93" s="4" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="E93" s="4"/>
       <c r="F93" s="4"/>
@@ -4807,11 +4830,11 @@
     <row x14ac:dyDescent="0.25" r="94" customHeight="1" ht="36" customFormat="1" s="1">
       <c r="A94" s="13"/>
       <c r="B94" s="23" t="s">
-        <v>163</v>
+        <v>165</v>
       </c>
       <c r="C94" s="10"/>
       <c r="D94" s="4" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="E94" s="4"/>
       <c r="F94" s="4"/>
@@ -4839,11 +4862,11 @@
     <row x14ac:dyDescent="0.25" r="95" customHeight="1" ht="36.75" customFormat="1" s="1">
       <c r="A95" s="25"/>
       <c r="B95" s="17" t="s">
-        <v>164</v>
+        <v>166</v>
       </c>
       <c r="C95" s="18"/>
       <c r="D95" s="4" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="E95" s="4"/>
       <c r="F95" s="4"/>
@@ -4870,16 +4893,16 @@
     </row>
     <row x14ac:dyDescent="0.25" r="96" customHeight="1" ht="64.5" customFormat="1" s="1">
       <c r="A96" s="7" t="s">
-        <v>165</v>
+        <v>167</v>
       </c>
       <c r="B96" s="7" t="s">
-        <v>166</v>
+        <v>168</v>
       </c>
       <c r="C96" s="12" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="D96" s="4" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="E96" s="4"/>
       <c r="F96" s="4"/>
@@ -4906,14 +4929,14 @@
     </row>
     <row x14ac:dyDescent="0.25" r="97" customHeight="1" ht="36" customFormat="1" s="1">
       <c r="A97" s="20" t="s">
-        <v>167</v>
+        <v>169</v>
       </c>
       <c r="B97" s="14" t="s">
-        <v>168</v>
+        <v>170</v>
       </c>
       <c r="C97" s="10"/>
       <c r="D97" s="4" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="E97" s="4"/>
       <c r="F97" s="4"/>
@@ -4941,11 +4964,11 @@
     <row x14ac:dyDescent="0.25" r="98" customHeight="1" ht="50.25" customFormat="1" s="1">
       <c r="A98" s="10"/>
       <c r="B98" s="14" t="s">
-        <v>169</v>
+        <v>171</v>
       </c>
       <c r="C98" s="10"/>
       <c r="D98" s="4" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="E98" s="4"/>
       <c r="F98" s="4"/>
@@ -4973,11 +4996,11 @@
     <row x14ac:dyDescent="0.25" r="99" customHeight="1" ht="72.75" customFormat="1" s="1">
       <c r="A99" s="11"/>
       <c r="B99" s="21" t="s">
-        <v>170</v>
+        <v>172</v>
       </c>
       <c r="C99" s="18"/>
       <c r="D99" s="4" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="E99" s="4"/>
       <c r="F99" s="4"/>
@@ -5005,13 +5028,13 @@
     <row x14ac:dyDescent="0.25" r="100" customHeight="1" ht="36" customFormat="1" s="1">
       <c r="A100" s="13"/>
       <c r="B100" s="7" t="s">
-        <v>171</v>
+        <v>173</v>
       </c>
       <c r="C100" s="12" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="D100" s="4" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="E100" s="4"/>
       <c r="F100" s="4"/>
@@ -5039,11 +5062,11 @@
     <row x14ac:dyDescent="0.25" r="101" customHeight="1" ht="50.25" customFormat="1" s="1">
       <c r="A101" s="13"/>
       <c r="B101" s="14" t="s">
-        <v>172</v>
+        <v>174</v>
       </c>
       <c r="C101" s="10"/>
       <c r="D101" s="4" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="E101" s="4"/>
       <c r="F101" s="4"/>
@@ -5071,11 +5094,11 @@
     <row x14ac:dyDescent="0.25" r="102" customHeight="1" ht="63" customFormat="1" s="1">
       <c r="A102" s="13"/>
       <c r="B102" s="21" t="s">
-        <v>173</v>
+        <v>175</v>
       </c>
       <c r="C102" s="18"/>
       <c r="D102" s="4" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="E102" s="4"/>
       <c r="F102" s="4"/>
@@ -5103,13 +5126,13 @@
     <row x14ac:dyDescent="0.25" r="103" customHeight="1" ht="36.75" customFormat="1" s="1">
       <c r="A103" s="13"/>
       <c r="B103" s="7" t="s">
-        <v>174</v>
+        <v>176</v>
       </c>
       <c r="C103" s="12" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="D103" s="4" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="E103" s="4"/>
       <c r="F103" s="4"/>
@@ -5137,11 +5160,11 @@
     <row x14ac:dyDescent="0.25" r="104" customHeight="1" ht="50.25" customFormat="1" s="1">
       <c r="A104" s="13"/>
       <c r="B104" s="14" t="s">
-        <v>175</v>
+        <v>177</v>
       </c>
       <c r="C104" s="10"/>
       <c r="D104" s="4" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="E104" s="4"/>
       <c r="F104" s="4"/>
@@ -5169,11 +5192,11 @@
     <row x14ac:dyDescent="0.25" r="105" customHeight="1" ht="36.75" customFormat="1" s="1">
       <c r="A105" s="13"/>
       <c r="B105" s="21" t="s">
-        <v>176</v>
+        <v>178</v>
       </c>
       <c r="C105" s="18"/>
       <c r="D105" s="4" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="E105" s="4"/>
       <c r="F105" s="4"/>
@@ -5201,13 +5224,13 @@
     <row x14ac:dyDescent="0.25" r="106" customHeight="1" ht="51" customFormat="1" s="1">
       <c r="A106" s="13"/>
       <c r="B106" s="7" t="s">
-        <v>177</v>
+        <v>179</v>
       </c>
       <c r="C106" s="12" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="D106" s="4" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="E106" s="4"/>
       <c r="F106" s="4"/>
@@ -5235,11 +5258,11 @@
     <row x14ac:dyDescent="0.25" r="107" customHeight="1" ht="36" customFormat="1" s="1">
       <c r="A107" s="13"/>
       <c r="B107" s="14" t="s">
-        <v>178</v>
+        <v>180</v>
       </c>
       <c r="C107" s="10"/>
       <c r="D107" s="4" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="E107" s="4"/>
       <c r="F107" s="4"/>
@@ -5267,11 +5290,11 @@
     <row x14ac:dyDescent="0.25" r="108" customHeight="1" ht="36" customFormat="1" s="1">
       <c r="A108" s="13"/>
       <c r="B108" s="14" t="s">
-        <v>179</v>
+        <v>181</v>
       </c>
       <c r="C108" s="10"/>
       <c r="D108" s="4" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="E108" s="4"/>
       <c r="F108" s="4"/>
@@ -5299,11 +5322,11 @@
     <row x14ac:dyDescent="0.25" r="109" customHeight="1" ht="21.75" customFormat="1" s="1">
       <c r="A109" s="13"/>
       <c r="B109" s="14" t="s">
-        <v>180</v>
+        <v>182</v>
       </c>
       <c r="C109" s="10"/>
       <c r="D109" s="4" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="E109" s="4"/>
       <c r="F109" s="4"/>
@@ -5331,11 +5354,11 @@
     <row x14ac:dyDescent="0.25" r="110" customHeight="1" ht="36" customFormat="1" s="1">
       <c r="A110" s="13"/>
       <c r="B110" s="14" t="s">
-        <v>181</v>
+        <v>183</v>
       </c>
       <c r="C110" s="10"/>
       <c r="D110" s="4" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="E110" s="4"/>
       <c r="F110" s="4"/>
@@ -5363,11 +5386,11 @@
     <row x14ac:dyDescent="0.25" r="111" customHeight="1" ht="36.75" customFormat="1" s="1">
       <c r="A111" s="13"/>
       <c r="B111" s="21" t="s">
-        <v>182</v>
+        <v>184</v>
       </c>
       <c r="C111" s="18"/>
       <c r="D111" s="4" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="E111" s="4"/>
       <c r="F111" s="4"/>
@@ -5395,13 +5418,13 @@
     <row x14ac:dyDescent="0.25" r="112" customHeight="1" ht="36.75" customFormat="1" s="1">
       <c r="A112" s="13"/>
       <c r="B112" s="7" t="s">
-        <v>183</v>
+        <v>185</v>
       </c>
       <c r="C112" s="12" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="D112" s="4" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="E112" s="4"/>
       <c r="F112" s="4"/>
@@ -5429,11 +5452,11 @@
     <row x14ac:dyDescent="0.25" r="113" customHeight="1" ht="36" customFormat="1" s="1">
       <c r="A113" s="13"/>
       <c r="B113" s="14" t="s">
-        <v>184</v>
+        <v>186</v>
       </c>
       <c r="C113" s="10"/>
       <c r="D113" s="4" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="E113" s="4"/>
       <c r="F113" s="4"/>
@@ -5461,11 +5484,11 @@
     <row x14ac:dyDescent="0.25" r="114" customHeight="1" ht="50.25" customFormat="1" s="1">
       <c r="A114" s="13"/>
       <c r="B114" s="14" t="s">
-        <v>185</v>
+        <v>187</v>
       </c>
       <c r="C114" s="10"/>
       <c r="D114" s="4" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="E114" s="4"/>
       <c r="F114" s="4"/>
@@ -5493,11 +5516,11 @@
     <row x14ac:dyDescent="0.25" r="115" customHeight="1" ht="36" customFormat="1" s="1">
       <c r="A115" s="13"/>
       <c r="B115" s="14" t="s">
-        <v>186</v>
+        <v>188</v>
       </c>
       <c r="C115" s="10"/>
       <c r="D115" s="4" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="E115" s="4"/>
       <c r="F115" s="4"/>
@@ -5525,11 +5548,11 @@
     <row x14ac:dyDescent="0.25" r="116" customHeight="1" ht="30.75" customFormat="1" s="1">
       <c r="A116" s="25"/>
       <c r="B116" s="21" t="s">
-        <v>187</v>
+        <v>189</v>
       </c>
       <c r="C116" s="18"/>
       <c r="D116" s="4" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="E116" s="4"/>
       <c r="F116" s="4"/>

</xml_diff>

<commit_message>
Ajout referntiel CNN, img/logos
</commit_message>
<xml_diff>
--- a/Referentiel_DFS.xlsx
+++ b/Referentiel_DFS.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="335" uniqueCount="193">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="338" uniqueCount="196">
   <si>
     <t>Tableau 1</t>
   </si>
@@ -572,6 +572,9 @@
     <t>C20 - Industrialiser le développement de la partie back-end de l’application ou du site web et automatiser les processus d’assurance qualité</t>
   </si>
   <si>
+    <t>git flow ?</t>
+  </si>
+  <si>
     <t>C20.1 - Mettre en oeuvre un processus d’intégration continue de manière à minimiser les erreurs humaines et de rationaliser le cycle de développement de la partie back-end de l’application.</t>
   </si>
   <si>
@@ -582,6 +585,9 @@
   </si>
   <si>
     <t>C20.3 - Automatiser la construction de l’application en configurant la chaînes de build, l’exécution des tests, l’exécution des outils d’assurance qualité et l’analyse statique de sécurité.</t>
+  </si>
+  <si>
+    <t>Test unitaires, sonarQube, TFS</t>
   </si>
   <si>
     <t>C21 - Faire évoluer ses connaissances et compétences en développement back-end</t>
@@ -684,6 +690,9 @@
     <t>C23.1 - Sécuriser les services et les réseaux d’une architecture d’hébergement</t>
   </si>
   <si>
+    <t>Privileges stagiaire pour arc, nouveau profil securise</t>
+  </si>
+  <si>
     <t>C23.2 - Mettre en oeuvre les liaisons sécurisées entre les différents services et les composants de l’application</t>
   </si>
   <si>
@@ -734,7 +743,15 @@
     <t>C24.4 - Rédiger la documentation d’une API afin de faciliter sa consommation par des tiers</t>
   </si>
   <si>
-    <t>style="font-family: Avenir Next Demi Bold;font-size: 15px;color: #00bfff;"&gt;A6 - Mettre en oeuvre des solutions techniques répondant aux besoins contextuels d’une application ou d’un site web (lois, normes et règlements, accessibilité, outils marketing et e-commerce) et piloter les performances.</t>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF00bfff"/>
+        <rFont val="Avenir Next Demi Bold"/>
+        <family val="2"/>
+      </rPr>
+      <t>style="font-family: Avenir Next Demi Bold;font-size: 15px;color: #00bfff;"&gt;A6 - Mettre en oeuvre des solutions techniques répondant aux besoins contextuels d’une application ou d’un site web (lois, normes et règlements, accessibilité, outils marketing et e-commerce) et piloter les performances.</t>
+    </r>
   </si>
   <si>
     <t>C25 - Mettre en oeuvre les outils et techniques permettant de respecter les aspects réglementaires au regard des données informatiques traitées et stockées</t>
@@ -1706,7 +1723,7 @@
       <c r="Y1" s="4"/>
       <c r="Z1" s="4"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="139.5" customFormat="1" s="1">
+    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="136.5" customFormat="1" s="1">
       <c r="A2" s="5" t="s">
         <v>2</v>
       </c>
@@ -1746,7 +1763,7 @@
       <c r="Y2" s="4"/>
       <c r="Z2" s="4"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="85.5" customFormat="1" s="1">
+    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="90.75" customFormat="1" s="1">
       <c r="A3" s="7" t="s">
         <v>8</v>
       </c>
@@ -1784,7 +1801,7 @@
       <c r="Y3" s="4"/>
       <c r="Z3" s="4"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="47.4375" customFormat="1" s="1">
+    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="46.125" customFormat="1" s="1">
       <c r="A4" s="9" t="s">
         <v>13</v>
       </c>
@@ -1822,7 +1839,7 @@
       <c r="Y4" s="4"/>
       <c r="Z4" s="4"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="96" customFormat="1" s="1">
+    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="102" customFormat="1" s="1">
       <c r="A5" s="10"/>
       <c r="B5" s="8" t="s">
         <v>17</v>
@@ -3873,7 +3890,9 @@
       <c r="D64" s="4" t="s">
         <v>81</v>
       </c>
-      <c r="E64" s="4"/>
+      <c r="E64" s="4" t="s">
+        <v>129</v>
+      </c>
       <c r="F64" s="4"/>
       <c r="G64" s="4"/>
       <c r="H64" s="4"/>
@@ -3896,14 +3915,14 @@
       <c r="Y64" s="4"/>
       <c r="Z64" s="4"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="65" customHeight="1" ht="30" customFormat="1" s="1">
+    <row x14ac:dyDescent="0.25" r="65" customHeight="1" ht="42.75" customFormat="1" s="1">
       <c r="A65" s="13"/>
       <c r="B65" s="14" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="C65" s="10"/>
       <c r="D65" s="4" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="E65" s="4"/>
       <c r="F65" s="4"/>
@@ -3931,7 +3950,7 @@
     <row x14ac:dyDescent="0.25" r="66" customHeight="1" ht="36.75" customFormat="1" s="1">
       <c r="A66" s="13"/>
       <c r="B66" s="14" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="C66" s="10"/>
       <c r="D66" s="4" t="s">
@@ -3963,13 +3982,15 @@
     <row x14ac:dyDescent="0.25" r="67" customHeight="1" ht="36.75" customFormat="1" s="1">
       <c r="A67" s="13"/>
       <c r="B67" s="21" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="C67" s="18"/>
       <c r="D67" s="4" t="s">
-        <v>81</v>
-      </c>
-      <c r="E67" s="4"/>
+        <v>11</v>
+      </c>
+      <c r="E67" s="4" t="s">
+        <v>134</v>
+      </c>
       <c r="F67" s="4"/>
       <c r="G67" s="4"/>
       <c r="H67" s="4"/>
@@ -3995,7 +4016,7 @@
     <row x14ac:dyDescent="0.25" r="68" customHeight="1" ht="18.75" customFormat="1" s="1">
       <c r="A68" s="13"/>
       <c r="B68" s="7" t="s">
-        <v>133</v>
+        <v>135</v>
       </c>
       <c r="C68" s="12" t="s">
         <v>15</v>
@@ -4004,7 +4025,7 @@
         <v>11</v>
       </c>
       <c r="E68" s="4" t="s">
-        <v>134</v>
+        <v>136</v>
       </c>
       <c r="F68" s="4"/>
       <c r="G68" s="4"/>
@@ -4031,14 +4052,14 @@
     <row x14ac:dyDescent="0.25" r="69" customHeight="1" ht="18.75" customFormat="1" s="1">
       <c r="A69" s="13"/>
       <c r="B69" s="14" t="s">
-        <v>135</v>
+        <v>137</v>
       </c>
       <c r="C69" s="10"/>
       <c r="D69" s="4" t="s">
         <v>11</v>
       </c>
       <c r="E69" s="4" t="s">
-        <v>136</v>
+        <v>138</v>
       </c>
       <c r="F69" s="4"/>
       <c r="G69" s="4"/>
@@ -4065,14 +4086,14 @@
     <row x14ac:dyDescent="0.25" r="70" customHeight="1" ht="27" customFormat="1" s="1">
       <c r="A70" s="25"/>
       <c r="B70" s="21" t="s">
-        <v>137</v>
+        <v>139</v>
       </c>
       <c r="C70" s="18"/>
       <c r="D70" s="4" t="s">
-        <v>138</v>
+        <v>140</v>
       </c>
       <c r="E70" s="4" t="s">
-        <v>139</v>
+        <v>141</v>
       </c>
       <c r="F70" s="4"/>
       <c r="G70" s="4"/>
@@ -4098,13 +4119,13 @@
     </row>
     <row x14ac:dyDescent="0.25" r="71" customHeight="1" ht="43.5" customFormat="1" s="1">
       <c r="A71" s="7" t="s">
-        <v>140</v>
+        <v>142</v>
       </c>
       <c r="B71" s="7" t="s">
-        <v>141</v>
+        <v>143</v>
       </c>
       <c r="C71" s="12" t="s">
-        <v>142</v>
+        <v>144</v>
       </c>
       <c r="D71" s="4" t="s">
         <v>81</v>
@@ -4134,14 +4155,14 @@
     </row>
     <row x14ac:dyDescent="0.25" r="72" customHeight="1" ht="45.75" customFormat="1" s="1">
       <c r="A72" s="20" t="s">
-        <v>143</v>
+        <v>145</v>
       </c>
       <c r="B72" s="14" t="s">
-        <v>144</v>
+        <v>146</v>
       </c>
       <c r="C72" s="10"/>
       <c r="D72" s="4" t="s">
-        <v>145</v>
+        <v>147</v>
       </c>
       <c r="E72" s="4"/>
       <c r="F72" s="4"/>
@@ -4169,7 +4190,7 @@
     <row x14ac:dyDescent="0.25" r="73" customHeight="1" ht="45.75" customFormat="1" s="1">
       <c r="A73" s="10"/>
       <c r="B73" s="14" t="s">
-        <v>146</v>
+        <v>148</v>
       </c>
       <c r="C73" s="10"/>
       <c r="D73" s="4" t="s">
@@ -4201,7 +4222,7 @@
     <row x14ac:dyDescent="0.25" r="74" customHeight="1" ht="39" customFormat="1" s="1">
       <c r="A74" s="11"/>
       <c r="B74" s="14" t="s">
-        <v>147</v>
+        <v>149</v>
       </c>
       <c r="C74" s="10"/>
       <c r="D74" s="4" t="s">
@@ -4233,7 +4254,7 @@
     <row x14ac:dyDescent="0.25" r="75" customHeight="1" ht="26.25" customFormat="1" s="1">
       <c r="A75" s="13"/>
       <c r="B75" s="27" t="s">
-        <v>148</v>
+        <v>150</v>
       </c>
       <c r="C75" s="10"/>
       <c r="D75" s="4" t="s">
@@ -4265,7 +4286,7 @@
     <row x14ac:dyDescent="0.25" r="76" customHeight="1" ht="62.25" customFormat="1" s="1">
       <c r="A76" s="13"/>
       <c r="B76" s="14" t="s">
-        <v>149</v>
+        <v>151</v>
       </c>
       <c r="C76" s="10"/>
       <c r="D76" s="4" t="s">
@@ -4297,7 +4318,7 @@
     <row x14ac:dyDescent="0.25" r="77" customHeight="1" ht="43.5" customFormat="1" s="1">
       <c r="A77" s="13"/>
       <c r="B77" s="14" t="s">
-        <v>150</v>
+        <v>152</v>
       </c>
       <c r="C77" s="10"/>
       <c r="D77" s="4" t="s">
@@ -4329,7 +4350,7 @@
     <row x14ac:dyDescent="0.25" r="78" customHeight="1" ht="42" customFormat="1" s="1">
       <c r="A78" s="13"/>
       <c r="B78" s="21" t="s">
-        <v>151</v>
+        <v>153</v>
       </c>
       <c r="C78" s="18"/>
       <c r="D78" s="4" t="s">
@@ -4361,7 +4382,7 @@
     <row x14ac:dyDescent="0.25" r="79" customHeight="1" ht="36.75" customFormat="1" s="1">
       <c r="A79" s="13"/>
       <c r="B79" s="7" t="s">
-        <v>152</v>
+        <v>154</v>
       </c>
       <c r="C79" s="12" t="s">
         <v>15</v>
@@ -4395,13 +4416,15 @@
     <row x14ac:dyDescent="0.25" r="80" customHeight="1" ht="62.25" customFormat="1" s="1">
       <c r="A80" s="13"/>
       <c r="B80" s="14" t="s">
-        <v>153</v>
+        <v>155</v>
       </c>
       <c r="C80" s="10"/>
       <c r="D80" s="4" t="s">
         <v>81</v>
       </c>
-      <c r="E80" s="4"/>
+      <c r="E80" s="4" t="s">
+        <v>156</v>
+      </c>
       <c r="F80" s="4"/>
       <c r="G80" s="4"/>
       <c r="H80" s="4"/>
@@ -4427,7 +4450,7 @@
     <row x14ac:dyDescent="0.25" r="81" customHeight="1" ht="62.25" customFormat="1" s="1">
       <c r="A81" s="13"/>
       <c r="B81" s="14" t="s">
-        <v>154</v>
+        <v>157</v>
       </c>
       <c r="C81" s="10"/>
       <c r="D81" s="4" t="s">
@@ -4459,7 +4482,7 @@
     <row x14ac:dyDescent="0.25" r="82" customHeight="1" ht="62.25" customFormat="1" s="1">
       <c r="A82" s="13"/>
       <c r="B82" s="14" t="s">
-        <v>155</v>
+        <v>158</v>
       </c>
       <c r="C82" s="10"/>
       <c r="D82" s="4" t="s">
@@ -4491,7 +4514,7 @@
     <row x14ac:dyDescent="0.25" r="83" customHeight="1" ht="62.25" customFormat="1" s="1">
       <c r="A83" s="13"/>
       <c r="B83" s="14" t="s">
-        <v>156</v>
+        <v>159</v>
       </c>
       <c r="C83" s="10"/>
       <c r="D83" s="4" t="s">
@@ -4523,7 +4546,7 @@
     <row x14ac:dyDescent="0.25" r="84" customHeight="1" ht="62.25" customFormat="1" s="1">
       <c r="A84" s="13"/>
       <c r="B84" s="14" t="s">
-        <v>157</v>
+        <v>160</v>
       </c>
       <c r="C84" s="10"/>
       <c r="D84" s="4" t="s">
@@ -4555,7 +4578,7 @@
     <row x14ac:dyDescent="0.25" r="85" customHeight="1" ht="36" customFormat="1" s="1">
       <c r="A85" s="13"/>
       <c r="B85" s="14" t="s">
-        <v>158</v>
+        <v>161</v>
       </c>
       <c r="C85" s="10"/>
       <c r="D85" s="4" t="s">
@@ -4587,7 +4610,7 @@
     <row x14ac:dyDescent="0.25" r="86" customHeight="1" ht="36" customFormat="1" s="1">
       <c r="A86" s="13"/>
       <c r="B86" s="14" t="s">
-        <v>159</v>
+        <v>162</v>
       </c>
       <c r="C86" s="10"/>
       <c r="D86" s="4" t="s">
@@ -4619,7 +4642,7 @@
     <row x14ac:dyDescent="0.25" r="87" customHeight="1" ht="36" customFormat="1" s="1">
       <c r="A87" s="13"/>
       <c r="B87" s="14" t="s">
-        <v>160</v>
+        <v>163</v>
       </c>
       <c r="C87" s="10"/>
       <c r="D87" s="4" t="s">
@@ -4651,7 +4674,7 @@
     <row x14ac:dyDescent="0.25" r="88" customHeight="1" ht="50.25" customFormat="1" s="1">
       <c r="A88" s="13"/>
       <c r="B88" s="14" t="s">
-        <v>161</v>
+        <v>164</v>
       </c>
       <c r="C88" s="10"/>
       <c r="D88" s="4" t="s">
@@ -4683,11 +4706,11 @@
     <row x14ac:dyDescent="0.25" r="89" customHeight="1" ht="36" customFormat="1" s="1">
       <c r="A89" s="13"/>
       <c r="B89" s="14" t="s">
-        <v>162</v>
+        <v>165</v>
       </c>
       <c r="C89" s="10"/>
       <c r="D89" s="4" t="s">
-        <v>81</v>
+        <v>11</v>
       </c>
       <c r="E89" s="4"/>
       <c r="F89" s="4"/>
@@ -4715,7 +4738,7 @@
     <row x14ac:dyDescent="0.25" r="90" customHeight="1" ht="36.75" customFormat="1" s="1">
       <c r="A90" s="13"/>
       <c r="B90" s="21" t="s">
-        <v>163</v>
+        <v>166</v>
       </c>
       <c r="C90" s="18"/>
       <c r="D90" s="4" t="s">
@@ -4747,10 +4770,10 @@
     <row x14ac:dyDescent="0.25" r="91" customHeight="1" ht="51" customFormat="1" s="1">
       <c r="A91" s="13"/>
       <c r="B91" s="22" t="s">
-        <v>164</v>
+        <v>167</v>
       </c>
       <c r="C91" s="12" t="s">
-        <v>165</v>
+        <v>168</v>
       </c>
       <c r="D91" s="4" t="s">
         <v>81</v>
@@ -4781,7 +4804,7 @@
     <row x14ac:dyDescent="0.25" r="92" customHeight="1" ht="50.25" customFormat="1" s="1">
       <c r="A92" s="13"/>
       <c r="B92" s="23" t="s">
-        <v>166</v>
+        <v>169</v>
       </c>
       <c r="C92" s="10"/>
       <c r="D92" s="4" t="s">
@@ -4813,7 +4836,7 @@
     <row x14ac:dyDescent="0.25" r="93" customHeight="1" ht="36" customFormat="1" s="1">
       <c r="A93" s="13"/>
       <c r="B93" s="23" t="s">
-        <v>167</v>
+        <v>170</v>
       </c>
       <c r="C93" s="10"/>
       <c r="D93" s="4" t="s">
@@ -4845,7 +4868,7 @@
     <row x14ac:dyDescent="0.25" r="94" customHeight="1" ht="36" customFormat="1" s="1">
       <c r="A94" s="13"/>
       <c r="B94" s="23" t="s">
-        <v>168</v>
+        <v>171</v>
       </c>
       <c r="C94" s="10"/>
       <c r="D94" s="4" t="s">
@@ -4877,7 +4900,7 @@
     <row x14ac:dyDescent="0.25" r="95" customHeight="1" ht="36.75" customFormat="1" s="1">
       <c r="A95" s="25"/>
       <c r="B95" s="17" t="s">
-        <v>169</v>
+        <v>172</v>
       </c>
       <c r="C95" s="18"/>
       <c r="D95" s="4" t="s">
@@ -4908,10 +4931,10 @@
     </row>
     <row x14ac:dyDescent="0.25" r="96" customHeight="1" ht="64.5" customFormat="1" s="1">
       <c r="A96" s="7" t="s">
-        <v>170</v>
+        <v>173</v>
       </c>
       <c r="B96" s="7" t="s">
-        <v>171</v>
+        <v>174</v>
       </c>
       <c r="C96" s="12" t="s">
         <v>15</v>
@@ -4944,10 +4967,10 @@
     </row>
     <row x14ac:dyDescent="0.25" r="97" customHeight="1" ht="36" customFormat="1" s="1">
       <c r="A97" s="20" t="s">
-        <v>172</v>
+        <v>175</v>
       </c>
       <c r="B97" s="14" t="s">
-        <v>173</v>
+        <v>176</v>
       </c>
       <c r="C97" s="10"/>
       <c r="D97" s="4" t="s">
@@ -4979,7 +5002,7 @@
     <row x14ac:dyDescent="0.25" r="98" customHeight="1" ht="50.25" customFormat="1" s="1">
       <c r="A98" s="10"/>
       <c r="B98" s="14" t="s">
-        <v>174</v>
+        <v>177</v>
       </c>
       <c r="C98" s="10"/>
       <c r="D98" s="4" t="s">
@@ -5011,7 +5034,7 @@
     <row x14ac:dyDescent="0.25" r="99" customHeight="1" ht="72.75" customFormat="1" s="1">
       <c r="A99" s="11"/>
       <c r="B99" s="21" t="s">
-        <v>175</v>
+        <v>178</v>
       </c>
       <c r="C99" s="18"/>
       <c r="D99" s="4" t="s">
@@ -5043,7 +5066,7 @@
     <row x14ac:dyDescent="0.25" r="100" customHeight="1" ht="36" customFormat="1" s="1">
       <c r="A100" s="13"/>
       <c r="B100" s="7" t="s">
-        <v>176</v>
+        <v>179</v>
       </c>
       <c r="C100" s="12" t="s">
         <v>15</v>
@@ -5077,7 +5100,7 @@
     <row x14ac:dyDescent="0.25" r="101" customHeight="1" ht="50.25" customFormat="1" s="1">
       <c r="A101" s="13"/>
       <c r="B101" s="14" t="s">
-        <v>177</v>
+        <v>180</v>
       </c>
       <c r="C101" s="10"/>
       <c r="D101" s="4" t="s">
@@ -5109,7 +5132,7 @@
     <row x14ac:dyDescent="0.25" r="102" customHeight="1" ht="63" customFormat="1" s="1">
       <c r="A102" s="13"/>
       <c r="B102" s="21" t="s">
-        <v>178</v>
+        <v>181</v>
       </c>
       <c r="C102" s="18"/>
       <c r="D102" s="4" t="s">
@@ -5141,7 +5164,7 @@
     <row x14ac:dyDescent="0.25" r="103" customHeight="1" ht="36.75" customFormat="1" s="1">
       <c r="A103" s="13"/>
       <c r="B103" s="7" t="s">
-        <v>179</v>
+        <v>182</v>
       </c>
       <c r="C103" s="12" t="s">
         <v>15</v>
@@ -5175,7 +5198,7 @@
     <row x14ac:dyDescent="0.25" r="104" customHeight="1" ht="50.25" customFormat="1" s="1">
       <c r="A104" s="13"/>
       <c r="B104" s="14" t="s">
-        <v>180</v>
+        <v>183</v>
       </c>
       <c r="C104" s="10"/>
       <c r="D104" s="4" t="s">
@@ -5207,7 +5230,7 @@
     <row x14ac:dyDescent="0.25" r="105" customHeight="1" ht="36.75" customFormat="1" s="1">
       <c r="A105" s="13"/>
       <c r="B105" s="21" t="s">
-        <v>181</v>
+        <v>184</v>
       </c>
       <c r="C105" s="18"/>
       <c r="D105" s="4" t="s">
@@ -5239,7 +5262,7 @@
     <row x14ac:dyDescent="0.25" r="106" customHeight="1" ht="51" customFormat="1" s="1">
       <c r="A106" s="13"/>
       <c r="B106" s="7" t="s">
-        <v>182</v>
+        <v>185</v>
       </c>
       <c r="C106" s="12" t="s">
         <v>15</v>
@@ -5273,7 +5296,7 @@
     <row x14ac:dyDescent="0.25" r="107" customHeight="1" ht="36" customFormat="1" s="1">
       <c r="A107" s="13"/>
       <c r="B107" s="14" t="s">
-        <v>183</v>
+        <v>186</v>
       </c>
       <c r="C107" s="10"/>
       <c r="D107" s="4" t="s">
@@ -5305,7 +5328,7 @@
     <row x14ac:dyDescent="0.25" r="108" customHeight="1" ht="36" customFormat="1" s="1">
       <c r="A108" s="13"/>
       <c r="B108" s="14" t="s">
-        <v>184</v>
+        <v>187</v>
       </c>
       <c r="C108" s="10"/>
       <c r="D108" s="4" t="s">
@@ -5337,7 +5360,7 @@
     <row x14ac:dyDescent="0.25" r="109" customHeight="1" ht="21.75" customFormat="1" s="1">
       <c r="A109" s="13"/>
       <c r="B109" s="14" t="s">
-        <v>185</v>
+        <v>188</v>
       </c>
       <c r="C109" s="10"/>
       <c r="D109" s="4" t="s">
@@ -5369,7 +5392,7 @@
     <row x14ac:dyDescent="0.25" r="110" customHeight="1" ht="36" customFormat="1" s="1">
       <c r="A110" s="13"/>
       <c r="B110" s="14" t="s">
-        <v>186</v>
+        <v>189</v>
       </c>
       <c r="C110" s="10"/>
       <c r="D110" s="4" t="s">
@@ -5401,7 +5424,7 @@
     <row x14ac:dyDescent="0.25" r="111" customHeight="1" ht="36.75" customFormat="1" s="1">
       <c r="A111" s="13"/>
       <c r="B111" s="21" t="s">
-        <v>187</v>
+        <v>190</v>
       </c>
       <c r="C111" s="18"/>
       <c r="D111" s="4" t="s">
@@ -5433,7 +5456,7 @@
     <row x14ac:dyDescent="0.25" r="112" customHeight="1" ht="36.75" customFormat="1" s="1">
       <c r="A112" s="13"/>
       <c r="B112" s="7" t="s">
-        <v>188</v>
+        <v>191</v>
       </c>
       <c r="C112" s="12" t="s">
         <v>15</v>
@@ -5467,7 +5490,7 @@
     <row x14ac:dyDescent="0.25" r="113" customHeight="1" ht="36" customFormat="1" s="1">
       <c r="A113" s="13"/>
       <c r="B113" s="14" t="s">
-        <v>189</v>
+        <v>192</v>
       </c>
       <c r="C113" s="10"/>
       <c r="D113" s="4" t="s">
@@ -5499,7 +5522,7 @@
     <row x14ac:dyDescent="0.25" r="114" customHeight="1" ht="50.25" customFormat="1" s="1">
       <c r="A114" s="13"/>
       <c r="B114" s="14" t="s">
-        <v>190</v>
+        <v>193</v>
       </c>
       <c r="C114" s="10"/>
       <c r="D114" s="4" t="s">
@@ -5531,7 +5554,7 @@
     <row x14ac:dyDescent="0.25" r="115" customHeight="1" ht="36" customFormat="1" s="1">
       <c r="A115" s="13"/>
       <c r="B115" s="14" t="s">
-        <v>191</v>
+        <v>194</v>
       </c>
       <c r="C115" s="10"/>
       <c r="D115" s="4" t="s">
@@ -5563,7 +5586,7 @@
     <row x14ac:dyDescent="0.25" r="116" customHeight="1" ht="30.75" customFormat="1" s="1">
       <c r="A116" s="25"/>
       <c r="B116" s="21" t="s">
-        <v>192</v>
+        <v>195</v>
       </c>
       <c r="C116" s="18"/>
       <c r="D116" s="4" t="s">

</xml_diff>

<commit_message>
Maj soutenance + ajout img header
</commit_message>
<xml_diff>
--- a/Referentiel_DFS.xlsx
+++ b/Referentiel_DFS.xlsx
@@ -743,6 +743,9 @@
     <t>C24.4 - Rédiger la documentation d’une API afin de faciliter sa consommation par des tiers</t>
   </si>
   <si>
+    <r>
+      <t/>
+    </r>
     <r>
       <rPr>
         <sz val="11"/>
@@ -3783,7 +3786,7 @@
       <c r="Y60" s="4"/>
       <c r="Z60" s="4"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="61" customHeight="1" ht="49.5" customFormat="1" s="1">
+    <row x14ac:dyDescent="0.25" r="61" customHeight="1" ht="62.25" customFormat="1" s="1">
       <c r="A61" s="13"/>
       <c r="B61" s="26" t="s">
         <v>123</v>
@@ -3879,7 +3882,7 @@
       <c r="Y63" s="4"/>
       <c r="Z63" s="4"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="64" customHeight="1" ht="33.75" customFormat="1" s="1">
+    <row x14ac:dyDescent="0.25" r="64" customHeight="1" ht="28.5" customFormat="1" s="1">
       <c r="A64" s="13"/>
       <c r="B64" s="7" t="s">
         <v>128</v>
@@ -3915,7 +3918,7 @@
       <c r="Y64" s="4"/>
       <c r="Z64" s="4"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="65" customHeight="1" ht="42.75" customFormat="1" s="1">
+    <row x14ac:dyDescent="0.25" r="65" customHeight="1" ht="39.75" customFormat="1" s="1">
       <c r="A65" s="13"/>
       <c r="B65" s="14" t="s">
         <v>130</v>
@@ -3947,7 +3950,7 @@
       <c r="Y65" s="4"/>
       <c r="Z65" s="4"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="66" customHeight="1" ht="36.75" customFormat="1" s="1">
+    <row x14ac:dyDescent="0.25" r="66" customHeight="1" ht="28.5" customFormat="1" s="1">
       <c r="A66" s="13"/>
       <c r="B66" s="14" t="s">
         <v>132</v>
@@ -3979,7 +3982,7 @@
       <c r="Y66" s="4"/>
       <c r="Z66" s="4"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="67" customHeight="1" ht="36.75" customFormat="1" s="1">
+    <row x14ac:dyDescent="0.25" r="67" customHeight="1" ht="40.5" customFormat="1" s="1">
       <c r="A67" s="13"/>
       <c r="B67" s="21" t="s">
         <v>133</v>
@@ -4083,7 +4086,7 @@
       <c r="Y69" s="4"/>
       <c r="Z69" s="4"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="70" customHeight="1" ht="27" customFormat="1" s="1">
+    <row x14ac:dyDescent="0.25" r="70" customHeight="1" ht="18.75" customFormat="1" s="1">
       <c r="A70" s="25"/>
       <c r="B70" s="21" t="s">
         <v>139</v>
@@ -4117,7 +4120,7 @@
       <c r="Y70" s="4"/>
       <c r="Z70" s="4"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="71" customHeight="1" ht="43.5" customFormat="1" s="1">
+    <row x14ac:dyDescent="0.25" r="71" customHeight="1" ht="45" customFormat="1" s="1">
       <c r="A71" s="7" t="s">
         <v>142</v>
       </c>
@@ -4153,7 +4156,7 @@
       <c r="Y71" s="4"/>
       <c r="Z71" s="4"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="72" customHeight="1" ht="45.75" customFormat="1" s="1">
+    <row x14ac:dyDescent="0.25" r="72" customHeight="1" ht="45" customFormat="1" s="1">
       <c r="A72" s="20" t="s">
         <v>145</v>
       </c>
@@ -4187,7 +4190,7 @@
       <c r="Y72" s="4"/>
       <c r="Z72" s="4"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="73" customHeight="1" ht="45.75" customFormat="1" s="1">
+    <row x14ac:dyDescent="0.25" r="73" customHeight="1" ht="45" customFormat="1" s="1">
       <c r="A73" s="10"/>
       <c r="B73" s="14" t="s">
         <v>148</v>

</xml_diff>

<commit_message>
grosse Maj img, soutenance
</commit_message>
<xml_diff>
--- a/Referentiel_DFS.xlsx
+++ b/Referentiel_DFS.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="338" uniqueCount="196">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="338" uniqueCount="202">
   <si>
     <t>Tableau 1</t>
   </si>
@@ -161,7 +161,7 @@
 par un membre de la famille (cadre non formel).</t>
   </si>
   <si>
-    <t>Fait</t>
+    <t>Fait p9</t>
   </si>
   <si>
     <t>Purpaws, Comprendre les besoins de l'ecole et mettre en place notre projet commun</t>
@@ -178,6 +178,9 @@
     <t>aucun</t>
   </si>
   <si>
+    <t>p15</t>
+  </si>
+  <si>
     <t>Cahier des charges fonctionnel dans canva</t>
   </si>
   <si>
@@ -192,6 +195,9 @@
   <si>
     <t>débutant.
 cadre personnel : utilisation de photoshop et/ou illustrator pour concevoir une maquette de site.</t>
+  </si>
+  <si>
+    <t>Fait p16</t>
   </si>
   <si>
     <t>Wireframes dans canva</t>
@@ -204,7 +210,7 @@
     <t>débutant.
 cadre personnel
 C5.1 : utilisation de github dans le cadre d'un tutoriel
-C5.2 : aucun
+C5.2 : aucun docker?
 C5.3 : notepad++, VSCode
 C5.4 : aucun</t>
   </si>
@@ -215,6 +221,9 @@
     <t>C5.1 - Mettre en oeuvre et maîtriser l’utilisation d’un système de gestion de code source distribué (SCM) permettant de conserver l’historique des développements, d’organiser la collaboration des développeurs et d’appliquer un workflow standard pour la revue de code et le suivi des bugs.</t>
   </si>
   <si>
+    <t>Fait</t>
+  </si>
+  <si>
     <t>Utilisation de Notion et github</t>
   </si>
   <si>
@@ -239,10 +248,16 @@
     <t xml:space="preserve">C6 - Comprendre le cycle de développement et mettre en oeuvre les principales méthodes de gestion de projet de développement afin de les appliquer au sein d’une équipe (XP, SCRUM, DSDM, ASD). </t>
   </si>
   <si>
+    <t>Fait p12</t>
+  </si>
+  <si>
     <t>Scrum master Yannis, et répartition des taches entre nous</t>
   </si>
   <si>
     <t>C7 - Rédiger des compte-rendu d’activité destinés aux membres d’une équipe de projet afin de permettre le suivi de l’avancement du projet et la traçabilité des réalisations techniques</t>
+  </si>
+  <si>
+    <t>Fait p15</t>
   </si>
   <si>
     <t>Ryan a fait les compte rendu sur notion</t>
@@ -263,6 +278,9 @@
   </si>
   <si>
     <t>C8 - Rédiger les spécifications techniques de besoin (STB) d’un projet d’application ou de site web à partir d’un cahier des charges afin de décrire de manière exhaustif les exigences à satisfaire en termes d’utilisation</t>
+  </si>
+  <si>
+    <t>Fait p18</t>
   </si>
   <si>
     <t>Vu avec julio</t>
@@ -1726,7 +1744,7 @@
       <c r="Y1" s="4"/>
       <c r="Z1" s="4"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="136.5" customFormat="1" s="1">
+    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="139.5" customFormat="1" s="1">
       <c r="A2" s="5" t="s">
         <v>2</v>
       </c>
@@ -1766,7 +1784,7 @@
       <c r="Y2" s="4"/>
       <c r="Z2" s="4"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="90.75" customFormat="1" s="1">
+    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="85.5" customFormat="1" s="1">
       <c r="A3" s="7" t="s">
         <v>8</v>
       </c>
@@ -1804,7 +1822,7 @@
       <c r="Y3" s="4"/>
       <c r="Z3" s="4"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="46.125" customFormat="1" s="1">
+    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="47.4375" customFormat="1" s="1">
       <c r="A4" s="9" t="s">
         <v>13</v>
       </c>
@@ -1815,10 +1833,10 @@
         <v>15</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>11</v>
+        <v>16</v>
       </c>
       <c r="E4" s="4" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="F4" s="4"/>
       <c r="G4" s="4"/>
@@ -1842,10 +1860,10 @@
       <c r="Y4" s="4"/>
       <c r="Z4" s="4"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="102" customFormat="1" s="1">
+    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="96" customFormat="1" s="1">
       <c r="A5" s="10"/>
       <c r="B5" s="8" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C5" s="8" t="s">
         <v>15</v>
@@ -1854,7 +1872,7 @@
         <v>11</v>
       </c>
       <c r="E5" s="4" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="F5" s="4"/>
       <c r="G5" s="4"/>
@@ -1881,16 +1899,16 @@
     <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="63" customFormat="1" s="1">
       <c r="A6" s="10"/>
       <c r="B6" s="8" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C6" s="8" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>11</v>
+        <v>22</v>
       </c>
       <c r="E6" s="4" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="F6" s="4"/>
       <c r="G6" s="4"/>
@@ -1917,16 +1935,16 @@
     <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="39.75" customFormat="1" s="1">
       <c r="A7" s="11"/>
       <c r="B7" s="7" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="C7" s="12" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="D7" s="4" t="s">
         <v>11</v>
       </c>
       <c r="E7" s="4" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="F7" s="4"/>
       <c r="G7" s="4"/>
@@ -1953,14 +1971,14 @@
     <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="51" customFormat="1" s="1">
       <c r="A8" s="13"/>
       <c r="B8" s="14" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="C8" s="10"/>
       <c r="D8" s="4" t="s">
-        <v>11</v>
+        <v>28</v>
       </c>
       <c r="E8" s="4" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="F8" s="4"/>
       <c r="G8" s="4"/>
@@ -1987,14 +2005,14 @@
     <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="44.25" customFormat="1" s="1">
       <c r="A9" s="13"/>
       <c r="B9" s="14" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="C9" s="10"/>
       <c r="D9" s="4" t="s">
-        <v>11</v>
+        <v>28</v>
       </c>
       <c r="E9" s="4" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="F9" s="4"/>
       <c r="G9" s="4"/>
@@ -2021,14 +2039,14 @@
     <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="36" customFormat="1" s="1">
       <c r="A10" s="13"/>
       <c r="B10" s="15" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="C10" s="10"/>
       <c r="D10" s="4" t="s">
-        <v>11</v>
+        <v>28</v>
       </c>
       <c r="E10" s="4" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="F10" s="4"/>
       <c r="G10" s="4"/>
@@ -2055,14 +2073,14 @@
     <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="31.5" customFormat="1" s="1">
       <c r="A11" s="16"/>
       <c r="B11" s="17" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="C11" s="18"/>
       <c r="D11" s="4" t="s">
-        <v>11</v>
+        <v>28</v>
       </c>
       <c r="E11" s="4" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="F11" s="4"/>
       <c r="G11" s="4"/>
@@ -2089,16 +2107,16 @@
     <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="42" customFormat="1" s="1">
       <c r="A12" s="19"/>
       <c r="B12" s="8" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="C12" s="8" t="s">
         <v>15</v>
       </c>
       <c r="D12" s="4" t="s">
-        <v>11</v>
+        <v>37</v>
       </c>
       <c r="E12" s="4" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="F12" s="4"/>
       <c r="G12" s="4"/>
@@ -2125,16 +2143,16 @@
     <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="33.75" customFormat="1" s="1">
       <c r="A13" s="17"/>
       <c r="B13" s="8" t="s">
-        <v>35</v>
+        <v>39</v>
       </c>
       <c r="C13" s="8" t="s">
         <v>15</v>
       </c>
       <c r="D13" s="4" t="s">
-        <v>11</v>
+        <v>40</v>
       </c>
       <c r="E13" s="4" t="s">
-        <v>36</v>
+        <v>41</v>
       </c>
       <c r="F13" s="4"/>
       <c r="G13" s="4"/>
@@ -2160,19 +2178,19 @@
     </row>
     <row x14ac:dyDescent="0.25" r="14" customHeight="1" ht="45" customFormat="1" s="1">
       <c r="A14" s="7" t="s">
-        <v>37</v>
+        <v>42</v>
       </c>
       <c r="B14" s="8" t="s">
-        <v>38</v>
+        <v>43</v>
       </c>
       <c r="C14" s="8" t="s">
         <v>15</v>
       </c>
       <c r="D14" s="4" t="s">
-        <v>11</v>
+        <v>44</v>
       </c>
       <c r="E14" s="4" t="s">
-        <v>39</v>
+        <v>45</v>
       </c>
       <c r="F14" s="4"/>
       <c r="G14" s="4"/>
@@ -2198,19 +2216,19 @@
     </row>
     <row x14ac:dyDescent="0.25" r="15" customHeight="1" ht="36.75" customFormat="1" s="1">
       <c r="A15" s="20" t="s">
-        <v>40</v>
+        <v>46</v>
       </c>
       <c r="B15" s="7" t="s">
-        <v>41</v>
+        <v>47</v>
       </c>
       <c r="C15" s="12" t="s">
-        <v>42</v>
+        <v>48</v>
       </c>
       <c r="D15" s="4" t="s">
-        <v>11</v>
+        <v>44</v>
       </c>
       <c r="E15" s="4" t="s">
-        <v>43</v>
+        <v>49</v>
       </c>
       <c r="F15" s="4"/>
       <c r="G15" s="4"/>
@@ -2237,14 +2255,14 @@
     <row x14ac:dyDescent="0.25" r="16" customHeight="1" ht="36" customFormat="1" s="1">
       <c r="A16" s="10"/>
       <c r="B16" s="14" t="s">
-        <v>44</v>
+        <v>50</v>
       </c>
       <c r="C16" s="10"/>
       <c r="D16" s="4" t="s">
-        <v>11</v>
+        <v>28</v>
       </c>
       <c r="E16" s="4" t="s">
-        <v>45</v>
+        <v>51</v>
       </c>
       <c r="F16" s="4"/>
       <c r="G16" s="4"/>
@@ -2271,14 +2289,14 @@
     <row x14ac:dyDescent="0.25" r="17" customHeight="1" ht="42.75" customFormat="1" s="1">
       <c r="A17" s="11"/>
       <c r="B17" s="14" t="s">
-        <v>46</v>
+        <v>52</v>
       </c>
       <c r="C17" s="10"/>
       <c r="D17" s="4" t="s">
-        <v>11</v>
+        <v>28</v>
       </c>
       <c r="E17" s="4" t="s">
-        <v>45</v>
+        <v>51</v>
       </c>
       <c r="F17" s="4"/>
       <c r="G17" s="4"/>
@@ -2305,14 +2323,14 @@
     <row x14ac:dyDescent="0.25" r="18" customHeight="1" ht="36.75" customFormat="1" s="1">
       <c r="A18" s="13"/>
       <c r="B18" s="21" t="s">
-        <v>47</v>
+        <v>53</v>
       </c>
       <c r="C18" s="18"/>
       <c r="D18" s="4" t="s">
-        <v>11</v>
+        <v>28</v>
       </c>
       <c r="E18" s="4" t="s">
-        <v>48</v>
+        <v>54</v>
       </c>
       <c r="F18" s="4"/>
       <c r="G18" s="4"/>
@@ -2339,16 +2357,16 @@
     <row x14ac:dyDescent="0.25" r="19" customHeight="1" ht="51" customFormat="1" s="1">
       <c r="A19" s="13"/>
       <c r="B19" s="22" t="s">
-        <v>49</v>
+        <v>55</v>
       </c>
       <c r="C19" s="12" t="s">
-        <v>50</v>
+        <v>56</v>
       </c>
       <c r="D19" s="4" t="s">
-        <v>11</v>
+        <v>28</v>
       </c>
       <c r="E19" s="4" t="s">
-        <v>51</v>
+        <v>57</v>
       </c>
       <c r="F19" s="4"/>
       <c r="G19" s="4"/>
@@ -2375,14 +2393,14 @@
     <row x14ac:dyDescent="0.25" r="20" customHeight="1" ht="36" customFormat="1" s="1">
       <c r="A20" s="13"/>
       <c r="B20" s="23" t="s">
-        <v>52</v>
+        <v>58</v>
       </c>
       <c r="C20" s="10"/>
       <c r="D20" s="4" t="s">
-        <v>11</v>
+        <v>28</v>
       </c>
       <c r="E20" s="4" t="s">
-        <v>53</v>
+        <v>59</v>
       </c>
       <c r="F20" s="4"/>
       <c r="G20" s="4"/>
@@ -2409,14 +2427,14 @@
     <row x14ac:dyDescent="0.25" r="21" customHeight="1" ht="50.25" customFormat="1" s="1">
       <c r="A21" s="13"/>
       <c r="B21" s="23" t="s">
-        <v>54</v>
+        <v>60</v>
       </c>
       <c r="C21" s="10"/>
       <c r="D21" s="4" t="s">
-        <v>11</v>
+        <v>28</v>
       </c>
       <c r="E21" s="4" t="s">
-        <v>55</v>
+        <v>61</v>
       </c>
       <c r="F21" s="4"/>
       <c r="G21" s="4"/>
@@ -2443,14 +2461,14 @@
     <row x14ac:dyDescent="0.25" r="22" customHeight="1" ht="51" customFormat="1" s="1">
       <c r="A22" s="13"/>
       <c r="B22" s="24" t="s">
-        <v>56</v>
+        <v>62</v>
       </c>
       <c r="C22" s="18"/>
       <c r="D22" s="4" t="s">
-        <v>11</v>
+        <v>28</v>
       </c>
       <c r="E22" s="4" t="s">
-        <v>57</v>
+        <v>63</v>
       </c>
       <c r="F22" s="4"/>
       <c r="G22" s="4"/>
@@ -2477,16 +2495,16 @@
     <row x14ac:dyDescent="0.25" r="23" customHeight="1" ht="37.5" customFormat="1" s="1">
       <c r="A23" s="25"/>
       <c r="B23" s="8" t="s">
-        <v>58</v>
+        <v>64</v>
       </c>
       <c r="C23" s="8" t="s">
         <v>15</v>
       </c>
       <c r="D23" s="4" t="s">
-        <v>11</v>
+        <v>28</v>
       </c>
       <c r="E23" s="4" t="s">
-        <v>59</v>
+        <v>65</v>
       </c>
       <c r="F23" s="4"/>
       <c r="G23" s="4"/>
@@ -2512,19 +2530,19 @@
     </row>
     <row x14ac:dyDescent="0.25" r="24" customHeight="1" ht="57" customFormat="1" s="1">
       <c r="A24" s="7" t="s">
-        <v>60</v>
+        <v>66</v>
       </c>
       <c r="B24" s="7" t="s">
-        <v>61</v>
+        <v>67</v>
       </c>
       <c r="C24" s="12" t="s">
-        <v>62</v>
+        <v>68</v>
       </c>
       <c r="D24" s="4" t="s">
-        <v>11</v>
+        <v>28</v>
       </c>
       <c r="E24" s="4" t="s">
-        <v>63</v>
+        <v>69</v>
       </c>
       <c r="F24" s="4"/>
       <c r="G24" s="4"/>
@@ -2550,17 +2568,17 @@
     </row>
     <row x14ac:dyDescent="0.25" r="25" customHeight="1" ht="36" customFormat="1" s="1">
       <c r="A25" s="20" t="s">
-        <v>64</v>
+        <v>70</v>
       </c>
       <c r="B25" s="14" t="s">
-        <v>65</v>
+        <v>71</v>
       </c>
       <c r="C25" s="10"/>
       <c r="D25" s="4" t="s">
-        <v>11</v>
+        <v>28</v>
       </c>
       <c r="E25" s="4" t="s">
-        <v>66</v>
+        <v>72</v>
       </c>
       <c r="F25" s="4"/>
       <c r="G25" s="4"/>
@@ -2587,14 +2605,14 @@
     <row x14ac:dyDescent="0.25" r="26" customHeight="1" ht="50.25" customFormat="1" s="1">
       <c r="A26" s="10"/>
       <c r="B26" s="14" t="s">
-        <v>67</v>
+        <v>73</v>
       </c>
       <c r="C26" s="10"/>
       <c r="D26" s="4" t="s">
-        <v>11</v>
+        <v>28</v>
       </c>
       <c r="E26" s="4" t="s">
-        <v>66</v>
+        <v>72</v>
       </c>
       <c r="F26" s="4"/>
       <c r="G26" s="4"/>
@@ -2621,14 +2639,14 @@
     <row x14ac:dyDescent="0.25" r="27" customHeight="1" ht="35.75" customFormat="1" s="1">
       <c r="A27" s="11"/>
       <c r="B27" s="14" t="s">
-        <v>68</v>
+        <v>74</v>
       </c>
       <c r="C27" s="10"/>
       <c r="D27" s="4" t="s">
-        <v>11</v>
+        <v>28</v>
       </c>
       <c r="E27" s="4" t="s">
-        <v>69</v>
+        <v>75</v>
       </c>
       <c r="F27" s="4"/>
       <c r="G27" s="4"/>
@@ -2655,14 +2673,14 @@
     <row x14ac:dyDescent="0.25" r="28" customHeight="1" ht="28.5" customFormat="1" s="1">
       <c r="A28" s="13"/>
       <c r="B28" s="14" t="s">
-        <v>70</v>
+        <v>76</v>
       </c>
       <c r="C28" s="10"/>
       <c r="D28" s="4" t="s">
-        <v>11</v>
+        <v>28</v>
       </c>
       <c r="E28" s="4" t="s">
-        <v>71</v>
+        <v>77</v>
       </c>
       <c r="F28" s="4"/>
       <c r="G28" s="4"/>
@@ -2689,14 +2707,14 @@
     <row x14ac:dyDescent="0.25" r="29" customHeight="1" ht="39.75" customFormat="1" s="1">
       <c r="A29" s="13"/>
       <c r="B29" s="14" t="s">
-        <v>72</v>
+        <v>78</v>
       </c>
       <c r="C29" s="10"/>
       <c r="D29" s="4" t="s">
-        <v>11</v>
+        <v>28</v>
       </c>
       <c r="E29" s="4" t="s">
-        <v>66</v>
+        <v>72</v>
       </c>
       <c r="F29" s="4"/>
       <c r="G29" s="4"/>
@@ -2723,14 +2741,14 @@
     <row x14ac:dyDescent="0.25" r="30" customHeight="1" ht="18.75" customFormat="1" s="1">
       <c r="A30" s="13"/>
       <c r="B30" s="14" t="s">
-        <v>73</v>
+        <v>79</v>
       </c>
       <c r="C30" s="10"/>
       <c r="D30" s="4" t="s">
-        <v>11</v>
+        <v>28</v>
       </c>
       <c r="E30" s="4" t="s">
-        <v>66</v>
+        <v>72</v>
       </c>
       <c r="F30" s="4"/>
       <c r="G30" s="4"/>
@@ -2757,14 +2775,14 @@
     <row x14ac:dyDescent="0.25" r="31" customHeight="1" ht="28.5" customFormat="1" s="1">
       <c r="A31" s="13"/>
       <c r="B31" s="14" t="s">
-        <v>74</v>
+        <v>80</v>
       </c>
       <c r="C31" s="10"/>
       <c r="D31" s="4" t="s">
-        <v>11</v>
+        <v>28</v>
       </c>
       <c r="E31" s="4" t="s">
-        <v>75</v>
+        <v>81</v>
       </c>
       <c r="F31" s="4"/>
       <c r="G31" s="4"/>
@@ -2791,14 +2809,14 @@
     <row x14ac:dyDescent="0.25" r="32" customHeight="1" ht="29.25" customFormat="1" s="1">
       <c r="A32" s="13"/>
       <c r="B32" s="21" t="s">
-        <v>76</v>
+        <v>82</v>
       </c>
       <c r="C32" s="18"/>
       <c r="D32" s="4" t="s">
-        <v>11</v>
+        <v>28</v>
       </c>
       <c r="E32" s="4" t="s">
-        <v>66</v>
+        <v>72</v>
       </c>
       <c r="F32" s="4"/>
       <c r="G32" s="4"/>
@@ -2825,16 +2843,16 @@
     <row x14ac:dyDescent="0.25" r="33" customHeight="1" ht="39.75" customFormat="1" s="1">
       <c r="A33" s="13"/>
       <c r="B33" s="7" t="s">
-        <v>77</v>
+        <v>83</v>
       </c>
       <c r="C33" s="12" t="s">
-        <v>78</v>
+        <v>84</v>
       </c>
       <c r="D33" s="4" t="s">
-        <v>11</v>
+        <v>28</v>
       </c>
       <c r="E33" s="4" t="s">
-        <v>79</v>
+        <v>85</v>
       </c>
       <c r="F33" s="4"/>
       <c r="G33" s="4"/>
@@ -2861,11 +2879,11 @@
     <row x14ac:dyDescent="0.25" r="34" customHeight="1" ht="51" customFormat="1" s="1">
       <c r="A34" s="13"/>
       <c r="B34" s="14" t="s">
-        <v>80</v>
+        <v>86</v>
       </c>
       <c r="C34" s="10"/>
       <c r="D34" s="4" t="s">
-        <v>81</v>
+        <v>87</v>
       </c>
       <c r="E34" s="4"/>
       <c r="F34" s="4"/>
@@ -2893,11 +2911,11 @@
     <row x14ac:dyDescent="0.25" r="35" customHeight="1" ht="51" customFormat="1" s="1">
       <c r="A35" s="13"/>
       <c r="B35" s="14" t="s">
-        <v>82</v>
+        <v>88</v>
       </c>
       <c r="C35" s="10"/>
       <c r="D35" s="4" t="s">
-        <v>81</v>
+        <v>87</v>
       </c>
       <c r="E35" s="4"/>
       <c r="F35" s="4"/>
@@ -2925,14 +2943,14 @@
     <row x14ac:dyDescent="0.25" r="36" customHeight="1" ht="18.75" customFormat="1" s="1">
       <c r="A36" s="13"/>
       <c r="B36" s="14" t="s">
-        <v>83</v>
+        <v>89</v>
       </c>
       <c r="C36" s="10"/>
       <c r="D36" s="4" t="s">
-        <v>11</v>
+        <v>28</v>
       </c>
       <c r="E36" s="4" t="s">
-        <v>84</v>
+        <v>90</v>
       </c>
       <c r="F36" s="4"/>
       <c r="G36" s="4"/>
@@ -2959,14 +2977,14 @@
     <row x14ac:dyDescent="0.25" r="37" customHeight="1" ht="29.25" customFormat="1" s="1">
       <c r="A37" s="13"/>
       <c r="B37" s="21" t="s">
-        <v>85</v>
+        <v>91</v>
       </c>
       <c r="C37" s="18"/>
       <c r="D37" s="4" t="s">
-        <v>11</v>
+        <v>28</v>
       </c>
       <c r="E37" s="4" t="s">
-        <v>86</v>
+        <v>92</v>
       </c>
       <c r="F37" s="4"/>
       <c r="G37" s="4"/>
@@ -2993,16 +3011,16 @@
     <row x14ac:dyDescent="0.25" r="38" customHeight="1" ht="28.5" customFormat="1" s="1">
       <c r="A38" s="13"/>
       <c r="B38" s="7" t="s">
-        <v>87</v>
+        <v>93</v>
       </c>
       <c r="C38" s="12" t="s">
-        <v>88</v>
+        <v>94</v>
       </c>
       <c r="D38" s="4" t="s">
-        <v>11</v>
+        <v>28</v>
       </c>
       <c r="E38" s="4" t="s">
-        <v>86</v>
+        <v>92</v>
       </c>
       <c r="F38" s="4"/>
       <c r="G38" s="4"/>
@@ -3029,14 +3047,14 @@
     <row x14ac:dyDescent="0.25" r="39" customHeight="1" ht="28.5" customFormat="1" s="1">
       <c r="A39" s="13"/>
       <c r="B39" s="14" t="s">
-        <v>89</v>
+        <v>95</v>
       </c>
       <c r="C39" s="10"/>
       <c r="D39" s="4" t="s">
-        <v>11</v>
+        <v>28</v>
       </c>
       <c r="E39" s="4" t="s">
-        <v>90</v>
+        <v>96</v>
       </c>
       <c r="F39" s="4"/>
       <c r="G39" s="4"/>
@@ -3063,14 +3081,14 @@
     <row x14ac:dyDescent="0.25" r="40" customHeight="1" ht="28.5" customFormat="1" s="1">
       <c r="A40" s="13"/>
       <c r="B40" s="14" t="s">
-        <v>91</v>
+        <v>97</v>
       </c>
       <c r="C40" s="10"/>
       <c r="D40" s="4" t="s">
-        <v>92</v>
+        <v>98</v>
       </c>
       <c r="E40" s="4" t="s">
-        <v>93</v>
+        <v>99</v>
       </c>
       <c r="F40" s="4"/>
       <c r="G40" s="4"/>
@@ -3097,14 +3115,14 @@
     <row x14ac:dyDescent="0.25" r="41" customHeight="1" ht="40.5" customFormat="1" s="1">
       <c r="A41" s="25"/>
       <c r="B41" s="21" t="s">
-        <v>94</v>
+        <v>100</v>
       </c>
       <c r="C41" s="18"/>
       <c r="D41" s="4" t="s">
-        <v>95</v>
+        <v>101</v>
       </c>
       <c r="E41" s="4" t="s">
-        <v>96</v>
+        <v>102</v>
       </c>
       <c r="F41" s="4"/>
       <c r="G41" s="4"/>
@@ -3130,19 +3148,19 @@
     </row>
     <row x14ac:dyDescent="0.25" r="42" customHeight="1" ht="51" customFormat="1" s="1">
       <c r="A42" s="7" t="s">
-        <v>97</v>
+        <v>103</v>
       </c>
       <c r="B42" s="7" t="s">
-        <v>98</v>
+        <v>104</v>
       </c>
       <c r="C42" s="12" t="s">
-        <v>99</v>
+        <v>105</v>
       </c>
       <c r="D42" s="4" t="s">
-        <v>100</v>
+        <v>106</v>
       </c>
       <c r="E42" s="4" t="s">
-        <v>101</v>
+        <v>107</v>
       </c>
       <c r="F42" s="4"/>
       <c r="G42" s="4"/>
@@ -3168,17 +3186,17 @@
     </row>
     <row x14ac:dyDescent="0.25" r="43" customHeight="1" ht="27.75" customFormat="1" s="1">
       <c r="A43" s="20" t="s">
-        <v>102</v>
+        <v>108</v>
       </c>
       <c r="B43" s="14" t="s">
-        <v>103</v>
+        <v>109</v>
       </c>
       <c r="C43" s="10"/>
       <c r="D43" s="4" t="s">
-        <v>11</v>
+        <v>28</v>
       </c>
       <c r="E43" s="4" t="s">
-        <v>93</v>
+        <v>99</v>
       </c>
       <c r="F43" s="4"/>
       <c r="G43" s="4"/>
@@ -3205,14 +3223,14 @@
     <row x14ac:dyDescent="0.25" r="44" customHeight="1" ht="27.75" customFormat="1" s="1">
       <c r="A44" s="10"/>
       <c r="B44" s="14" t="s">
-        <v>104</v>
+        <v>110</v>
       </c>
       <c r="C44" s="10"/>
       <c r="D44" s="4" t="s">
-        <v>11</v>
+        <v>28</v>
       </c>
       <c r="E44" s="4" t="s">
-        <v>93</v>
+        <v>99</v>
       </c>
       <c r="F44" s="4"/>
       <c r="G44" s="4"/>
@@ -3239,14 +3257,14 @@
     <row x14ac:dyDescent="0.25" r="45" customHeight="1" ht="27.75" customFormat="1" s="1">
       <c r="A45" s="10"/>
       <c r="B45" s="14" t="s">
-        <v>105</v>
+        <v>111</v>
       </c>
       <c r="C45" s="10"/>
       <c r="D45" s="4" t="s">
-        <v>11</v>
+        <v>28</v>
       </c>
       <c r="E45" s="4" t="s">
-        <v>93</v>
+        <v>99</v>
       </c>
       <c r="F45" s="4"/>
       <c r="G45" s="4"/>
@@ -3273,14 +3291,14 @@
     <row x14ac:dyDescent="0.25" r="46" customHeight="1" ht="66" customFormat="1" s="1">
       <c r="A46" s="11"/>
       <c r="B46" s="14" t="s">
-        <v>106</v>
+        <v>112</v>
       </c>
       <c r="C46" s="10"/>
       <c r="D46" s="4" t="s">
-        <v>11</v>
+        <v>28</v>
       </c>
       <c r="E46" s="4" t="s">
-        <v>93</v>
+        <v>99</v>
       </c>
       <c r="F46" s="4"/>
       <c r="G46" s="4"/>
@@ -3307,14 +3325,14 @@
     <row x14ac:dyDescent="0.25" r="47" customHeight="1" ht="30.75" customFormat="1" s="1">
       <c r="A47" s="13"/>
       <c r="B47" s="21" t="s">
-        <v>107</v>
+        <v>113</v>
       </c>
       <c r="C47" s="18"/>
       <c r="D47" s="4" t="s">
-        <v>11</v>
+        <v>28</v>
       </c>
       <c r="E47" s="4" t="s">
-        <v>93</v>
+        <v>99</v>
       </c>
       <c r="F47" s="4"/>
       <c r="G47" s="4"/>
@@ -3341,16 +3359,16 @@
     <row x14ac:dyDescent="0.25" r="48" customHeight="1" ht="42.75" customFormat="1" s="1">
       <c r="A48" s="13"/>
       <c r="B48" s="7" t="s">
-        <v>108</v>
+        <v>114</v>
       </c>
       <c r="C48" s="12" t="s">
         <v>15</v>
       </c>
       <c r="D48" s="4" t="s">
-        <v>11</v>
+        <v>28</v>
       </c>
       <c r="E48" s="4" t="s">
-        <v>93</v>
+        <v>99</v>
       </c>
       <c r="F48" s="4"/>
       <c r="G48" s="4"/>
@@ -3377,14 +3395,14 @@
     <row x14ac:dyDescent="0.25" r="49" customHeight="1" ht="35.25" customFormat="1" s="1">
       <c r="A49" s="13"/>
       <c r="B49" s="14" t="s">
-        <v>109</v>
+        <v>115</v>
       </c>
       <c r="C49" s="10"/>
       <c r="D49" s="4" t="s">
-        <v>11</v>
+        <v>28</v>
       </c>
       <c r="E49" s="4" t="s">
-        <v>93</v>
+        <v>99</v>
       </c>
       <c r="F49" s="4"/>
       <c r="G49" s="4"/>
@@ -3411,14 +3429,14 @@
     <row x14ac:dyDescent="0.25" r="50" customHeight="1" ht="36" customFormat="1" s="1">
       <c r="A50" s="13"/>
       <c r="B50" s="14" t="s">
-        <v>110</v>
+        <v>116</v>
       </c>
       <c r="C50" s="10"/>
       <c r="D50" s="4" t="s">
-        <v>100</v>
+        <v>106</v>
       </c>
       <c r="E50" s="4" t="s">
-        <v>111</v>
+        <v>117</v>
       </c>
       <c r="F50" s="4"/>
       <c r="G50" s="4"/>
@@ -3445,14 +3463,14 @@
     <row x14ac:dyDescent="0.25" r="51" customHeight="1" ht="50.25" customFormat="1" s="1">
       <c r="A51" s="13"/>
       <c r="B51" s="14" t="s">
-        <v>112</v>
+        <v>118</v>
       </c>
       <c r="C51" s="10"/>
       <c r="D51" s="4" t="s">
-        <v>11</v>
+        <v>28</v>
       </c>
       <c r="E51" s="4" t="s">
-        <v>93</v>
+        <v>99</v>
       </c>
       <c r="F51" s="4"/>
       <c r="G51" s="4"/>
@@ -3479,14 +3497,14 @@
     <row x14ac:dyDescent="0.25" r="52" customHeight="1" ht="36" customFormat="1" s="1">
       <c r="A52" s="13"/>
       <c r="B52" s="14" t="s">
-        <v>113</v>
+        <v>119</v>
       </c>
       <c r="C52" s="10"/>
       <c r="D52" s="4" t="s">
-        <v>11</v>
+        <v>28</v>
       </c>
       <c r="E52" s="4" t="s">
-        <v>93</v>
+        <v>99</v>
       </c>
       <c r="F52" s="4"/>
       <c r="G52" s="4"/>
@@ -3513,14 +3531,14 @@
     <row x14ac:dyDescent="0.25" r="53" customHeight="1" ht="36.75" customFormat="1" s="1">
       <c r="A53" s="13"/>
       <c r="B53" s="21" t="s">
-        <v>114</v>
+        <v>120</v>
       </c>
       <c r="C53" s="18"/>
       <c r="D53" s="4" t="s">
-        <v>11</v>
+        <v>28</v>
       </c>
       <c r="E53" s="4" t="s">
-        <v>93</v>
+        <v>99</v>
       </c>
       <c r="F53" s="4"/>
       <c r="G53" s="4"/>
@@ -3547,16 +3565,16 @@
     <row x14ac:dyDescent="0.25" r="54" customHeight="1" ht="44.25" customFormat="1" s="1">
       <c r="A54" s="13"/>
       <c r="B54" s="8" t="s">
-        <v>115</v>
+        <v>121</v>
       </c>
       <c r="C54" s="8" t="s">
         <v>15</v>
       </c>
       <c r="D54" s="4" t="s">
-        <v>11</v>
+        <v>28</v>
       </c>
       <c r="E54" s="4" t="s">
-        <v>93</v>
+        <v>99</v>
       </c>
       <c r="F54" s="4"/>
       <c r="G54" s="4"/>
@@ -3583,16 +3601,16 @@
     <row x14ac:dyDescent="0.25" r="55" customHeight="1" ht="30" customFormat="1" s="1">
       <c r="A55" s="13"/>
       <c r="B55" s="7" t="s">
-        <v>116</v>
+        <v>122</v>
       </c>
       <c r="C55" s="12" t="s">
         <v>15</v>
       </c>
       <c r="D55" s="4" t="s">
-        <v>11</v>
+        <v>28</v>
       </c>
       <c r="E55" s="4" t="s">
-        <v>93</v>
+        <v>99</v>
       </c>
       <c r="F55" s="4"/>
       <c r="G55" s="4"/>
@@ -3619,14 +3637,14 @@
     <row x14ac:dyDescent="0.25" r="56" customHeight="1" ht="30" customFormat="1" s="1">
       <c r="A56" s="13"/>
       <c r="B56" s="14" t="s">
-        <v>117</v>
+        <v>123</v>
       </c>
       <c r="C56" s="10"/>
       <c r="D56" s="4" t="s">
-        <v>11</v>
+        <v>28</v>
       </c>
       <c r="E56" s="4" t="s">
-        <v>66</v>
+        <v>72</v>
       </c>
       <c r="F56" s="4"/>
       <c r="G56" s="4"/>
@@ -3653,14 +3671,14 @@
     <row x14ac:dyDescent="0.25" r="57" customHeight="1" ht="30" customFormat="1" s="1">
       <c r="A57" s="13"/>
       <c r="B57" s="14" t="s">
-        <v>118</v>
+        <v>124</v>
       </c>
       <c r="C57" s="10"/>
       <c r="D57" s="4" t="s">
-        <v>11</v>
+        <v>28</v>
       </c>
       <c r="E57" s="4" t="s">
-        <v>66</v>
+        <v>72</v>
       </c>
       <c r="F57" s="4"/>
       <c r="G57" s="4"/>
@@ -3687,14 +3705,14 @@
     <row x14ac:dyDescent="0.25" r="58" customHeight="1" ht="32.25" customFormat="1" s="1">
       <c r="A58" s="13"/>
       <c r="B58" s="14" t="s">
-        <v>119</v>
+        <v>125</v>
       </c>
       <c r="C58" s="10"/>
       <c r="D58" s="4" t="s">
-        <v>120</v>
+        <v>126</v>
       </c>
       <c r="E58" s="4" t="s">
-        <v>93</v>
+        <v>99</v>
       </c>
       <c r="F58" s="4"/>
       <c r="G58" s="4"/>
@@ -3721,11 +3739,11 @@
     <row x14ac:dyDescent="0.25" r="59" customHeight="1" ht="26.25" customFormat="1" s="1">
       <c r="A59" s="13"/>
       <c r="B59" s="21" t="s">
-        <v>121</v>
+        <v>127</v>
       </c>
       <c r="C59" s="18"/>
       <c r="D59" s="4" t="s">
-        <v>81</v>
+        <v>87</v>
       </c>
       <c r="E59" s="4"/>
       <c r="F59" s="4"/>
@@ -3753,16 +3771,16 @@
     <row x14ac:dyDescent="0.25" r="60" customHeight="1" ht="40.5" customFormat="1" s="1">
       <c r="A60" s="13"/>
       <c r="B60" s="22" t="s">
-        <v>122</v>
+        <v>128</v>
       </c>
       <c r="C60" s="12" t="s">
         <v>15</v>
       </c>
       <c r="D60" s="4" t="s">
-        <v>11</v>
+        <v>28</v>
       </c>
       <c r="E60" s="4" t="s">
-        <v>93</v>
+        <v>99</v>
       </c>
       <c r="F60" s="4"/>
       <c r="G60" s="4"/>
@@ -3789,11 +3807,11 @@
     <row x14ac:dyDescent="0.25" r="61" customHeight="1" ht="62.25" customFormat="1" s="1">
       <c r="A61" s="13"/>
       <c r="B61" s="26" t="s">
-        <v>123</v>
+        <v>129</v>
       </c>
       <c r="C61" s="10"/>
       <c r="D61" s="4" t="s">
-        <v>124</v>
+        <v>130</v>
       </c>
       <c r="E61" s="4"/>
       <c r="F61" s="4"/>
@@ -3821,11 +3839,11 @@
     <row x14ac:dyDescent="0.25" r="62" customHeight="1" ht="18.75" customFormat="1" s="1">
       <c r="A62" s="13"/>
       <c r="B62" s="14" t="s">
-        <v>125</v>
+        <v>131</v>
       </c>
       <c r="C62" s="10"/>
       <c r="D62" s="4" t="s">
-        <v>126</v>
+        <v>132</v>
       </c>
       <c r="E62" s="4"/>
       <c r="F62" s="4"/>
@@ -3853,11 +3871,11 @@
     <row x14ac:dyDescent="0.25" r="63" customHeight="1" ht="18.75" customFormat="1" s="1">
       <c r="A63" s="13"/>
       <c r="B63" s="21" t="s">
-        <v>127</v>
+        <v>133</v>
       </c>
       <c r="C63" s="18"/>
       <c r="D63" s="4" t="s">
-        <v>81</v>
+        <v>87</v>
       </c>
       <c r="E63" s="4"/>
       <c r="F63" s="4"/>
@@ -3885,16 +3903,16 @@
     <row x14ac:dyDescent="0.25" r="64" customHeight="1" ht="28.5" customFormat="1" s="1">
       <c r="A64" s="13"/>
       <c r="B64" s="7" t="s">
-        <v>128</v>
+        <v>134</v>
       </c>
       <c r="C64" s="12" t="s">
         <v>15</v>
       </c>
       <c r="D64" s="4" t="s">
-        <v>81</v>
+        <v>87</v>
       </c>
       <c r="E64" s="4" t="s">
-        <v>129</v>
+        <v>135</v>
       </c>
       <c r="F64" s="4"/>
       <c r="G64" s="4"/>
@@ -3921,11 +3939,11 @@
     <row x14ac:dyDescent="0.25" r="65" customHeight="1" ht="39.75" customFormat="1" s="1">
       <c r="A65" s="13"/>
       <c r="B65" s="14" t="s">
-        <v>130</v>
+        <v>136</v>
       </c>
       <c r="C65" s="10"/>
       <c r="D65" s="4" t="s">
-        <v>131</v>
+        <v>137</v>
       </c>
       <c r="E65" s="4"/>
       <c r="F65" s="4"/>
@@ -3953,11 +3971,11 @@
     <row x14ac:dyDescent="0.25" r="66" customHeight="1" ht="28.5" customFormat="1" s="1">
       <c r="A66" s="13"/>
       <c r="B66" s="14" t="s">
-        <v>132</v>
+        <v>138</v>
       </c>
       <c r="C66" s="10"/>
       <c r="D66" s="4" t="s">
-        <v>81</v>
+        <v>87</v>
       </c>
       <c r="E66" s="4"/>
       <c r="F66" s="4"/>
@@ -3985,14 +4003,14 @@
     <row x14ac:dyDescent="0.25" r="67" customHeight="1" ht="40.5" customFormat="1" s="1">
       <c r="A67" s="13"/>
       <c r="B67" s="21" t="s">
-        <v>133</v>
+        <v>139</v>
       </c>
       <c r="C67" s="18"/>
       <c r="D67" s="4" t="s">
-        <v>11</v>
+        <v>28</v>
       </c>
       <c r="E67" s="4" t="s">
-        <v>134</v>
+        <v>140</v>
       </c>
       <c r="F67" s="4"/>
       <c r="G67" s="4"/>
@@ -4019,16 +4037,16 @@
     <row x14ac:dyDescent="0.25" r="68" customHeight="1" ht="18.75" customFormat="1" s="1">
       <c r="A68" s="13"/>
       <c r="B68" s="7" t="s">
-        <v>135</v>
+        <v>141</v>
       </c>
       <c r="C68" s="12" t="s">
         <v>15</v>
       </c>
       <c r="D68" s="4" t="s">
-        <v>11</v>
+        <v>28</v>
       </c>
       <c r="E68" s="4" t="s">
-        <v>136</v>
+        <v>142</v>
       </c>
       <c r="F68" s="4"/>
       <c r="G68" s="4"/>
@@ -4055,14 +4073,14 @@
     <row x14ac:dyDescent="0.25" r="69" customHeight="1" ht="18.75" customFormat="1" s="1">
       <c r="A69" s="13"/>
       <c r="B69" s="14" t="s">
-        <v>137</v>
+        <v>143</v>
       </c>
       <c r="C69" s="10"/>
       <c r="D69" s="4" t="s">
-        <v>11</v>
+        <v>28</v>
       </c>
       <c r="E69" s="4" t="s">
-        <v>138</v>
+        <v>144</v>
       </c>
       <c r="F69" s="4"/>
       <c r="G69" s="4"/>
@@ -4089,14 +4107,14 @@
     <row x14ac:dyDescent="0.25" r="70" customHeight="1" ht="18.75" customFormat="1" s="1">
       <c r="A70" s="25"/>
       <c r="B70" s="21" t="s">
-        <v>139</v>
+        <v>145</v>
       </c>
       <c r="C70" s="18"/>
       <c r="D70" s="4" t="s">
-        <v>140</v>
+        <v>146</v>
       </c>
       <c r="E70" s="4" t="s">
-        <v>141</v>
+        <v>147</v>
       </c>
       <c r="F70" s="4"/>
       <c r="G70" s="4"/>
@@ -4122,16 +4140,16 @@
     </row>
     <row x14ac:dyDescent="0.25" r="71" customHeight="1" ht="45" customFormat="1" s="1">
       <c r="A71" s="7" t="s">
-        <v>142</v>
+        <v>148</v>
       </c>
       <c r="B71" s="7" t="s">
-        <v>143</v>
+        <v>149</v>
       </c>
       <c r="C71" s="12" t="s">
-        <v>144</v>
+        <v>150</v>
       </c>
       <c r="D71" s="4" t="s">
-        <v>81</v>
+        <v>87</v>
       </c>
       <c r="E71" s="4"/>
       <c r="F71" s="4"/>
@@ -4158,14 +4176,14 @@
     </row>
     <row x14ac:dyDescent="0.25" r="72" customHeight="1" ht="45" customFormat="1" s="1">
       <c r="A72" s="20" t="s">
-        <v>145</v>
+        <v>151</v>
       </c>
       <c r="B72" s="14" t="s">
-        <v>146</v>
+        <v>152</v>
       </c>
       <c r="C72" s="10"/>
       <c r="D72" s="4" t="s">
-        <v>147</v>
+        <v>153</v>
       </c>
       <c r="E72" s="4"/>
       <c r="F72" s="4"/>
@@ -4193,11 +4211,11 @@
     <row x14ac:dyDescent="0.25" r="73" customHeight="1" ht="45" customFormat="1" s="1">
       <c r="A73" s="10"/>
       <c r="B73" s="14" t="s">
-        <v>148</v>
+        <v>154</v>
       </c>
       <c r="C73" s="10"/>
       <c r="D73" s="4" t="s">
-        <v>81</v>
+        <v>87</v>
       </c>
       <c r="E73" s="4"/>
       <c r="F73" s="4"/>
@@ -4225,11 +4243,11 @@
     <row x14ac:dyDescent="0.25" r="74" customHeight="1" ht="39" customFormat="1" s="1">
       <c r="A74" s="11"/>
       <c r="B74" s="14" t="s">
-        <v>149</v>
+        <v>155</v>
       </c>
       <c r="C74" s="10"/>
       <c r="D74" s="4" t="s">
-        <v>81</v>
+        <v>87</v>
       </c>
       <c r="E74" s="4"/>
       <c r="F74" s="4"/>
@@ -4257,11 +4275,11 @@
     <row x14ac:dyDescent="0.25" r="75" customHeight="1" ht="26.25" customFormat="1" s="1">
       <c r="A75" s="13"/>
       <c r="B75" s="27" t="s">
-        <v>150</v>
+        <v>156</v>
       </c>
       <c r="C75" s="10"/>
       <c r="D75" s="4" t="s">
-        <v>81</v>
+        <v>87</v>
       </c>
       <c r="E75" s="4"/>
       <c r="F75" s="4"/>
@@ -4289,11 +4307,11 @@
     <row x14ac:dyDescent="0.25" r="76" customHeight="1" ht="62.25" customFormat="1" s="1">
       <c r="A76" s="13"/>
       <c r="B76" s="14" t="s">
-        <v>151</v>
+        <v>157</v>
       </c>
       <c r="C76" s="10"/>
       <c r="D76" s="4" t="s">
-        <v>81</v>
+        <v>87</v>
       </c>
       <c r="E76" s="4"/>
       <c r="F76" s="4"/>
@@ -4321,11 +4339,11 @@
     <row x14ac:dyDescent="0.25" r="77" customHeight="1" ht="43.5" customFormat="1" s="1">
       <c r="A77" s="13"/>
       <c r="B77" s="14" t="s">
-        <v>152</v>
+        <v>158</v>
       </c>
       <c r="C77" s="10"/>
       <c r="D77" s="4" t="s">
-        <v>81</v>
+        <v>87</v>
       </c>
       <c r="E77" s="4"/>
       <c r="F77" s="4"/>
@@ -4353,11 +4371,11 @@
     <row x14ac:dyDescent="0.25" r="78" customHeight="1" ht="42" customFormat="1" s="1">
       <c r="A78" s="13"/>
       <c r="B78" s="21" t="s">
-        <v>153</v>
+        <v>159</v>
       </c>
       <c r="C78" s="18"/>
       <c r="D78" s="4" t="s">
-        <v>81</v>
+        <v>87</v>
       </c>
       <c r="E78" s="4"/>
       <c r="F78" s="4"/>
@@ -4385,13 +4403,13 @@
     <row x14ac:dyDescent="0.25" r="79" customHeight="1" ht="36.75" customFormat="1" s="1">
       <c r="A79" s="13"/>
       <c r="B79" s="7" t="s">
-        <v>154</v>
+        <v>160</v>
       </c>
       <c r="C79" s="12" t="s">
         <v>15</v>
       </c>
       <c r="D79" s="4" t="s">
-        <v>81</v>
+        <v>87</v>
       </c>
       <c r="E79" s="4"/>
       <c r="F79" s="4"/>
@@ -4419,14 +4437,14 @@
     <row x14ac:dyDescent="0.25" r="80" customHeight="1" ht="62.25" customFormat="1" s="1">
       <c r="A80" s="13"/>
       <c r="B80" s="14" t="s">
-        <v>155</v>
+        <v>161</v>
       </c>
       <c r="C80" s="10"/>
       <c r="D80" s="4" t="s">
-        <v>81</v>
+        <v>87</v>
       </c>
       <c r="E80" s="4" t="s">
-        <v>156</v>
+        <v>162</v>
       </c>
       <c r="F80" s="4"/>
       <c r="G80" s="4"/>
@@ -4450,14 +4468,14 @@
       <c r="Y80" s="4"/>
       <c r="Z80" s="4"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="81" customHeight="1" ht="62.25" customFormat="1" s="1">
+    <row x14ac:dyDescent="0.25" r="81" customHeight="1" ht="28.5" customFormat="1" s="1">
       <c r="A81" s="13"/>
       <c r="B81" s="14" t="s">
-        <v>157</v>
+        <v>163</v>
       </c>
       <c r="C81" s="10"/>
       <c r="D81" s="4" t="s">
-        <v>81</v>
+        <v>87</v>
       </c>
       <c r="E81" s="4"/>
       <c r="F81" s="4"/>
@@ -4482,14 +4500,14 @@
       <c r="Y81" s="4"/>
       <c r="Z81" s="4"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="82" customHeight="1" ht="62.25" customFormat="1" s="1">
+    <row x14ac:dyDescent="0.25" r="82" customHeight="1" ht="28.5" customFormat="1" s="1">
       <c r="A82" s="13"/>
       <c r="B82" s="14" t="s">
-        <v>158</v>
+        <v>164</v>
       </c>
       <c r="C82" s="10"/>
       <c r="D82" s="4" t="s">
-        <v>81</v>
+        <v>87</v>
       </c>
       <c r="E82" s="4"/>
       <c r="F82" s="4"/>
@@ -4514,14 +4532,14 @@
       <c r="Y82" s="4"/>
       <c r="Z82" s="4"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="83" customHeight="1" ht="62.25" customFormat="1" s="1">
+    <row x14ac:dyDescent="0.25" r="83" customHeight="1" ht="28.5" customFormat="1" s="1">
       <c r="A83" s="13"/>
       <c r="B83" s="14" t="s">
-        <v>159</v>
+        <v>165</v>
       </c>
       <c r="C83" s="10"/>
       <c r="D83" s="4" t="s">
-        <v>81</v>
+        <v>87</v>
       </c>
       <c r="E83" s="4"/>
       <c r="F83" s="4"/>
@@ -4546,14 +4564,14 @@
       <c r="Y83" s="4"/>
       <c r="Z83" s="4"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="84" customHeight="1" ht="62.25" customFormat="1" s="1">
+    <row x14ac:dyDescent="0.25" r="84" customHeight="1" ht="28.5" customFormat="1" s="1">
       <c r="A84" s="13"/>
       <c r="B84" s="14" t="s">
-        <v>160</v>
+        <v>166</v>
       </c>
       <c r="C84" s="10"/>
       <c r="D84" s="4" t="s">
-        <v>81</v>
+        <v>87</v>
       </c>
       <c r="E84" s="4"/>
       <c r="F84" s="4"/>
@@ -4578,14 +4596,14 @@
       <c r="Y84" s="4"/>
       <c r="Z84" s="4"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="85" customHeight="1" ht="36" customFormat="1" s="1">
+    <row x14ac:dyDescent="0.25" r="85" customHeight="1" ht="28.5" customFormat="1" s="1">
       <c r="A85" s="13"/>
       <c r="B85" s="14" t="s">
-        <v>161</v>
+        <v>167</v>
       </c>
       <c r="C85" s="10"/>
       <c r="D85" s="4" t="s">
-        <v>81</v>
+        <v>87</v>
       </c>
       <c r="E85" s="4"/>
       <c r="F85" s="4"/>
@@ -4610,14 +4628,14 @@
       <c r="Y85" s="4"/>
       <c r="Z85" s="4"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="86" customHeight="1" ht="36" customFormat="1" s="1">
+    <row x14ac:dyDescent="0.25" r="86" customHeight="1" ht="28.5" customFormat="1" s="1">
       <c r="A86" s="13"/>
       <c r="B86" s="14" t="s">
-        <v>162</v>
+        <v>168</v>
       </c>
       <c r="C86" s="10"/>
       <c r="D86" s="4" t="s">
-        <v>81</v>
+        <v>87</v>
       </c>
       <c r="E86" s="4"/>
       <c r="F86" s="4"/>
@@ -4642,14 +4660,14 @@
       <c r="Y86" s="4"/>
       <c r="Z86" s="4"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="87" customHeight="1" ht="36" customFormat="1" s="1">
+    <row x14ac:dyDescent="0.25" r="87" customHeight="1" ht="28.5" customFormat="1" s="1">
       <c r="A87" s="13"/>
       <c r="B87" s="14" t="s">
-        <v>163</v>
+        <v>169</v>
       </c>
       <c r="C87" s="10"/>
       <c r="D87" s="4" t="s">
-        <v>81</v>
+        <v>87</v>
       </c>
       <c r="E87" s="4"/>
       <c r="F87" s="4"/>
@@ -4674,14 +4692,14 @@
       <c r="Y87" s="4"/>
       <c r="Z87" s="4"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="88" customHeight="1" ht="50.25" customFormat="1" s="1">
+    <row x14ac:dyDescent="0.25" r="88" customHeight="1" ht="28.5" customFormat="1" s="1">
       <c r="A88" s="13"/>
       <c r="B88" s="14" t="s">
-        <v>164</v>
+        <v>170</v>
       </c>
       <c r="C88" s="10"/>
       <c r="D88" s="4" t="s">
-        <v>81</v>
+        <v>87</v>
       </c>
       <c r="E88" s="4"/>
       <c r="F88" s="4"/>
@@ -4706,14 +4724,14 @@
       <c r="Y88" s="4"/>
       <c r="Z88" s="4"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="89" customHeight="1" ht="36" customFormat="1" s="1">
+    <row x14ac:dyDescent="0.25" r="89" customHeight="1" ht="28.5" customFormat="1" s="1">
       <c r="A89" s="13"/>
       <c r="B89" s="14" t="s">
-        <v>165</v>
+        <v>171</v>
       </c>
       <c r="C89" s="10"/>
       <c r="D89" s="4" t="s">
-        <v>11</v>
+        <v>28</v>
       </c>
       <c r="E89" s="4"/>
       <c r="F89" s="4"/>
@@ -4738,14 +4756,14 @@
       <c r="Y89" s="4"/>
       <c r="Z89" s="4"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="90" customHeight="1" ht="36.75" customFormat="1" s="1">
+    <row x14ac:dyDescent="0.25" r="90" customHeight="1" ht="29.25" customFormat="1" s="1">
       <c r="A90" s="13"/>
       <c r="B90" s="21" t="s">
-        <v>166</v>
+        <v>172</v>
       </c>
       <c r="C90" s="18"/>
       <c r="D90" s="4" t="s">
-        <v>81</v>
+        <v>87</v>
       </c>
       <c r="E90" s="4"/>
       <c r="F90" s="4"/>
@@ -4770,16 +4788,16 @@
       <c r="Y90" s="4"/>
       <c r="Z90" s="4"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="91" customHeight="1" ht="51" customFormat="1" s="1">
+    <row x14ac:dyDescent="0.25" r="91" customHeight="1" ht="39.75" customFormat="1" s="1">
       <c r="A91" s="13"/>
       <c r="B91" s="22" t="s">
-        <v>167</v>
+        <v>173</v>
       </c>
       <c r="C91" s="12" t="s">
-        <v>168</v>
+        <v>174</v>
       </c>
       <c r="D91" s="4" t="s">
-        <v>81</v>
+        <v>87</v>
       </c>
       <c r="E91" s="4"/>
       <c r="F91" s="4"/>
@@ -4807,11 +4825,11 @@
     <row x14ac:dyDescent="0.25" r="92" customHeight="1" ht="50.25" customFormat="1" s="1">
       <c r="A92" s="13"/>
       <c r="B92" s="23" t="s">
-        <v>169</v>
+        <v>175</v>
       </c>
       <c r="C92" s="10"/>
       <c r="D92" s="4" t="s">
-        <v>81</v>
+        <v>87</v>
       </c>
       <c r="E92" s="4"/>
       <c r="F92" s="4"/>
@@ -4839,11 +4857,11 @@
     <row x14ac:dyDescent="0.25" r="93" customHeight="1" ht="36" customFormat="1" s="1">
       <c r="A93" s="13"/>
       <c r="B93" s="23" t="s">
-        <v>170</v>
+        <v>176</v>
       </c>
       <c r="C93" s="10"/>
       <c r="D93" s="4" t="s">
-        <v>81</v>
+        <v>87</v>
       </c>
       <c r="E93" s="4"/>
       <c r="F93" s="4"/>
@@ -4871,11 +4889,11 @@
     <row x14ac:dyDescent="0.25" r="94" customHeight="1" ht="36" customFormat="1" s="1">
       <c r="A94" s="13"/>
       <c r="B94" s="23" t="s">
-        <v>171</v>
+        <v>177</v>
       </c>
       <c r="C94" s="10"/>
       <c r="D94" s="4" t="s">
-        <v>81</v>
+        <v>87</v>
       </c>
       <c r="E94" s="4"/>
       <c r="F94" s="4"/>
@@ -4903,11 +4921,11 @@
     <row x14ac:dyDescent="0.25" r="95" customHeight="1" ht="36.75" customFormat="1" s="1">
       <c r="A95" s="25"/>
       <c r="B95" s="17" t="s">
-        <v>172</v>
+        <v>178</v>
       </c>
       <c r="C95" s="18"/>
       <c r="D95" s="4" t="s">
-        <v>81</v>
+        <v>87</v>
       </c>
       <c r="E95" s="4"/>
       <c r="F95" s="4"/>
@@ -4934,16 +4952,16 @@
     </row>
     <row x14ac:dyDescent="0.25" r="96" customHeight="1" ht="64.5" customFormat="1" s="1">
       <c r="A96" s="7" t="s">
-        <v>173</v>
+        <v>179</v>
       </c>
       <c r="B96" s="7" t="s">
-        <v>174</v>
+        <v>180</v>
       </c>
       <c r="C96" s="12" t="s">
         <v>15</v>
       </c>
       <c r="D96" s="4" t="s">
-        <v>81</v>
+        <v>87</v>
       </c>
       <c r="E96" s="4"/>
       <c r="F96" s="4"/>
@@ -4970,14 +4988,14 @@
     </row>
     <row x14ac:dyDescent="0.25" r="97" customHeight="1" ht="36" customFormat="1" s="1">
       <c r="A97" s="20" t="s">
-        <v>175</v>
+        <v>181</v>
       </c>
       <c r="B97" s="14" t="s">
-        <v>176</v>
+        <v>182</v>
       </c>
       <c r="C97" s="10"/>
       <c r="D97" s="4" t="s">
-        <v>81</v>
+        <v>87</v>
       </c>
       <c r="E97" s="4"/>
       <c r="F97" s="4"/>
@@ -5005,11 +5023,11 @@
     <row x14ac:dyDescent="0.25" r="98" customHeight="1" ht="50.25" customFormat="1" s="1">
       <c r="A98" s="10"/>
       <c r="B98" s="14" t="s">
-        <v>177</v>
+        <v>183</v>
       </c>
       <c r="C98" s="10"/>
       <c r="D98" s="4" t="s">
-        <v>81</v>
+        <v>87</v>
       </c>
       <c r="E98" s="4"/>
       <c r="F98" s="4"/>
@@ -5037,11 +5055,11 @@
     <row x14ac:dyDescent="0.25" r="99" customHeight="1" ht="72.75" customFormat="1" s="1">
       <c r="A99" s="11"/>
       <c r="B99" s="21" t="s">
-        <v>178</v>
+        <v>184</v>
       </c>
       <c r="C99" s="18"/>
       <c r="D99" s="4" t="s">
-        <v>81</v>
+        <v>87</v>
       </c>
       <c r="E99" s="4"/>
       <c r="F99" s="4"/>
@@ -5069,13 +5087,13 @@
     <row x14ac:dyDescent="0.25" r="100" customHeight="1" ht="36" customFormat="1" s="1">
       <c r="A100" s="13"/>
       <c r="B100" s="7" t="s">
-        <v>179</v>
+        <v>185</v>
       </c>
       <c r="C100" s="12" t="s">
         <v>15</v>
       </c>
       <c r="D100" s="4" t="s">
-        <v>81</v>
+        <v>87</v>
       </c>
       <c r="E100" s="4"/>
       <c r="F100" s="4"/>
@@ -5103,11 +5121,11 @@
     <row x14ac:dyDescent="0.25" r="101" customHeight="1" ht="50.25" customFormat="1" s="1">
       <c r="A101" s="13"/>
       <c r="B101" s="14" t="s">
-        <v>180</v>
+        <v>186</v>
       </c>
       <c r="C101" s="10"/>
       <c r="D101" s="4" t="s">
-        <v>81</v>
+        <v>87</v>
       </c>
       <c r="E101" s="4"/>
       <c r="F101" s="4"/>
@@ -5135,11 +5153,11 @@
     <row x14ac:dyDescent="0.25" r="102" customHeight="1" ht="63" customFormat="1" s="1">
       <c r="A102" s="13"/>
       <c r="B102" s="21" t="s">
-        <v>181</v>
+        <v>187</v>
       </c>
       <c r="C102" s="18"/>
       <c r="D102" s="4" t="s">
-        <v>81</v>
+        <v>87</v>
       </c>
       <c r="E102" s="4"/>
       <c r="F102" s="4"/>
@@ -5167,13 +5185,13 @@
     <row x14ac:dyDescent="0.25" r="103" customHeight="1" ht="36.75" customFormat="1" s="1">
       <c r="A103" s="13"/>
       <c r="B103" s="7" t="s">
-        <v>182</v>
+        <v>188</v>
       </c>
       <c r="C103" s="12" t="s">
         <v>15</v>
       </c>
       <c r="D103" s="4" t="s">
-        <v>81</v>
+        <v>87</v>
       </c>
       <c r="E103" s="4"/>
       <c r="F103" s="4"/>
@@ -5201,11 +5219,11 @@
     <row x14ac:dyDescent="0.25" r="104" customHeight="1" ht="50.25" customFormat="1" s="1">
       <c r="A104" s="13"/>
       <c r="B104" s="14" t="s">
-        <v>183</v>
+        <v>189</v>
       </c>
       <c r="C104" s="10"/>
       <c r="D104" s="4" t="s">
-        <v>81</v>
+        <v>87</v>
       </c>
       <c r="E104" s="4"/>
       <c r="F104" s="4"/>
@@ -5233,11 +5251,11 @@
     <row x14ac:dyDescent="0.25" r="105" customHeight="1" ht="36.75" customFormat="1" s="1">
       <c r="A105" s="13"/>
       <c r="B105" s="21" t="s">
-        <v>184</v>
+        <v>190</v>
       </c>
       <c r="C105" s="18"/>
       <c r="D105" s="4" t="s">
-        <v>81</v>
+        <v>87</v>
       </c>
       <c r="E105" s="4"/>
       <c r="F105" s="4"/>
@@ -5265,13 +5283,13 @@
     <row x14ac:dyDescent="0.25" r="106" customHeight="1" ht="51" customFormat="1" s="1">
       <c r="A106" s="13"/>
       <c r="B106" s="7" t="s">
-        <v>185</v>
+        <v>191</v>
       </c>
       <c r="C106" s="12" t="s">
         <v>15</v>
       </c>
       <c r="D106" s="4" t="s">
-        <v>81</v>
+        <v>87</v>
       </c>
       <c r="E106" s="4"/>
       <c r="F106" s="4"/>
@@ -5299,11 +5317,11 @@
     <row x14ac:dyDescent="0.25" r="107" customHeight="1" ht="36" customFormat="1" s="1">
       <c r="A107" s="13"/>
       <c r="B107" s="14" t="s">
-        <v>186</v>
+        <v>192</v>
       </c>
       <c r="C107" s="10"/>
       <c r="D107" s="4" t="s">
-        <v>81</v>
+        <v>87</v>
       </c>
       <c r="E107" s="4"/>
       <c r="F107" s="4"/>
@@ -5331,11 +5349,11 @@
     <row x14ac:dyDescent="0.25" r="108" customHeight="1" ht="36" customFormat="1" s="1">
       <c r="A108" s="13"/>
       <c r="B108" s="14" t="s">
-        <v>187</v>
+        <v>193</v>
       </c>
       <c r="C108" s="10"/>
       <c r="D108" s="4" t="s">
-        <v>81</v>
+        <v>87</v>
       </c>
       <c r="E108" s="4"/>
       <c r="F108" s="4"/>
@@ -5363,11 +5381,11 @@
     <row x14ac:dyDescent="0.25" r="109" customHeight="1" ht="21.75" customFormat="1" s="1">
       <c r="A109" s="13"/>
       <c r="B109" s="14" t="s">
-        <v>188</v>
+        <v>194</v>
       </c>
       <c r="C109" s="10"/>
       <c r="D109" s="4" t="s">
-        <v>81</v>
+        <v>87</v>
       </c>
       <c r="E109" s="4"/>
       <c r="F109" s="4"/>
@@ -5395,11 +5413,11 @@
     <row x14ac:dyDescent="0.25" r="110" customHeight="1" ht="36" customFormat="1" s="1">
       <c r="A110" s="13"/>
       <c r="B110" s="14" t="s">
-        <v>189</v>
+        <v>195</v>
       </c>
       <c r="C110" s="10"/>
       <c r="D110" s="4" t="s">
-        <v>81</v>
+        <v>87</v>
       </c>
       <c r="E110" s="4"/>
       <c r="F110" s="4"/>
@@ -5427,11 +5445,11 @@
     <row x14ac:dyDescent="0.25" r="111" customHeight="1" ht="36.75" customFormat="1" s="1">
       <c r="A111" s="13"/>
       <c r="B111" s="21" t="s">
-        <v>190</v>
+        <v>196</v>
       </c>
       <c r="C111" s="18"/>
       <c r="D111" s="4" t="s">
-        <v>81</v>
+        <v>87</v>
       </c>
       <c r="E111" s="4"/>
       <c r="F111" s="4"/>
@@ -5459,13 +5477,13 @@
     <row x14ac:dyDescent="0.25" r="112" customHeight="1" ht="36.75" customFormat="1" s="1">
       <c r="A112" s="13"/>
       <c r="B112" s="7" t="s">
-        <v>191</v>
+        <v>197</v>
       </c>
       <c r="C112" s="12" t="s">
         <v>15</v>
       </c>
       <c r="D112" s="4" t="s">
-        <v>81</v>
+        <v>87</v>
       </c>
       <c r="E112" s="4"/>
       <c r="F112" s="4"/>
@@ -5493,11 +5511,11 @@
     <row x14ac:dyDescent="0.25" r="113" customHeight="1" ht="36" customFormat="1" s="1">
       <c r="A113" s="13"/>
       <c r="B113" s="14" t="s">
-        <v>192</v>
+        <v>198</v>
       </c>
       <c r="C113" s="10"/>
       <c r="D113" s="4" t="s">
-        <v>81</v>
+        <v>87</v>
       </c>
       <c r="E113" s="4"/>
       <c r="F113" s="4"/>
@@ -5525,11 +5543,11 @@
     <row x14ac:dyDescent="0.25" r="114" customHeight="1" ht="50.25" customFormat="1" s="1">
       <c r="A114" s="13"/>
       <c r="B114" s="14" t="s">
-        <v>193</v>
+        <v>199</v>
       </c>
       <c r="C114" s="10"/>
       <c r="D114" s="4" t="s">
-        <v>81</v>
+        <v>87</v>
       </c>
       <c r="E114" s="4"/>
       <c r="F114" s="4"/>
@@ -5557,11 +5575,11 @@
     <row x14ac:dyDescent="0.25" r="115" customHeight="1" ht="36" customFormat="1" s="1">
       <c r="A115" s="13"/>
       <c r="B115" s="14" t="s">
-        <v>194</v>
+        <v>200</v>
       </c>
       <c r="C115" s="10"/>
       <c r="D115" s="4" t="s">
-        <v>81</v>
+        <v>87</v>
       </c>
       <c r="E115" s="4"/>
       <c r="F115" s="4"/>
@@ -5589,11 +5607,11 @@
     <row x14ac:dyDescent="0.25" r="116" customHeight="1" ht="30.75" customFormat="1" s="1">
       <c r="A116" s="25"/>
       <c r="B116" s="21" t="s">
-        <v>195</v>
+        <v>201</v>
       </c>
       <c r="C116" s="18"/>
       <c r="D116" s="4" t="s">
-        <v>81</v>
+        <v>87</v>
       </c>
       <c r="E116" s="4"/>
       <c r="F116" s="4"/>

</xml_diff>